<commit_message>
Add more tests and upgrade GPT-4 model
</commit_message>
<xml_diff>
--- a/documents/QnA_OSM.xlsx
+++ b/documents/QnA_OSM.xlsx
@@ -8,10 +8,11 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dev\master-thesis\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787DAEB8-0168-43B6-AA48-5AD7D2CDEAD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6846F66-E3D9-44EA-B108-75B606F90B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="16305" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="16305" activeTab="1" xr2:uid="{4644477B-1EF6-4C86-97DC-241B9BD87314}"/>
+    <workbookView xWindow="30195" yWindow="1395" windowWidth="21600" windowHeight="11775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{4644477B-1EF6-4C86-97DC-241B9BD87314}"/>
+    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="16305" activeTab="1" xr2:uid="{6781345F-657A-4A33-A440-5439B4508001}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="108">
   <si>
     <t>Query</t>
   </si>
@@ -77,9 +78,6 @@
   </si>
   <si>
     <t>county_names</t>
-  </si>
-  <si>
-    <t>What are the name of the available couties?</t>
   </si>
   <si>
     <t>Nordland, Telemark, Troms, Rogaland, Vestland, Trøndelag, Vestfold, Buskerud, Akershus, Østfold, Innlandet, Møre og Romsdal, Agder Finnmark</t>
@@ -118,9 +116,6 @@
     <t>LangSmith Traces</t>
   </si>
   <si>
-    <t>Giving the correct number of trees (about 50).</t>
-  </si>
-  <si>
     <t>num_trees_along_munkegata</t>
   </si>
   <si>
@@ -128,9 +123,6 @@
 - Get tree data for Trondheim
 - Create a  suitable buffer around the road data and perform an intersection
 - Count the number of hits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">larges_county </t>
   </si>
   <si>
     <t>Nordland</t>
@@ -170,12 +162,6 @@
 - Filter using `maxspeed&gt;=70`</t>
   </si>
   <si>
-    <t>shortest_path</t>
-  </si>
-  <si>
-    <t>What is the shortest path between City Syd and City Lade?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Display the outline of Viken, based on the outlines of Buskerud, Aksershus, and Østfold, that are found in the data. Should be dissolved, i.e., no borders. </t>
   </si>
   <si>
@@ -309,6 +295,105 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>What are the names of the counties in found in the data?</t>
+  </si>
+  <si>
+    <t>/home/dev/master-thesis/tex/figs/county_names_oaf.png</t>
+  </si>
+  <si>
+    <t>75e133f8-1c23-4e1d-b30d-b0bad4e11c5b</t>
+  </si>
+  <si>
+    <t>/home/dev/master-thesis/tex/figs/county_names_sql.png</t>
+  </si>
+  <si>
+    <t>/home/dev/master-thesis/tex/figs/county_names_python.png</t>
+  </si>
+  <si>
+    <t>f116bb4f-c983-4a95-a8e5-3bba7c1ede88</t>
+  </si>
+  <si>
+    <t>785d0ea2-0f38-451e-8216-8ef4ef0ff239</t>
+  </si>
+  <si>
+    <t>/home/dev/master-thesis/tex/figs/nidarosdomen_retrieval_oaf.png</t>
+  </si>
+  <si>
+    <t>/home/dev/master-thesis/tex/figs/nidarosdomen_retrieval_sql.png</t>
+  </si>
+  <si>
+    <t>nidarosdomen_retrieval</t>
+  </si>
+  <si>
+    <t>3bba3d1f-f395-4ff7-a4b3-2c06c4041b71</t>
+  </si>
+  <si>
+    <t>005e2084-19e2-4f4b-b0dd-04d115d2ed3a</t>
+  </si>
+  <si>
+    <t>/home/dev/master-thesis/tex/figs/nidarosdomen_retrieval_python.png</t>
+  </si>
+  <si>
+    <t>6f32f803-8258-48f3-8593-190ef8658350</t>
+  </si>
+  <si>
+    <t>837878a7-eacd-49b0-bca6-a030f2bf3265</t>
+  </si>
+  <si>
+    <t>/home/dev/master-thesis/tex/figs/num_trees_along_munkegata_oaf.png</t>
+  </si>
+  <si>
+    <t>/home/dev/master-thesis/tex/figs/num_trees_along_munkegata_sql.png</t>
+  </si>
+  <si>
+    <t>Giving the correct number of trees (about 70-80).</t>
+  </si>
+  <si>
+    <t>7aa667f5-0ec1-4820-ab33-686bb70a0078</t>
+  </si>
+  <si>
+    <t>098f22ec-6d0a-4424-955c-dfe5c6085718
+d4ed059a-dd61-45d9-aa3b-02f8b05fba19
+57acac87-84b1-4e8f-9363-fe64945a456c</t>
+  </si>
+  <si>
+    <t>/home/dev/master-thesis/tex/figs/num_trees_along_munkegata_python.png
+Question was answered in the first run, so only this is used for cost/duration.</t>
+  </si>
+  <si>
+    <t>b8ceddb4-c463-42c9-a8a9-0ec0dd9acda7
+d04de59b-ed5f-4ddf-9f8e-c6b8565c2427
+be713323-5a9d-4d80-bd1a-0bb18248a33c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/dev/master-thesis/tex/figs/oslo_roads_maxspeed_hte_70_kmh_oaf.png
+/home/dev/master-thesis/tex/figs/oslo_roads_maxspeed_hte_70_kmh_oaf_bbox_and_outline.png
+Created a good bounding box from the top of its head, but did not use the actual outline. </t>
+  </si>
+  <si>
+    <t>0d23c9b5-e6dd-4fe5-b126-6c4c38452f3f</t>
+  </si>
+  <si>
+    <t>/home/dev/master-thesis/tex/figs/oslo_roads_maxspeed_hte_70_kmh_sql.png
+Same issue as the `oaf` run above.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">largest_county </t>
+  </si>
+  <si>
+    <t>dafe8eb6-ee3f-495a-ad36-566ca45f9a57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/dev/master-thesis/tex/figs/oslo_roads_maxspeed_hte_70_kmh_python.png
+Returned results for the whole country. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find building clusters consisting of more than 50 000 buildings. </t>
+  </si>
+  <si>
+    <t>building_clusters</t>
   </si>
 </sst>
 </file>
@@ -316,7 +401,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -382,7 +467,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -393,11 +478,11 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -409,10 +494,41 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -438,19 +554,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -462,41 +569,19 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -512,29 +597,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{83D2B9CE-16C8-4DB7-89A3-592E6CC65025}" name="Table3" displayName="Table3" ref="A1:G26" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="6">
-  <autoFilter ref="A1:G26" xr:uid="{83D2B9CE-16C8-4DB7-89A3-592E6CC65025}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{83D2B9CE-16C8-4DB7-89A3-592E6CC65025}" name="Table3" displayName="Table3" ref="A1:G37" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15">
+  <autoFilter ref="A1:G37" xr:uid="{83D2B9CE-16C8-4DB7-89A3-592E6CC65025}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{5E217325-9314-4066-9478-85ED196C3B0A}" name="Query ID" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{97EF1974-2076-449A-A0D4-15EA85F8280F}" name="Agent Type" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{8D1D516B-C100-437C-94C9-405B27E99C54}" name="Outcome" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{62F2D408-C3F9-4A29-8859-C68FE5808C7B}" name="Duration [s]" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{D7F4AA3D-7E52-4896-B7EA-B50F31C8EB43}" name="Cost [$]" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{A1053517-318C-4EC5-B223-7161442ACA6F}" name="LangSmith Traces" dataDxfId="4" dataCellStyle="Hyperlink"/>
-    <tableColumn id="7" xr3:uid="{67E2112F-399B-47A4-AB16-E0E342B8B15C}" name="Comments" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{5E217325-9314-4066-9478-85ED196C3B0A}" name="Query ID" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{97EF1974-2076-449A-A0D4-15EA85F8280F}" name="Agent Type" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{8D1D516B-C100-437C-94C9-405B27E99C54}" name="Outcome" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{62F2D408-C3F9-4A29-8859-C68FE5808C7B}" name="Duration [s]" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{D7F4AA3D-7E52-4896-B7EA-B50F31C8EB43}" name="Cost [$]" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{A1053517-318C-4EC5-B223-7161442ACA6F}" name="LangSmith Traces" dataDxfId="9" dataCellStyle="Hyperlink"/>
+    <tableColumn id="7" xr3:uid="{67E2112F-399B-47A4-AB16-E0E342B8B15C}" name="Comments" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{78FA15C9-D8E3-4683-98B8-69E5AAB2BDFB}" name="Table2" displayName="Table2" ref="A1:E15" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" headerRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{78FA15C9-D8E3-4683-98B8-69E5AAB2BDFB}" name="Table2" displayName="Table2" ref="A1:E15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6">
   <autoFilter ref="A1:E15" xr:uid="{78FA15C9-D8E3-4683-98B8-69E5AAB2BDFB}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{DF94BDDE-72C2-4E46-ACD5-0E5A636ABE68}" name="Query ID" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{D36448D7-13F4-4A67-88D5-39F0C9732E25}" name="Query" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{88EFB23F-53BA-48C7-8DB1-E4BFB7F240EE}" name="Correct  Response" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{568271BE-C334-41D7-BECB-CE936A642BD1}" name="Steps" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{DF94BDDE-72C2-4E46-ACD5-0E5A636ABE68}" name="Query ID" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{D36448D7-13F4-4A67-88D5-39F0C9732E25}" name="Query" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{88EFB23F-53BA-48C7-8DB1-E4BFB7F240EE}" name="Correct  Response" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{568271BE-C334-41D7-BECB-CE936A642BD1}" name="Steps" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{13F83F64-A4E0-456B-9916-E486752D5330}" name="Difficulty" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -804,22 +889,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0"/>
-    <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="1">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="1">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="35" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.109375" style="5" customWidth="1"/>
     <col min="3" max="3" width="15.21875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="11" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
     <col min="5" max="5" width="13" style="9" customWidth="1"/>
     <col min="6" max="6" width="38.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="62.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.21875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -832,14 +918,14 @@
       <c r="C1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>2</v>
@@ -847,318 +933,604 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="11">
+        <v>37</v>
+      </c>
+      <c r="D2" s="10">
         <v>68.23</v>
       </c>
       <c r="E2" s="9">
         <v>6.3450000000000006E-2</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="11">
+        <v>51</v>
+      </c>
+      <c r="D3" s="10">
         <v>26.49</v>
       </c>
       <c r="E3" s="9">
         <v>1.553E-2</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="11">
+        <v>37</v>
+      </c>
+      <c r="D4" s="10">
         <v>52.24</v>
       </c>
       <c r="E4" s="9">
         <v>3.3930000000000002E-2</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="11">
+        <v>37</v>
+      </c>
+      <c r="D5" s="10">
         <v>168.13</v>
       </c>
       <c r="E5" s="9">
         <v>2.01E-2</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="11">
+        <v>53</v>
+      </c>
+      <c r="D6" s="10">
         <v>119.39</v>
       </c>
       <c r="E6" s="9">
         <v>2.4670000000000001E-2</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="11">
+        <v>37</v>
+      </c>
+      <c r="D7" s="10">
         <v>673.96</v>
       </c>
       <c r="E7" s="9">
         <v>4.1889999999999997E-2</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="11">
+        <v>37</v>
+      </c>
+      <c r="D8" s="10">
         <v>69.73</v>
       </c>
       <c r="E8" s="9">
         <v>2.2929999999999999E-2</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="11">
+        <v>37</v>
+      </c>
+      <c r="D9" s="10">
         <v>36.54</v>
       </c>
       <c r="E9" s="9">
         <v>1.2529999999999999E-2</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="11">
+        <v>37</v>
+      </c>
+      <c r="D10" s="10">
         <v>663.22</v>
       </c>
       <c r="E10" s="9">
         <v>3.9739999999999998E-2</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>103</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="11">
+        <v>51</v>
+      </c>
+      <c r="D11" s="10">
         <v>29.37</v>
       </c>
       <c r="E11" s="9">
         <v>2.4570000000000002E-2</v>
       </c>
       <c r="F11" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>103</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="11">
+        <v>37</v>
+      </c>
+      <c r="D12" s="10">
         <v>41.82</v>
       </c>
       <c r="E12" s="9">
         <v>1.7749999999999998E-2</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>27</v>
+        <v>103</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="11">
+        <v>37</v>
+      </c>
+      <c r="D13" s="10">
         <v>37.520000000000003</v>
       </c>
       <c r="E13" s="9">
         <v>1.7239999999999998E-2</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F14" s="6"/>
+      <c r="A14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="10">
+        <v>78.08</v>
+      </c>
+      <c r="E14" s="9">
+        <v>2.555E-2</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F15" s="6"/>
+      <c r="A15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="10">
+        <v>18.89</v>
+      </c>
+      <c r="E15" s="9">
+        <v>1.3350000000000001E-2</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F20" s="6"/>
-    </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F23" s="6"/>
-    </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F24" s="6"/>
-    </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="10">
+        <v>44.33</v>
+      </c>
+      <c r="E16" s="9">
+        <v>2.682E-2</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="10">
+        <v>29.82</v>
+      </c>
+      <c r="E17" s="9">
+        <v>1.9890000000000001E-2</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="10">
+        <v>34.6</v>
+      </c>
+      <c r="E18" s="9">
+        <v>1.5509999999999999E-2</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="10">
+        <v>35.1</v>
+      </c>
+      <c r="E19" s="9">
+        <v>4.5560000000000003E-2</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="10">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="E20" s="9">
+        <v>3.0589999999999999E-2</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="10">
+        <v>63.93</v>
+      </c>
+      <c r="E21" s="9">
+        <v>1.8970000000000001E-2</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="10">
+        <v>122.99</v>
+      </c>
+      <c r="E22" s="9">
+        <v>3.9579999999999997E-2</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="10">
+        <v>44.44</v>
+      </c>
+      <c r="E23" s="9">
+        <v>2.0389999999999998E-2</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="10">
+        <v>59.47</v>
+      </c>
+      <c r="E24" s="9">
+        <v>1.6449999999999999E-2</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="10">
+        <v>983.76</v>
+      </c>
+      <c r="E25" s="9">
+        <v>4.0579999999999998E-2</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
       <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D27" s="10"/>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D28" s="10"/>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D29" s="10"/>
+      <c r="F29" s="6"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D30" s="10"/>
+      <c r="F30" s="6"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D31" s="10"/>
+      <c r="F31" s="6"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D32" s="10"/>
+      <c r="F32" s="6"/>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D33" s="10"/>
+      <c r="F33" s="6"/>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D34" s="10"/>
+      <c r="F34" s="6"/>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D35" s="10"/>
+      <c r="F35" s="6"/>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D36" s="10"/>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D37" s="10"/>
+      <c r="F37" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1172,10 +1544,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3BFF00C-9B20-4D57-A0F3-3732FF3EA698}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="82" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="1"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="1">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="84" workbookViewId="2">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1201,7 +1578,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1215,27 +1592,27 @@
         <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
@@ -1243,143 +1620,141 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="167.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>27</v>
+        <v>103</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+        <v>48</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="4"/>
       <c r="E10" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="93.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="4"/>
+        <v>58</v>
+      </c>
+      <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>61</v>
+        <v>107</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>63</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="3" t="s">
-        <v>82</v>
-      </c>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>

</xml_diff>

<commit_message>
Finish novice vs. expert experiments
</commit_message>
<xml_diff>
--- a/documents/QnA_OSM.xlsx
+++ b/documents/QnA_OSM.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dev\master-thesis\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F3F2E8-E3F3-4468-A96F-D1B5D875D8B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8B8880-1FC9-4A65-9565-D48184CADB22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30630" yWindow="1830" windowWidth="21600" windowHeight="11775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{4644477B-1EF6-4C86-97DC-241B9BD87314}"/>
-    <workbookView minimized="1" xWindow="31065" yWindow="2265" windowWidth="21600" windowHeight="11775" activeTab="1" xr2:uid="{6781345F-657A-4A33-A440-5439B4508001}"/>
+    <workbookView xWindow="1830" yWindow="1830" windowWidth="21600" windowHeight="11775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="16305" activeTab="3" xr2:uid="{4644477B-1EF6-4C86-97DC-241B9BD87314}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" activeTab="2" xr2:uid="{4727A768-4BCB-40CC-83D8-01A50FFB84D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
     <sheet name="Questions" sheetId="2" r:id="rId2"/>
+    <sheet name="Prompt Levels" sheetId="3" r:id="rId3"/>
+    <sheet name="PL Tests" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="183">
   <si>
     <t>Query</t>
   </si>
@@ -93,9 +95,6 @@
   </si>
   <si>
     <t>Adding corresponding line segments to the map.</t>
-  </si>
-  <si>
-    <t>oslo_roads_maxspeed_hte_70_kmh</t>
   </si>
   <si>
     <t>LangSmith Traces</t>
@@ -492,15 +491,172 @@
   <si>
     <t>Tokens</t>
   </si>
+  <si>
+    <t>A geodesic, slightly curved line between Gardermoen and Flesland.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a geodesic curve between the airports of Oslo and Bergen. </t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Formulation</t>
+  </si>
+  <si>
+    <t>novice</t>
+  </si>
+  <si>
+    <t>expert</t>
+  </si>
+  <si>
+    <t>oslo_bergen_geodesic_novice</t>
+  </si>
+  <si>
+    <t>oslo_bergen_geodesic_expert</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Please plot the shortest flight path on a map between Oslo and Bergen's airports.</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>step-by-step</t>
+  </si>
+  <si>
+    <t>Could you count how many trees there are on Munkegata street in Trondheim?</t>
+  </si>
+  <si>
+    <t>oslo_bergen_geodesic_expert_sbs</t>
+  </si>
+  <si>
+    <t>munkegata_trees_count_novice</t>
+  </si>
+  <si>
+    <t>munkegata_trees_count_expert</t>
+  </si>
+  <si>
+    <t>munkegata_trees_count_expert_sbs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sql </t>
+  </si>
+  <si>
+    <t>42f887d6-e241-45f4-84d2-63ec88ba497a</t>
+  </si>
+  <si>
+    <t>1. Get info on all potentially relevant datasets. The airports are possibly stored as polygons in the available data. 
+2. Filter those datasets for airports and list the names of the airports. 
+3. Retrieve the geographic coordinates for Oslo Gardermoen Airport (OSL) and Bergen Flesland Airport (BGO) by filtering on the names you found. 
+4. If no name was found, try a different dataset and go back to step 2. 
+5. Utilize available tools to draw a geodesic curve that represents the shortest path on the earth's surface between these two points.
+6. Present the findings with a map highlighting the largest county.</t>
+  </si>
+  <si>
+    <t>00ef0753-259e-48e1-9900-d5c80ca6bd25
+613f58a0-1ff6-4509-a65f-d51c4b7f3d42
+5893074f-6b73-413c-8a58-0e389ce4caf2</t>
+  </si>
+  <si>
+    <t>3703bd50-bb92-4bcf-8bae-f004a2e8000b</t>
+  </si>
+  <si>
+    <t>520bd384-3c44-4c3c-8134-54c596544ca2
+a8af379b-bb7f-4564-a30b-64f528812c54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retrieve roads in Oslo that have speed limit greater than or equal to 70 km/h. </t>
+  </si>
+  <si>
+    <t>oslo_roads_maxspeed_gte_70_kmh</t>
+  </si>
+  <si>
+    <t>oslo_roads_maxspeed_gte_70_kmh_novice</t>
+  </si>
+  <si>
+    <t>oslo_roads_maxspeed_gte_70_kmh_expert</t>
+  </si>
+  <si>
+    <t>oslo_roads_maxspeed_gte_70_kmh_expert_sbs</t>
+  </si>
+  <si>
+    <t>1. Retrieve an outline of Oslo. 
+2. Calculate max/min lat/lon values for this bounding box, and use it to retrieve a subset of the road data. 
+3. Select road segments within the outline from step 1 that have a max speed &gt;= 70.  
+4. Present the findings with a map highlighting the selected roads.</t>
+  </si>
+  <si>
+    <t>0e03dad4-3e88-414e-a5ea-2322f2e85345
+6efb4132-201a-47fc-88f2-035173db94eb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. List all datasets that could possibly include trees. 
+2. Find the correct feature class and filter the relevant dataset to access tree data for Trondheim. Use a bounding box to reduce the number of trees to analyse. 
+4. Fetch road data for Munkegata. Use a bounding box for Trondheim in case there are streets elsewhere named Munkegata. 
+5. Convert both datasets to a suitable metric CRS and add a 20-meter buffer around the road data. 
+6. Find all trees that lie within this buffer and count them. 
+7. Present the findings with a map highlighting the roads and the trees. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find the number of trees within a 20-meter buffer of Munkegata in Trondheim. </t>
+  </si>
+  <si>
+    <t>83a2d982-5272-4453-8c9e-18c46f46915b</t>
+  </si>
+  <si>
+    <t>aea043ab-1bb5-40fc-aa4d-77719ce12b47</t>
+  </si>
+  <si>
+    <t>74568360-49f8-424e-953a-076adea4f40f
+6136f87e-16e4-4a65-b857-316c288d8346</t>
+  </si>
+  <si>
+    <t>71ebab57-5dbf-46c2-bcf4-37fafeb18471</t>
+  </si>
+  <si>
+    <t>b0a4037d-0977-4be2-be2e-ac8b013833ac</t>
+  </si>
+  <si>
+    <t>c7206383-e1dd-4df4-ace2-e1e35d7edf7a</t>
+  </si>
+  <si>
+    <t>f2b5578a-8a75-4533-ac97-7ffb4082becc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Draw roads in Oslo where you can drive at least 70. </t>
+  </si>
+  <si>
+    <t>2d46071a-28ae-4dab-b4f0-6d1f3800d181</t>
+  </si>
+  <si>
+    <t>353a9b66-8c25-4405-b7c9-d431d74bd896</t>
+  </si>
+  <si>
+    <t>7850e0d4-3d18-4a06-abfa-49b0909fdd09</t>
+  </si>
+  <si>
+    <t>677da9e9-6ca7-4cc5-969f-79eebb0ef073</t>
+  </si>
+  <si>
+    <t>1bdaf03d-a3ce-4ff5-8948-103d0f8e71b1</t>
+  </si>
+  <si>
+    <t>ff4e6511-f899-4837-89e2-35ecbc6d6013</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="168" formatCode="[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -534,16 +690,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri "/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -560,12 +741,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -586,13 +795,216 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF0D0D0D"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="9"/>
+        </left>
+        <right style="thin">
+          <color theme="9"/>
+        </right>
+        <top style="thin">
+          <color theme="9"/>
+        </top>
+        <bottom style="thin">
+          <color theme="9"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="9"/>
+        </left>
+        <right style="thin">
+          <color theme="9"/>
+        </right>
+        <top style="thin">
+          <color theme="9"/>
+        </top>
+        <bottom style="thin">
+          <color theme="9"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri "/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -704,17 +1116,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{83D2B9CE-16C8-4DB7-89A3-592E6CC65025}" name="Table3" displayName="Table3" ref="A1:I37" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{83D2B9CE-16C8-4DB7-89A3-592E6CC65025}" name="Table3" displayName="Table3" ref="A1:I37" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25">
   <autoFilter ref="A1:I37" xr:uid="{83D2B9CE-16C8-4DB7-89A3-592E6CC65025}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5E217325-9314-4066-9478-85ED196C3B0A}" name="Query ID" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{97EF1974-2076-449A-A0D4-15EA85F8280F}" name="Agent Type" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{8D1D516B-C100-437C-94C9-405B27E99C54}" name="Outcome" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{62F2D408-C3F9-4A29-8859-C68FE5808C7B}" name="Duration [s]" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{E204E73A-EDA9-4F27-8D7B-6E638A0FF18B}" name="Tokens" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{D7F4AA3D-7E52-4896-B7EA-B50F31C8EB43}" name="Cost [$]" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{A1053517-318C-4EC5-B223-7161442ACA6F}" name="LangSmith Traces" dataDxfId="12" dataCellStyle="Hyperlink"/>
-    <tableColumn id="7" xr3:uid="{67E2112F-399B-47A4-AB16-E0E342B8B15C}" name="Comments" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{5E217325-9314-4066-9478-85ED196C3B0A}" name="Query ID" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{97EF1974-2076-449A-A0D4-15EA85F8280F}" name="Agent Type" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{8D1D516B-C100-437C-94C9-405B27E99C54}" name="Outcome" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{62F2D408-C3F9-4A29-8859-C68FE5808C7B}" name="Duration [s]" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{E204E73A-EDA9-4F27-8D7B-6E638A0FF18B}" name="Tokens" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{D7F4AA3D-7E52-4896-B7EA-B50F31C8EB43}" name="Cost [$]" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{A1053517-318C-4EC5-B223-7161442ACA6F}" name="LangSmith Traces" dataDxfId="21" dataCellStyle="Hyperlink"/>
+    <tableColumn id="7" xr3:uid="{67E2112F-399B-47A4-AB16-E0E342B8B15C}" name="Comments" dataDxfId="20"/>
     <tableColumn id="10" xr3:uid="{63EE7C62-A488-4C94-A292-957054A783BD}" name="Model"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -722,17 +1134,48 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{78FA15C9-D8E3-4683-98B8-69E5AAB2BDFB}" name="Table2" displayName="Table2" ref="A1:E15" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9">
-  <autoFilter ref="A1:E15" xr:uid="{78FA15C9-D8E3-4683-98B8-69E5AAB2BDFB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E15">
-    <sortCondition ref="E1:E15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{78FA15C9-D8E3-4683-98B8-69E5AAB2BDFB}" name="Table2" displayName="Table2" ref="A1:E13" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18">
+  <autoFilter ref="A1:E13" xr:uid="{78FA15C9-D8E3-4683-98B8-69E5AAB2BDFB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E13">
+    <sortCondition ref="E1:E13"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{DF94BDDE-72C2-4E46-ACD5-0E5A636ABE68}" name="Query ID" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{D36448D7-13F4-4A67-88D5-39F0C9732E25}" name="Query" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{88EFB23F-53BA-48C7-8DB1-E4BFB7F240EE}" name="Correct  Response" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{568271BE-C334-41D7-BECB-CE936A642BD1}" name="Steps" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{13F83F64-A4E0-456B-9916-E486752D5330}" name="Difficulty" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{DF94BDDE-72C2-4E46-ACD5-0E5A636ABE68}" name="Query ID" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{D36448D7-13F4-4A67-88D5-39F0C9732E25}" name="Query" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{88EFB23F-53BA-48C7-8DB1-E4BFB7F240EE}" name="Correct  Response" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{568271BE-C334-41D7-BECB-CE936A642BD1}" name="Steps" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{13F83F64-A4E0-456B-9916-E486752D5330}" name="Difficulty" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{196D0887-5250-43FF-A287-28CA4A8E592F}" name="Table1" displayName="Table1" ref="A1:D10" totalsRowShown="0" headerRowDxfId="8" dataDxfId="5">
+  <autoFilter ref="A1:D10" xr:uid="{196D0887-5250-43FF-A287-28CA4A8E592F}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{BB7680CC-D6B4-4A54-8010-3749DEE3CBE6}" name="Query ID" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{D915BF0A-EE69-4AF7-9164-9E88C8FDBE7E}" name="Level" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{5274E49A-ABB1-4FBE-A864-8E07DAA5C8A9}" name="Type" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{80F6FFEF-7E46-4686-BA17-BB3CBD130F08}" name="Formulation" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6FDFBCD9-DEE7-43F6-B225-8DEF2DE803FD}" name="Table4" displayName="Table4" ref="A1:I19" totalsRowShown="0">
+  <autoFilter ref="A1:I19" xr:uid="{6FDFBCD9-DEE7-43F6-B225-8DEF2DE803FD}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{D03B1644-1C7C-4FCE-9DB9-747262C3C960}" name="Query ID" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{D379A25A-D035-498B-B8CF-AD0E2A81496B}" name="Agent Type"/>
+    <tableColumn id="3" xr3:uid="{E57A08B9-2E85-4F54-8E95-AB8F5DD74EF8}" name="Outcome"/>
+    <tableColumn id="4" xr3:uid="{6E678DF2-F0CD-40A6-AEDB-CC2E158D34C7}" name="Duration [s]"/>
+    <tableColumn id="5" xr3:uid="{E7E60375-F0D0-4F78-98DC-842559FEA71B}" name="Tokens"/>
+    <tableColumn id="6" xr3:uid="{6A2B8CFD-216F-42A3-AD46-D5BDE92AE5B4}" name="Cost [$]" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{E12EEE88-959B-4D71-A927-9789CECC1F97}" name="LangSmith Traces"/>
+    <tableColumn id="8" xr3:uid="{42C9F38F-B4D9-45B5-BB31-A67F037C65AA}" name="Comments"/>
+    <tableColumn id="9" xr3:uid="{659C8448-0B70-40B5-AA26-7C10544D76F8}" name="Model" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1004,12 +1447,12 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0"/>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="82" zoomScaleNormal="82" workbookViewId="1">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="1">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
-    <sheetView topLeftCell="A11" workbookViewId="2"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="35" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" style="5" customWidth="1"/>
@@ -1022,7 +1465,7 @@
     <col min="9" max="9" width="21.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -1035,31 +1478,31 @@
       <c r="D1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>137</v>
+      <c r="E1" s="14" t="s">
+        <v>136</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" s="10">
         <v>68.23</v>
@@ -1071,24 +1514,24 @@
         <v>6.3450000000000006E-2</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="I2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="57.6">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="10">
         <v>26.49</v>
@@ -1100,24 +1543,24 @@
         <v>1.553E-2</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D4" s="10">
         <v>52.24</v>
@@ -1129,24 +1572,24 @@
         <v>3.3930000000000002E-2</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="10">
         <v>168.13</v>
@@ -1158,24 +1601,24 @@
         <v>2.01E-2</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="57.6">
       <c r="A6" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" s="10">
         <v>119.39</v>
@@ -1187,24 +1630,24 @@
         <v>2.4670000000000001E-2</v>
       </c>
       <c r="G6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="I6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="10">
         <v>673.96</v>
@@ -1216,24 +1659,24 @@
         <v>4.1889999999999997E-2</v>
       </c>
       <c r="G7" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="I7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D8" s="10">
         <v>69.73</v>
@@ -1245,24 +1688,24 @@
         <v>2.2929999999999999E-2</v>
       </c>
       <c r="G8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="I8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="10">
         <v>36.54</v>
@@ -1274,24 +1717,24 @@
         <v>1.2529999999999999E-2</v>
       </c>
       <c r="G9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="I9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="10">
         <v>663.22</v>
@@ -1303,24 +1746,24 @@
         <v>3.9739999999999998E-2</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="57.6">
       <c r="A11" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="10">
         <v>29.37</v>
@@ -1332,24 +1775,24 @@
         <v>2.4570000000000002E-2</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D12" s="10">
         <v>41.82</v>
@@ -1361,24 +1804,24 @@
         <v>1.7749999999999998E-2</v>
       </c>
       <c r="G12" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="I12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="10">
         <v>37.520000000000003</v>
@@ -1390,24 +1833,24 @@
         <v>1.7239999999999998E-2</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D14" s="10">
         <v>78.08</v>
@@ -1419,24 +1862,24 @@
         <v>2.555E-2</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I14" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" s="10">
         <v>18.89</v>
@@ -1448,24 +1891,24 @@
         <v>1.3350000000000001E-2</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" s="10">
         <v>44.33</v>
@@ -1477,24 +1920,24 @@
         <v>2.682E-2</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D17" s="10">
         <v>29.82</v>
@@ -1506,24 +1949,24 @@
         <v>1.9890000000000001E-2</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I17" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18" s="10">
         <v>34.6</v>
@@ -1535,24 +1978,24 @@
         <v>1.5509999999999999E-2</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H18" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="I18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="B19" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" s="10">
         <v>35.1</v>
@@ -1564,24 +2007,24 @@
         <v>4.5560000000000003E-2</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20" s="10">
         <v>75.599999999999994</v>
@@ -1593,24 +2036,24 @@
         <v>3.0589999999999999E-2</v>
       </c>
       <c r="G20" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H20" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="H20" s="5" t="s">
-        <v>88</v>
-      </c>
       <c r="I20" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21" s="10">
         <v>63.93</v>
@@ -1622,24 +2065,24 @@
         <v>1.8970000000000001E-2</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I21" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="81.599999999999994" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="D22" s="10">
         <v>122.99</v>
@@ -1651,24 +2094,24 @@
         <v>3.9579999999999997E-2</v>
       </c>
       <c r="G22" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="H22" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="H22" s="3" t="s">
-        <v>93</v>
-      </c>
       <c r="I22" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="115.2" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>17</v>
+        <v>161</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D23" s="10">
         <v>44.44</v>
@@ -1680,24 +2123,24 @@
         <v>2.0389999999999998E-2</v>
       </c>
       <c r="G23" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="H23" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="I23" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="43.2">
       <c r="A24" s="3" t="s">
-        <v>17</v>
+        <v>161</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D24" s="10">
         <v>59.47</v>
@@ -1709,24 +2152,24 @@
         <v>1.6449999999999999E-2</v>
       </c>
       <c r="G24" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H24" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="H24" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="I24" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="73.2" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>17</v>
+        <v>161</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D25" s="10">
         <v>983.76</v>
@@ -1738,24 +2181,24 @@
         <v>4.0579999999999998E-2</v>
       </c>
       <c r="G25" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="H25" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="I25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="I25" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="B26" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D26" s="10">
         <v>65.47</v>
@@ -1767,24 +2210,24 @@
         <v>2.009E-2</v>
       </c>
       <c r="G26" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="H26" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H26" s="5" t="s">
-        <v>106</v>
-      </c>
       <c r="I26" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D27" s="10">
         <v>93.21</v>
@@ -1796,24 +2239,24 @@
         <v>3.2629999999999999E-2</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I27" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="57.6">
       <c r="A28" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D28" s="10">
         <v>66.42</v>
@@ -1825,24 +2268,24 @@
         <v>5.5550000000000002E-2</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I28" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D29" s="10">
         <v>129.03</v>
@@ -1854,24 +2297,24 @@
         <v>4.5600000000000002E-2</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I29" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="57.6">
       <c r="A30" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D30" s="10">
         <v>87.16</v>
@@ -1883,24 +2326,24 @@
         <v>3.465E-2</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="72">
       <c r="A31" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D31" s="10">
         <v>68.099999999999994</v>
@@ -1912,24 +2355,24 @@
         <v>5.2220000000000003E-2</v>
       </c>
       <c r="G31" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="I31" t="s">
         <v>116</v>
       </c>
-      <c r="H31" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="I31" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D32" s="10">
         <v>25.81</v>
@@ -1941,24 +2384,24 @@
         <v>1.3259999999999999E-2</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I32" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="57.6">
       <c r="A33" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D33" s="10">
         <v>56.33</v>
@@ -1970,24 +2413,24 @@
         <v>2.1149999999999999E-2</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I33" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D34" s="10">
         <v>24.08</v>
@@ -1999,24 +2442,24 @@
         <v>1.772E-2</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I34" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D35" s="10">
         <v>118.54</v>
@@ -2028,24 +2471,24 @@
         <v>6.9169999999999995E-2</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I35" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="72">
       <c r="A36" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D36" s="10">
         <v>80.489999999999995</v>
@@ -2057,24 +2500,24 @@
         <v>3.9710000000000002E-2</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I36" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="100.8">
       <c r="A37" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D37" s="10">
         <v>652.88</v>
@@ -2086,13 +2529,13 @@
         <v>9.425E-2</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I37" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2111,14 +2554,12 @@
     <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
-    <sheetView topLeftCell="A3" zoomScale="78" zoomScaleNormal="100" workbookViewId="1">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A2" zoomScale="78" zoomScaleNormal="100" workbookViewId="1">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" workbookViewId="2">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
     <col min="2" max="2" width="22.44140625" style="1" bestFit="1" customWidth="1"/>
@@ -2128,7 +2569,7 @@
     <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -2142,10 +2583,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="43.2">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -2156,35 +2597,35 @@
         <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="94.8" customHeight="1">
+      <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="94.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="100.8">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>13</v>
@@ -2193,159 +2634,746 @@
         <v>14</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="43.2">
+      <c r="A5" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="72">
+      <c r="A6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="57.6">
+      <c r="A7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="28.8">
+      <c r="A8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="52.2" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="57.6">
+      <c r="A10" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" s="3" t="s">
+    <row r="11" spans="1:5" ht="100.8">
+      <c r="A11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="86.4">
       <c r="A12" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="C12" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="43.2">
       <c r="A13" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+        <v>129</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E13" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CACDBB6-EC7B-48C7-A660-9515B930A1AA}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="2">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="42.88671875" style="31" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="22" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" style="22" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="28.8">
+      <c r="A2" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+    </row>
+    <row r="3" spans="1:6" ht="14.4">
+      <c r="A3" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+    </row>
+    <row r="4" spans="1:6" ht="136.80000000000001" customHeight="1">
+      <c r="A4" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+    </row>
+    <row r="5" spans="1:6" ht="14.4">
+      <c r="A5" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+    </row>
+    <row r="6" spans="1:6" ht="28.8">
+      <c r="A6" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+    </row>
+    <row r="7" spans="1:6" ht="86.4">
+      <c r="A7" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+    </row>
+    <row r="8" spans="1:6" ht="28.8">
+      <c r="A8" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+    </row>
+    <row r="9" spans="1:6" ht="28.8">
+      <c r="A9" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+    </row>
+    <row r="10" spans="1:6" ht="144">
+      <c r="A10" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E478D2DA-2B8C-45DE-9406-9F4B224C2A25}">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="1">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="2">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="48.5546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" customWidth="1"/>
+    <col min="6" max="6" width="14" style="27" customWidth="1"/>
+    <col min="7" max="7" width="43.77734375" customWidth="1"/>
+    <col min="8" max="8" width="14.77734375" customWidth="1"/>
+    <col min="9" max="9" width="22.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2">
+        <v>105.27</v>
+      </c>
+      <c r="E2">
+        <v>3166</v>
+      </c>
+      <c r="F2" s="27">
+        <v>3.4299999999999997E-2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>155</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>174</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
+        <v>175</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="28.8">
+      <c r="A5" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="B5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" t="s">
+        <v>158</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="43.2">
+      <c r="A7" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" t="s">
+        <v>177</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" t="s">
+        <v>179</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" t="s">
+        <v>178</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="B11" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" t="s">
+        <v>180</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="28.8">
+      <c r="A12" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" t="s">
+        <v>181</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="B14" t="s">
+        <v>154</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" t="s">
+        <v>182</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" t="s">
+        <v>169</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" t="s">
+        <v>173</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="28.8">
+      <c r="A17" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="B17" t="s">
+        <v>154</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" t="s">
+        <v>170</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" t="s">
+        <v>172</v>
+      </c>
+      <c r="I19" s="25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="I20" s="26"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="I21" s="26"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="I22" s="26"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="I23" s="26"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="I24" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finish first three questions
</commit_message>
<xml_diff>
--- a/documents/QnA_OSM.xlsx
+++ b/documents/QnA_OSM.xlsx
@@ -8,11 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dev\master-thesis\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8B8880-1FC9-4A65-9565-D48184CADB22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0393EAA0-DF06-4631-9BD3-3D1F99E5A3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="1830" windowWidth="21600" windowHeight="11775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="16305" activeTab="3" xr2:uid="{4644477B-1EF6-4C86-97DC-241B9BD87314}"/>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" activeTab="2" xr2:uid="{4727A768-4BCB-40CC-83D8-01A50FFB84D3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{4644477B-1EF6-4C86-97DC-241B9BD87314}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{4727A768-4BCB-40CC-83D8-01A50FFB84D3}"/>
+    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="16305" activeTab="1" xr2:uid="{7CE71D1C-BB51-4650-8C03-0809E0E5E000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="211">
   <si>
     <t>Query</t>
   </si>
@@ -403,9 +404,6 @@
   </si>
   <si>
     <t>72e710c0-3f97-43eb-a304-8c63d97a0112</t>
-  </si>
-  <si>
-    <t>Which is the clostest railway station to Aker brygge?</t>
   </si>
   <si>
     <t>aker_brygge_national</t>
@@ -646,6 +644,102 @@
   </si>
   <si>
     <t>ff4e6511-f899-4837-89e2-35ecbc6d6013</t>
+  </si>
+  <si>
+    <t>6e4732ca-6774-46ad-8150-059432a0d174</t>
+  </si>
+  <si>
+    <t>4ed61d98-97e9-4930-b11f-a6c5b489191d</t>
+  </si>
+  <si>
+    <t>400c1a15-a5fe-4ca5-a1e2-fb2bedbe807c</t>
+  </si>
+  <si>
+    <t>54799937-297d-49f1-bc21-22f716358572</t>
+  </si>
+  <si>
+    <t>ec4bd8f0-7ae3-4e95-9e04-7c3d866e114e</t>
+  </si>
+  <si>
+    <t>744f1a00-cf24-4e67-98df-17dd2dc6706d</t>
+  </si>
+  <si>
+    <t>43ea7f1d-bfd7-4bbd-900f-9d0f8db68be9</t>
+  </si>
+  <si>
+    <t>e9ed7a87-3237-4a40-90b8-ad1e9607333d</t>
+  </si>
+  <si>
+    <t>/home/dev/master-thesis/tex/figs/cliff_clusters_sql_21.png
+/home/dev/master-thesis/tex/figs/cliff_clusters_sql_22.png</t>
+  </si>
+  <si>
+    <t>2a9b4f26-47d3-4bec-8ba4-ff000460175f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/dev/master-thesis/tex/figs/cliff_clusters_oaf_2.png
+Used an approximate number for degrees, probably because the function used only takes meters. </t>
+  </si>
+  <si>
+    <t>21bb7b6a-1e8b-4332-9a74-1bee9005a26d</t>
+  </si>
+  <si>
+    <t>107a76ec-8f8f-4d30-9d36-bf1684be6f54</t>
+  </si>
+  <si>
+    <t>79586aa0-63bc-4ecf-a622-48da49867a9e</t>
+  </si>
+  <si>
+    <t>32278f58-42fa-4989-94be-45a8b3911c37</t>
+  </si>
+  <si>
+    <t>87e29fe2-48f7-481f-9c64-1cd16eba10d7</t>
+  </si>
+  <si>
+    <t>Queried the wrong collection (places points).</t>
+  </si>
+  <si>
+    <t>c8b5bd0c-4515-448a-b246-e0aa5ebb4b27
+6bb3c188-f414-4641-927a-bad7bccee02b</t>
+  </si>
+  <si>
+    <t>f6ad6dfc-6a2f-4178-bc73-44d8f8bfb9c9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/dev/master-thesis/tex/figs/county_names_sql_partial_1.png
+/home/dev/master-thesis/tex/figs/county_names_sql_partial_2.png
+Had to ask follow-up question. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/dev/master-thesis/tex/figs/cliff_clusters_python.png
+Used 1000 m and got no clusters. </t>
+  </si>
+  <si>
+    <t>98c4beff-bd48-4eb4-b172-495d3d0ae5d2</t>
+  </si>
+  <si>
+    <t>Which is the closest railway station to Aker brygge?</t>
+  </si>
+  <si>
+    <t>1e64e5c8-e2b0-4422-8906-6261708a146e
+bf6fdf9f-4a45-4725-bb22-290bbc92836c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/dev/master-thesis/tex/figs/aker_national_sql_21.png
+/home/dev/master-thesis/tex/figs/aker_national_sql_22.png
+Follow-up needed. </t>
+  </si>
+  <si>
+    <t>86fea3ed-84ea-4bf4-b416-b31c44d028f3</t>
+  </si>
+  <si>
+    <t>e246c30c-16af-460d-8666-65d719488189</t>
+  </si>
+  <si>
+    <t>a965f60d-b0f5-49dd-b964-8ec7d1f778c7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used eps=0,1 with euclidean distance. No results. </t>
   </si>
 </sst>
 </file>
@@ -654,7 +748,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="168" formatCode="[$$-409]#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -724,7 +818,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -769,12 +863,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -795,43 +898,51 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -839,6 +950,49 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="27">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="9"/>
+        </left>
+        <right style="thin">
+          <color theme="9"/>
+        </right>
+        <top style="thin">
+          <color theme="9"/>
+        </top>
+        <bottom style="thin">
+          <color theme="9"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -891,65 +1045,7 @@
         <family val="2"/>
         <scheme val="major"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-409]#,##0.00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="9" tint="0.79998168889431442"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="9"/>
-        </left>
-        <right style="thin">
-          <color theme="9"/>
-        </right>
-        <top style="thin">
-          <color theme="9"/>
-        </top>
-        <bottom style="thin">
-          <color theme="9"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -977,7 +1073,22 @@
         <family val="2"/>
         <scheme val="major"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1004,15 +1115,6 @@
         <name val="Calibri "/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1079,6 +1181,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
@@ -1116,17 +1227,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{83D2B9CE-16C8-4DB7-89A3-592E6CC65025}" name="Table3" displayName="Table3" ref="A1:I37" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25">
-  <autoFilter ref="A1:I37" xr:uid="{83D2B9CE-16C8-4DB7-89A3-592E6CC65025}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{83D2B9CE-16C8-4DB7-89A3-592E6CC65025}" name="Table3" displayName="Table3" ref="A1:I109" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25">
+  <autoFilter ref="A1:I109" xr:uid="{83D2B9CE-16C8-4DB7-89A3-592E6CC65025}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I109">
+    <sortCondition ref="A2:A109"/>
+    <sortCondition ref="B2:B109"/>
+  </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{5E217325-9314-4066-9478-85ED196C3B0A}" name="Query ID" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{97EF1974-2076-449A-A0D4-15EA85F8280F}" name="Agent Type" dataDxfId="23"/>
     <tableColumn id="3" xr3:uid="{8D1D516B-C100-437C-94C9-405B27E99C54}" name="Outcome" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{62F2D408-C3F9-4A29-8859-C68FE5808C7B}" name="Duration [s]" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{E204E73A-EDA9-4F27-8D7B-6E638A0FF18B}" name="Tokens" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{D7F4AA3D-7E52-4896-B7EA-B50F31C8EB43}" name="Cost [$]" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{A1053517-318C-4EC5-B223-7161442ACA6F}" name="LangSmith Traces" dataDxfId="21" dataCellStyle="Hyperlink"/>
-    <tableColumn id="7" xr3:uid="{67E2112F-399B-47A4-AB16-E0E342B8B15C}" name="Comments" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{62F2D408-C3F9-4A29-8859-C68FE5808C7B}" name="Duration [s]" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{E204E73A-EDA9-4F27-8D7B-6E638A0FF18B}" name="Tokens" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{D7F4AA3D-7E52-4896-B7EA-B50F31C8EB43}" name="Cost [$]" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{A1053517-318C-4EC5-B223-7161442ACA6F}" name="LangSmith Traces" dataDxfId="18" dataCellStyle="Hyperlink"/>
+    <tableColumn id="7" xr3:uid="{67E2112F-399B-47A4-AB16-E0E342B8B15C}" name="Comments" dataDxfId="17"/>
     <tableColumn id="10" xr3:uid="{63EE7C62-A488-4C94-A292-957054A783BD}" name="Model"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1134,30 +1249,30 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{78FA15C9-D8E3-4683-98B8-69E5AAB2BDFB}" name="Table2" displayName="Table2" ref="A1:E13" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{78FA15C9-D8E3-4683-98B8-69E5AAB2BDFB}" name="Table2" displayName="Table2" ref="A1:E13" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15">
   <autoFilter ref="A1:E13" xr:uid="{78FA15C9-D8E3-4683-98B8-69E5AAB2BDFB}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E13">
-    <sortCondition ref="E1:E13"/>
+    <sortCondition ref="A2:A13"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{DF94BDDE-72C2-4E46-ACD5-0E5A636ABE68}" name="Query ID" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{D36448D7-13F4-4A67-88D5-39F0C9732E25}" name="Query" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{88EFB23F-53BA-48C7-8DB1-E4BFB7F240EE}" name="Correct  Response" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{568271BE-C334-41D7-BECB-CE936A642BD1}" name="Steps" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{13F83F64-A4E0-456B-9916-E486752D5330}" name="Difficulty" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{DF94BDDE-72C2-4E46-ACD5-0E5A636ABE68}" name="Query ID" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{D36448D7-13F4-4A67-88D5-39F0C9732E25}" name="Query" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{88EFB23F-53BA-48C7-8DB1-E4BFB7F240EE}" name="Correct  Response" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{568271BE-C334-41D7-BECB-CE936A642BD1}" name="Steps" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{13F83F64-A4E0-456B-9916-E486752D5330}" name="Difficulty" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{196D0887-5250-43FF-A287-28CA4A8E592F}" name="Table1" displayName="Table1" ref="A1:D10" totalsRowShown="0" headerRowDxfId="8" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{196D0887-5250-43FF-A287-28CA4A8E592F}" name="Table1" displayName="Table1" ref="A1:D10" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:D10" xr:uid="{196D0887-5250-43FF-A287-28CA4A8E592F}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BB7680CC-D6B4-4A54-8010-3749DEE3CBE6}" name="Query ID" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{D915BF0A-EE69-4AF7-9164-9E88C8FDBE7E}" name="Level" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{5274E49A-ABB1-4FBE-A864-8E07DAA5C8A9}" name="Type" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{80F6FFEF-7E46-4686-BA17-BB3CBD130F08}" name="Formulation" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{BB7680CC-D6B4-4A54-8010-3749DEE3CBE6}" name="Query ID" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{D915BF0A-EE69-4AF7-9164-9E88C8FDBE7E}" name="Level" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{5274E49A-ABB1-4FBE-A864-8E07DAA5C8A9}" name="Type" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{80F6FFEF-7E46-4686-BA17-BB3CBD130F08}" name="Formulation" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1167,15 +1282,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6FDFBCD9-DEE7-43F6-B225-8DEF2DE803FD}" name="Table4" displayName="Table4" ref="A1:I19" totalsRowShown="0">
   <autoFilter ref="A1:I19" xr:uid="{6FDFBCD9-DEE7-43F6-B225-8DEF2DE803FD}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{D03B1644-1C7C-4FCE-9DB9-747262C3C960}" name="Query ID" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D03B1644-1C7C-4FCE-9DB9-747262C3C960}" name="Query ID" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{D379A25A-D035-498B-B8CF-AD0E2A81496B}" name="Agent Type"/>
     <tableColumn id="3" xr3:uid="{E57A08B9-2E85-4F54-8E95-AB8F5DD74EF8}" name="Outcome"/>
     <tableColumn id="4" xr3:uid="{6E678DF2-F0CD-40A6-AEDB-CC2E158D34C7}" name="Duration [s]"/>
     <tableColumn id="5" xr3:uid="{E7E60375-F0D0-4F78-98DC-842559FEA71B}" name="Tokens"/>
-    <tableColumn id="6" xr3:uid="{6A2B8CFD-216F-42A3-AD46-D5BDE92AE5B4}" name="Cost [$]" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{6A2B8CFD-216F-42A3-AD46-D5BDE92AE5B4}" name="Cost [$]" dataDxfId="1"/>
     <tableColumn id="7" xr3:uid="{E12EEE88-959B-4D71-A927-9789CECC1F97}" name="LangSmith Traces"/>
     <tableColumn id="8" xr3:uid="{42C9F38F-B4D9-45B5-BB31-A67F037C65AA}" name="Comments"/>
-    <tableColumn id="9" xr3:uid="{659C8448-0B70-40B5-AA26-7C10544D76F8}" name="Model" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{659C8448-0B70-40B5-AA26-7C10544D76F8}" name="Model" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1444,25 +1559,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I109"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0"/>
-    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="1">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="68" zoomScaleNormal="25" workbookViewId="1">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
     <sheetView workbookViewId="2"/>
+    <sheetView workbookViewId="3"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="35" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" style="5" customWidth="1"/>
     <col min="3" max="3" width="15.21875" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" customWidth="1"/>
     <col min="5" max="5" width="13" style="10" customWidth="1"/>
     <col min="6" max="6" width="12.44140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="39.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="71.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1479,7 +1595,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>3</v>
@@ -1494,473 +1610,461 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="5" t="s">
-        <v>29</v>
+    <row r="2" spans="1:9" ht="57.6">
+      <c r="A2" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D2" s="10">
-        <v>68.23</v>
+        <v>87.16</v>
       </c>
       <c r="E2" s="10">
-        <v>6099</v>
+        <v>3347</v>
       </c>
       <c r="F2" s="9">
-        <v>6.3450000000000006E-2</v>
+        <v>3.465E-2</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>36</v>
+        <v>113</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="I2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="57.6">
-      <c r="A3" s="5" t="s">
-        <v>29</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>45</v>
       </c>
       <c r="D3" s="10">
-        <v>26.49</v>
+        <v>97.85</v>
       </c>
       <c r="E3" s="10">
-        <v>1447</v>
+        <v>3042</v>
       </c>
       <c r="F3" s="9">
-        <v>1.553E-2</v>
+        <v>3.1019999999999999E-2</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="H3" s="3"/>
       <c r="I3" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="5" t="s">
-        <v>29</v>
+      <c r="A4" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D4" s="10">
-        <v>52.24</v>
+        <v>70.36</v>
       </c>
       <c r="E4" s="10">
-        <v>2336</v>
-      </c>
-      <c r="F4" s="9">
-        <v>3.3930000000000002E-2</v>
+        <v>4563</v>
+      </c>
+      <c r="F4" s="28">
+        <v>5.0950000000000002E-2</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="H4" s="5"/>
       <c r="I4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="5" t="s">
-        <v>43</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="72">
+      <c r="A5" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D5" s="10">
-        <v>168.13</v>
+        <v>68.099999999999994</v>
       </c>
       <c r="E5" s="10">
-        <v>1944</v>
+        <v>4736</v>
       </c>
       <c r="F5" s="9">
-        <v>2.01E-2</v>
+        <v>5.2220000000000003E-2</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>40</v>
+        <v>114</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="I5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="57.6">
-      <c r="A6" s="5" t="s">
-        <v>43</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D6" s="10">
-        <v>119.39</v>
+        <v>49.48</v>
       </c>
       <c r="E6" s="10">
-        <v>2373</v>
+        <v>2192</v>
       </c>
       <c r="F6" s="9">
-        <v>2.4670000000000001E-2</v>
+        <v>2.2259999999999999E-2</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>49</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="H6" s="3"/>
       <c r="I6" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="5" t="s">
-        <v>43</v>
+      <c r="A7" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D7" s="10">
-        <v>673.96</v>
+        <v>76.84</v>
       </c>
       <c r="E7" s="10">
-        <v>4013</v>
-      </c>
-      <c r="F7" s="9">
-        <v>4.1889999999999997E-2</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>4270</v>
+      </c>
+      <c r="F7" s="28">
+        <v>4.6179999999999999E-2</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>183</v>
+      </c>
+      <c r="H7" s="5"/>
       <c r="I7" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
-        <v>50</v>
+        <v>111</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D8" s="10">
-        <v>69.73</v>
+        <v>129.03</v>
       </c>
       <c r="E8" s="10">
-        <v>2253</v>
+        <v>4498</v>
       </c>
       <c r="F8" s="9">
-        <v>2.2929999999999999E-2</v>
+        <v>4.5600000000000002E-2</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="I8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="5" t="s">
-        <v>50</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="57.6">
+      <c r="A9" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="10">
+        <v>114.39</v>
+      </c>
+      <c r="E9" s="10">
+        <v>5269</v>
+      </c>
+      <c r="F9" s="9">
+        <v>5.6070000000000002E-2</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="I9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" thickBot="1">
+      <c r="A10" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="10">
-        <v>36.54</v>
-      </c>
-      <c r="E9" s="10">
-        <v>1231</v>
-      </c>
-      <c r="F9" s="9">
-        <v>1.2529999999999999E-2</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="I9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="10">
-        <v>663.22</v>
-      </c>
-      <c r="E10" s="10">
-        <v>3658</v>
-      </c>
-      <c r="F10" s="9">
-        <v>3.9739999999999998E-2</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="57.6">
+      <c r="D10" s="30">
+        <v>95.83</v>
+      </c>
+      <c r="E10" s="30">
+        <v>5584</v>
+      </c>
+      <c r="F10" s="34">
+        <v>6.164E-2</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="H10" s="29"/>
+      <c r="I10" s="33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>45</v>
       </c>
       <c r="D11" s="10">
-        <v>29.37</v>
+        <v>93.21</v>
       </c>
       <c r="E11" s="10">
-        <v>2415</v>
+        <v>3047</v>
       </c>
       <c r="F11" s="9">
-        <v>2.4570000000000002E-2</v>
+        <v>3.2629999999999999E-2</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>67</v>
+        <v>107</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="I11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="57.6">
       <c r="A12" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D12" s="10">
-        <v>41.82</v>
+        <v>134.62</v>
       </c>
       <c r="E12" s="10">
-        <v>1713</v>
+        <v>3713</v>
       </c>
       <c r="F12" s="9">
-        <v>1.7749999999999998E-2</v>
+        <v>3.8510000000000003E-2</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>65</v>
+        <v>188</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="I12" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="D13" s="10">
-        <v>37.520000000000003</v>
+        <v>253.77</v>
       </c>
       <c r="E13" s="10">
-        <v>1654</v>
-      </c>
-      <c r="F13" s="9">
-        <v>1.7239999999999998E-2</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>66</v>
-      </c>
+        <v>6956</v>
+      </c>
+      <c r="F13" s="28">
+        <v>6.9680000000000006E-2</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="H13" s="5"/>
       <c r="I13" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="5" t="s">
-        <v>12</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="57.6">
+      <c r="A14" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="D14" s="10">
-        <v>78.08</v>
+        <v>66.42</v>
       </c>
       <c r="E14" s="10">
-        <v>2389</v>
+        <v>5421</v>
       </c>
       <c r="F14" s="9">
-        <v>2.555E-2</v>
+        <v>5.5550000000000002E-2</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>73</v>
+        <v>110</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="I14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="5" t="s">
-        <v>12</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="43.2">
+      <c r="A15" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="D15" s="10">
-        <v>18.89</v>
+        <v>125.96</v>
       </c>
       <c r="E15" s="10">
-        <v>1149</v>
+        <v>4650</v>
       </c>
       <c r="F15" s="9">
-        <v>1.3350000000000001E-2</v>
+        <v>4.8899999999999999E-2</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>75</v>
+        <v>191</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="I15" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="5" t="s">
-        <v>12</v>
+      <c r="A16" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="10">
+        <v>109.29</v>
+      </c>
+      <c r="E16" s="10">
+        <v>4768</v>
+      </c>
+      <c r="F16" s="28">
+        <v>4.87E-2</v>
+      </c>
+      <c r="G16" s="35" t="s">
+        <v>207</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="I16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="10">
-        <v>44.33</v>
-      </c>
-      <c r="E16" s="10">
-        <v>2532</v>
-      </c>
-      <c r="F16" s="9">
-        <v>2.682E-2</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="I16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="D17" s="10">
-        <v>29.82</v>
+        <v>65.47</v>
       </c>
       <c r="E17" s="10">
-        <v>1923</v>
+        <v>1909</v>
       </c>
       <c r="F17" s="9">
-        <v>1.9890000000000001E-2</v>
+        <v>2.009E-2</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="I17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="5" t="s">
-        <v>81</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="28.8">
+      <c r="A18" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>34</v>
@@ -1969,573 +2073,1947 @@
         <v>31</v>
       </c>
       <c r="D18" s="10">
-        <v>34.6</v>
+        <v>61.22</v>
       </c>
       <c r="E18" s="10">
-        <v>1495</v>
+        <v>2837</v>
       </c>
       <c r="F18" s="9">
-        <v>1.5509999999999999E-2</v>
+        <v>3.4770000000000002E-2</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>80</v>
+        <v>189</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>190</v>
       </c>
       <c r="I18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" thickBot="1">
+      <c r="A19" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="10">
-        <v>35.1</v>
-      </c>
-      <c r="E19" s="10">
-        <v>4510</v>
-      </c>
-      <c r="F19" s="9">
-        <v>4.5560000000000003E-2</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="I19" t="s">
-        <v>103</v>
+      <c r="D19" s="30">
+        <v>156</v>
+      </c>
+      <c r="E19" s="30">
+        <v>4485</v>
+      </c>
+      <c r="F19" s="34">
+        <v>5.2049999999999999E-2</v>
+      </c>
+      <c r="G19" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="H19" s="29"/>
+      <c r="I19" s="33" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="3" t="s">
-        <v>18</v>
+      <c r="A20" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="D20" s="10">
-        <v>75.599999999999994</v>
+        <v>78.08</v>
       </c>
       <c r="E20" s="10">
-        <v>2977</v>
+        <v>2389</v>
       </c>
       <c r="F20" s="9">
-        <v>3.0589999999999999E-2</v>
+        <v>2.555E-2</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="I20" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="3" t="s">
-        <v>18</v>
+      <c r="A21" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D21" s="10">
-        <v>63.93</v>
+        <v>67.45</v>
       </c>
       <c r="E21" s="10">
-        <v>1831</v>
+        <v>2399</v>
       </c>
       <c r="F21" s="9">
-        <v>1.8970000000000001E-2</v>
+        <v>2.5850000000000001E-2</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>88</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="H21" s="5"/>
       <c r="I21" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="81.599999999999994" customHeight="1">
-      <c r="A22" s="3" t="s">
-        <v>18</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="10">
+        <v>20.23</v>
+      </c>
+      <c r="E22" s="10">
+        <v>1471</v>
+      </c>
+      <c r="F22" s="28">
+        <v>1.617E-2</v>
+      </c>
+      <c r="G22" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="I22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="10">
-        <v>122.99</v>
-      </c>
-      <c r="E22" s="10">
-        <v>3930</v>
-      </c>
-      <c r="F22" s="9">
-        <v>3.9579999999999997E-2</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="I22" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="115.2" customHeight="1">
-      <c r="A23" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="C23" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D23" s="10">
-        <v>44.44</v>
+        <v>44.33</v>
       </c>
       <c r="E23" s="10">
-        <v>1959</v>
+        <v>2532</v>
       </c>
       <c r="F23" s="9">
-        <v>2.0389999999999998E-2</v>
+        <v>2.682E-2</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>94</v>
+        <v>78</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="I23" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="43.2">
-      <c r="A24" s="3" t="s">
-        <v>161</v>
+    <row r="24" spans="1:9">
+      <c r="A24" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D24" s="10">
-        <v>59.47</v>
+        <v>30.5</v>
       </c>
       <c r="E24" s="10">
-        <v>1571</v>
+        <v>2355</v>
       </c>
       <c r="F24" s="9">
-        <v>1.6449999999999999E-2</v>
+        <v>2.5049999999999999E-2</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>96</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="H24" s="5"/>
       <c r="I24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="73.2" customHeight="1">
-      <c r="A25" s="3" t="s">
-        <v>161</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="D25" s="10">
-        <v>983.76</v>
+        <v>31.09</v>
       </c>
       <c r="E25" s="10">
-        <v>3912</v>
-      </c>
-      <c r="F25" s="9">
-        <v>4.0579999999999998E-2</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>99</v>
-      </c>
+        <v>2355</v>
+      </c>
+      <c r="F25" s="28">
+        <v>2.5049999999999999E-2</v>
+      </c>
+      <c r="G25" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="H25" s="5"/>
       <c r="I25" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="3" t="s">
-        <v>100</v>
+      <c r="A26" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D26" s="10">
-        <v>65.47</v>
+        <v>18.89</v>
       </c>
       <c r="E26" s="10">
-        <v>1909</v>
+        <v>1149</v>
       </c>
       <c r="F26" s="9">
-        <v>2.009E-2</v>
+        <v>1.3350000000000001E-2</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="I26" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="3" t="s">
-        <v>100</v>
+      <c r="A27" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C27" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="10">
+        <v>19.739999999999998</v>
+      </c>
+      <c r="E27" s="10">
+        <v>1169</v>
+      </c>
+      <c r="F27" s="9">
+        <v>1.387E-2</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="H27" s="5"/>
+      <c r="I27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="58.2" thickBot="1">
+      <c r="A28" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="10">
-        <v>93.21</v>
-      </c>
-      <c r="E27" s="10">
-        <v>3047</v>
-      </c>
-      <c r="F27" s="9">
-        <v>3.2629999999999999E-2</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="I27" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="57.6">
-      <c r="A28" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D28" s="10">
-        <v>66.42</v>
-      </c>
-      <c r="E28" s="10">
-        <v>5421</v>
-      </c>
-      <c r="F28" s="9">
-        <v>5.5550000000000002E-2</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="I28" t="s">
-        <v>116</v>
+      <c r="D28" s="30">
+        <v>47.36</v>
+      </c>
+      <c r="E28" s="30">
+        <v>2489</v>
+      </c>
+      <c r="F28" s="34">
+        <v>2.767E-2</v>
+      </c>
+      <c r="G28" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="H28" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="I28" s="33" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="3" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D29" s="10">
-        <v>129.03</v>
+        <v>69.73</v>
       </c>
       <c r="E29" s="10">
-        <v>4498</v>
+        <v>2253</v>
       </c>
       <c r="F29" s="9">
-        <v>4.5600000000000002E-2</v>
+        <v>2.2929999999999999E-2</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>113</v>
+        <v>53</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>120</v>
+        <v>54</v>
       </c>
       <c r="I29" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="57.6">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" s="3" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D30" s="10">
-        <v>87.16</v>
-      </c>
-      <c r="E30" s="10">
-        <v>3347</v>
-      </c>
-      <c r="F30" s="9">
-        <v>3.465E-2</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>119</v>
-      </c>
+      <c r="D30" s="10"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="5"/>
       <c r="I30" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="72">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" s="3" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="10"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="5"/>
+      <c r="I31" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="10">
-        <v>68.099999999999994</v>
-      </c>
-      <c r="E31" s="10">
-        <v>4736</v>
-      </c>
-      <c r="F31" s="9">
-        <v>5.2220000000000003E-2</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="I31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D32" s="10">
-        <v>25.81</v>
+        <v>663.22</v>
       </c>
       <c r="E32" s="10">
-        <v>1170</v>
+        <v>3658</v>
       </c>
       <c r="F32" s="9">
-        <v>1.3259999999999999E-2</v>
+        <v>3.9739999999999998E-2</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>127</v>
+        <v>58</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>123</v>
+        <v>57</v>
       </c>
       <c r="I32" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="57.6">
-      <c r="A33" s="3" t="s">
-        <v>24</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D33" s="10">
-        <v>56.33</v>
-      </c>
-      <c r="E33" s="10">
-        <v>2001</v>
-      </c>
-      <c r="F33" s="9">
-        <v>2.1149999999999999E-2</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>128</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D33" s="10"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="5"/>
       <c r="I33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="3" t="s">
-        <v>24</v>
+      <c r="A34" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D34" s="10">
-        <v>24.08</v>
-      </c>
-      <c r="E34" s="10">
-        <v>1612</v>
-      </c>
-      <c r="F34" s="9">
-        <v>1.772E-2</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>124</v>
-      </c>
+      <c r="D34" s="10"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="5"/>
       <c r="I34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="5" t="s">
-        <v>129</v>
+        <v>50</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D35" s="10">
-        <v>118.54</v>
+        <v>36.54</v>
       </c>
       <c r="E35" s="10">
-        <v>6683</v>
+        <v>1231</v>
       </c>
       <c r="F35" s="9">
-        <v>6.9169999999999995E-2</v>
+        <v>1.2529999999999999E-2</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>131</v>
+        <v>55</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>130</v>
+        <v>56</v>
       </c>
       <c r="I35" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="72">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" s="5" t="s">
-        <v>129</v>
+        <v>50</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="D36" s="10"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="5"/>
+      <c r="I36" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15" thickBot="1">
+      <c r="A37" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="29"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" s="10">
+        <v>41.82</v>
+      </c>
+      <c r="E38" s="10">
+        <v>1713</v>
+      </c>
+      <c r="F38" s="9">
+        <v>1.7749999999999998E-2</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I38" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" s="10"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="5"/>
+      <c r="I39" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="10"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="5"/>
+      <c r="I40" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="57.6">
+      <c r="A41" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D41" s="10">
+        <v>29.37</v>
+      </c>
+      <c r="E41" s="10">
+        <v>2415</v>
+      </c>
+      <c r="F41" s="9">
+        <v>2.4570000000000002E-2</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I41" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="10"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="5"/>
+      <c r="I42" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" s="10"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="35"/>
+      <c r="H43" s="5"/>
+      <c r="I43" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D44" s="10">
+        <v>37.520000000000003</v>
+      </c>
+      <c r="E44" s="10">
+        <v>1654</v>
+      </c>
+      <c r="F44" s="9">
+        <v>1.7239999999999998E-2</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I44" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" s="10"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="5"/>
+      <c r="I45" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15" thickBot="1">
+      <c r="A46" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46" s="29"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="34"/>
+      <c r="G46" s="31"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="10">
+        <v>29.82</v>
+      </c>
+      <c r="E47" s="10">
+        <v>1923</v>
+      </c>
+      <c r="F47" s="9">
+        <v>1.9890000000000001E-2</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I47" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" s="10"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="5"/>
+      <c r="I48" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49" s="10"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="35"/>
+      <c r="H49" s="5"/>
+      <c r="I49" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D50" s="10">
+        <v>35.1</v>
+      </c>
+      <c r="E50" s="10">
+        <v>4510</v>
+      </c>
+      <c r="F50" s="9">
+        <v>4.5560000000000003E-2</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="I50" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D51" s="10"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="5"/>
+      <c r="I51" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D52" s="10"/>
+      <c r="F52" s="28"/>
+      <c r="G52" s="35"/>
+      <c r="H52" s="5"/>
+      <c r="I52" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D53" s="10">
+        <v>34.6</v>
+      </c>
+      <c r="E53" s="10">
+        <v>1495</v>
+      </c>
+      <c r="F53" s="9">
+        <v>1.5509999999999999E-2</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I53" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D54" s="10"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="5"/>
+      <c r="I54" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="15" thickBot="1">
+      <c r="A55" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C55" s="29"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="30"/>
+      <c r="F55" s="34"/>
+      <c r="G55" s="31"/>
+      <c r="H55" s="29"/>
+      <c r="I55" s="33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D56" s="10">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="E56" s="10">
+        <v>2977</v>
+      </c>
+      <c r="F56" s="9">
+        <v>3.0589999999999999E-2</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I56" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D57" s="10"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="3"/>
+      <c r="I57" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D58" s="10"/>
+      <c r="F58" s="28"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="5"/>
+      <c r="I58" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="43.2">
+      <c r="A59" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D59" s="10">
+        <v>122.99</v>
+      </c>
+      <c r="E59" s="10">
+        <v>3930</v>
+      </c>
+      <c r="F59" s="9">
+        <v>3.9579999999999997E-2</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I59" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D60" s="10"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="3"/>
+      <c r="I60" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D61" s="10"/>
+      <c r="F61" s="28"/>
+      <c r="G61" s="35"/>
+      <c r="H61" s="5"/>
+      <c r="I61" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D62" s="10">
+        <v>63.93</v>
+      </c>
+      <c r="E62" s="10">
+        <v>1831</v>
+      </c>
+      <c r="F62" s="9">
+        <v>1.8970000000000001E-2</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="I62" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D63" s="10"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="3"/>
+      <c r="I63" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="15" thickBot="1">
+      <c r="A64" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B64" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C64" s="29"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="34"/>
+      <c r="G64" s="31"/>
+      <c r="H64" s="29"/>
+      <c r="I64" s="33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="100.8">
+      <c r="A65" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D65" s="10">
+        <v>652.88</v>
+      </c>
+      <c r="E65" s="10">
+        <v>9253</v>
+      </c>
+      <c r="F65" s="9">
+        <v>9.425E-2</v>
+      </c>
+      <c r="G65" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="I65" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D66" s="10"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="35"/>
+      <c r="H66" s="3"/>
+      <c r="I66" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D67" s="10"/>
+      <c r="F67" s="28"/>
+      <c r="G67" s="35"/>
+      <c r="H67" s="5"/>
+      <c r="I67" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D68" s="10">
+        <v>118.54</v>
+      </c>
+      <c r="E68" s="10">
+        <v>6683</v>
+      </c>
+      <c r="F68" s="9">
+        <v>6.9169999999999995E-2</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="I68" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D69" s="10"/>
+      <c r="F69" s="9"/>
+      <c r="G69" s="35"/>
+      <c r="H69" s="3"/>
+      <c r="I69" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D70" s="10"/>
+      <c r="F70" s="28"/>
+      <c r="G70" s="6"/>
+      <c r="H70" s="5"/>
+      <c r="I70" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="72">
+      <c r="A71" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D71" s="10">
         <v>80.489999999999995</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E71" s="10">
         <v>3253</v>
       </c>
-      <c r="F36" s="9">
+      <c r="F71" s="9">
         <v>3.9710000000000002E-2</v>
       </c>
-      <c r="G36" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="I36" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="100.8">
-      <c r="A37" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B37" s="5" t="s">
+      <c r="G71" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="I71" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D72" s="10"/>
+      <c r="F72" s="9"/>
+      <c r="G72" s="35"/>
+      <c r="H72" s="3"/>
+      <c r="I72" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="15" thickBot="1">
+      <c r="A73" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="B73" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C73" s="29"/>
+      <c r="D73" s="30"/>
+      <c r="E73" s="30"/>
+      <c r="F73" s="34"/>
+      <c r="G73" s="31"/>
+      <c r="H73" s="29"/>
+      <c r="I73" s="33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="57.6">
+      <c r="A74" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B74" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C74" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D37" s="10">
-        <v>652.88</v>
-      </c>
-      <c r="E37" s="10">
-        <v>9253</v>
-      </c>
-      <c r="F37" s="9">
-        <v>9.425E-2</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="I37" t="s">
-        <v>116</v>
+      <c r="D74" s="10">
+        <v>119.39</v>
+      </c>
+      <c r="E74" s="10">
+        <v>2373</v>
+      </c>
+      <c r="F74" s="9">
+        <v>2.4670000000000001E-2</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I74" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D75" s="10"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="3"/>
+      <c r="I75" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D76" s="10"/>
+      <c r="F76" s="28"/>
+      <c r="G76" s="35"/>
+      <c r="H76" s="5"/>
+      <c r="I76" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D77" s="10">
+        <v>673.96</v>
+      </c>
+      <c r="E77" s="10">
+        <v>4013</v>
+      </c>
+      <c r="F77" s="9">
+        <v>4.1889999999999997E-2</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H77" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I77" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D78" s="10"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="3"/>
+      <c r="I78" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D79" s="10"/>
+      <c r="F79" s="28"/>
+      <c r="G79" s="35"/>
+      <c r="H79" s="5"/>
+      <c r="I79" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D80" s="10">
+        <v>168.13</v>
+      </c>
+      <c r="E80" s="10">
+        <v>1944</v>
+      </c>
+      <c r="F80" s="9">
+        <v>2.01E-2</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H80" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I80" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D81" s="10"/>
+      <c r="F81" s="9"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="3"/>
+      <c r="I81" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="15" thickBot="1">
+      <c r="A82" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B82" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C82" s="29"/>
+      <c r="D82" s="30"/>
+      <c r="E82" s="30"/>
+      <c r="F82" s="34"/>
+      <c r="G82" s="31"/>
+      <c r="H82" s="29"/>
+      <c r="I82" s="33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="86.4">
+      <c r="A83" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D83" s="10">
+        <v>44.44</v>
+      </c>
+      <c r="E83" s="10">
+        <v>1959</v>
+      </c>
+      <c r="F83" s="9">
+        <v>2.0389999999999998E-2</v>
+      </c>
+      <c r="G83" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I83" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D84" s="10"/>
+      <c r="F84" s="9"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="3"/>
+      <c r="I84" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D85" s="10"/>
+      <c r="F85" s="28"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="5"/>
+      <c r="I85" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="43.2">
+      <c r="A86" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D86" s="10">
+        <v>983.76</v>
+      </c>
+      <c r="E86" s="10">
+        <v>3912</v>
+      </c>
+      <c r="F86" s="9">
+        <v>4.0579999999999998E-2</v>
+      </c>
+      <c r="G86" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="I86" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="A87" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D87" s="10"/>
+      <c r="F87" s="9"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="3"/>
+      <c r="I87" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
+      <c r="A88" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D88" s="10"/>
+      <c r="F88" s="28"/>
+      <c r="G88" s="35"/>
+      <c r="H88" s="5"/>
+      <c r="I88" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="43.2">
+      <c r="A89" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D89" s="10">
+        <v>59.47</v>
+      </c>
+      <c r="E89" s="10">
+        <v>1571</v>
+      </c>
+      <c r="F89" s="9">
+        <v>1.6449999999999999E-2</v>
+      </c>
+      <c r="G89" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I89" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
+      <c r="A90" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D90" s="10"/>
+      <c r="F90" s="9"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="3"/>
+      <c r="I90" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="15" thickBot="1">
+      <c r="A91" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="B91" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C91" s="29"/>
+      <c r="D91" s="30"/>
+      <c r="E91" s="30"/>
+      <c r="F91" s="34"/>
+      <c r="G91" s="31"/>
+      <c r="H91" s="29"/>
+      <c r="I91" s="33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="57.6">
+      <c r="A92" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D92" s="10">
+        <v>56.33</v>
+      </c>
+      <c r="E92" s="10">
+        <v>2001</v>
+      </c>
+      <c r="F92" s="9">
+        <v>2.1149999999999999E-2</v>
+      </c>
+      <c r="G92" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I92" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
+      <c r="A93" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D93" s="10"/>
+      <c r="F93" s="9"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="5"/>
+      <c r="I93" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
+      <c r="A94" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D94" s="10">
+        <v>55.82</v>
+      </c>
+      <c r="E94" s="10">
+        <v>2480</v>
+      </c>
+      <c r="F94" s="28">
+        <v>2.64E-2</v>
+      </c>
+      <c r="G94" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="H94" s="5"/>
+      <c r="I94" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
+      <c r="A95" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D95" s="10">
+        <v>24.08</v>
+      </c>
+      <c r="E95" s="10">
+        <v>1612</v>
+      </c>
+      <c r="F95" s="9">
+        <v>1.772E-2</v>
+      </c>
+      <c r="G95" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="H95" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I95" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
+      <c r="A96" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D96" s="10"/>
+      <c r="F96" s="9"/>
+      <c r="G96" s="6"/>
+      <c r="H96" s="5"/>
+      <c r="I96" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
+      <c r="A97" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D97" s="10">
+        <v>42.36</v>
+      </c>
+      <c r="E97" s="10">
+        <v>2808</v>
+      </c>
+      <c r="F97" s="28">
+        <v>3.2559999999999999E-2</v>
+      </c>
+      <c r="G97" s="35" t="s">
+        <v>185</v>
+      </c>
+      <c r="H97" s="5"/>
+      <c r="I97" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
+      <c r="A98" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D98" s="10">
+        <v>25.81</v>
+      </c>
+      <c r="E98" s="10">
+        <v>1170</v>
+      </c>
+      <c r="F98" s="9">
+        <v>1.3259999999999999E-2</v>
+      </c>
+      <c r="G98" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="H98" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="I98" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
+      <c r="A99" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D99" s="10"/>
+      <c r="F99" s="9"/>
+      <c r="G99" s="6"/>
+      <c r="H99" s="5"/>
+      <c r="I99" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="15" thickBot="1">
+      <c r="A100" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B100" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C100" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D100" s="30">
+        <v>20</v>
+      </c>
+      <c r="E100" s="30">
+        <v>1192</v>
+      </c>
+      <c r="F100" s="34">
+        <v>1.384E-2</v>
+      </c>
+      <c r="G100" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="H100" s="29"/>
+      <c r="I100" s="33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
+      <c r="A101" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D101" s="10">
+        <v>52.24</v>
+      </c>
+      <c r="E101" s="10">
+        <v>2336</v>
+      </c>
+      <c r="F101" s="9">
+        <v>3.3930000000000002E-2</v>
+      </c>
+      <c r="G101" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H101" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I101" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
+      <c r="A102" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D102" s="10"/>
+      <c r="F102" s="9"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="5"/>
+      <c r="I102" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
+      <c r="A103" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D103" s="10"/>
+      <c r="F103" s="28"/>
+      <c r="G103" s="35"/>
+      <c r="H103" s="5"/>
+      <c r="I103" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
+      <c r="A104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D104" s="10">
+        <v>68.23</v>
+      </c>
+      <c r="E104" s="10">
+        <v>6099</v>
+      </c>
+      <c r="F104" s="9">
+        <v>6.3450000000000006E-2</v>
+      </c>
+      <c r="G104" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H104" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I104" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
+      <c r="A105" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D105" s="10"/>
+      <c r="F105" s="9"/>
+      <c r="G105" s="6"/>
+      <c r="H105" s="5"/>
+      <c r="I105" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
+      <c r="A106" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D106" s="10"/>
+      <c r="F106" s="28"/>
+      <c r="G106" s="35"/>
+      <c r="H106" s="5"/>
+      <c r="I106" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="57.6">
+      <c r="A107" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D107" s="10">
+        <v>26.49</v>
+      </c>
+      <c r="E107" s="10">
+        <v>1447</v>
+      </c>
+      <c r="F107" s="9">
+        <v>1.553E-2</v>
+      </c>
+      <c r="G107" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H107" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I107" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
+      <c r="A108" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D108" s="10"/>
+      <c r="F108" s="9"/>
+      <c r="G108" s="6"/>
+      <c r="H108" s="5"/>
+      <c r="I108" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="15" thickBot="1">
+      <c r="A109" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B109" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C109" s="29"/>
+      <c r="D109" s="30"/>
+      <c r="E109" s="30"/>
+      <c r="F109" s="34"/>
+      <c r="G109" s="31"/>
+      <c r="H109" s="29"/>
+      <c r="I109" s="33" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2557,7 +4035,12 @@
     <sheetView topLeftCell="A2" zoomScale="78" zoomScaleNormal="100" workbookViewId="1">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
-    <sheetView workbookViewId="2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="2">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="3">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -2588,16 +4071,16 @@
     </row>
     <row r="2" spans="1:5" ht="43.2">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>204</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>116</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
+        <v>117</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>69</v>
@@ -2605,19 +4088,17 @@
     </row>
     <row r="3" spans="1:5" ht="94.8" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>26</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="100.8">
@@ -2637,147 +4118,149 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="43.2">
+    <row r="5" spans="1:5" ht="28.8">
       <c r="A5" s="3" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>111</v>
+        <v>51</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>118</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="158.4">
       <c r="A6" s="3" t="s">
-        <v>29</v>
+        <v>97</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="E6" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="57.6">
+    <row r="7" spans="1:5" ht="43.2">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="E7" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="28.8">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="100.8">
       <c r="A8" s="3" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="3"/>
+        <v>89</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E8" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="52.2" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>97</v>
+        <v>128</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>61</v>
+        <v>137</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="57.6">
       <c r="A10" s="3" t="s">
-        <v>161</v>
+        <v>43</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="57.6">
+      <c r="A11" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="100.8">
-      <c r="A11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="86.4">
+    <row r="12" spans="1:5" ht="72">
       <c r="A12" s="3" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D12" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="E12" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="43.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="72">
       <c r="A13" s="3" t="s">
-        <v>129</v>
+        <v>29</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>138</v>
+        <v>39</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>137</v>
+        <v>28</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2810,178 +4293,179 @@
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="2">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="2">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
+    <sheetView workbookViewId="3"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="42.88671875" style="31" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" style="22" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" style="22" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="22"/>
+    <col min="1" max="1" width="42.88671875" style="23" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="19" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" style="19" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" style="19" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="20" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="28.8">
+      <c r="A2" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="1:6" ht="14.4">
+      <c r="A3" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="1:6" ht="136.80000000000001" customHeight="1">
+      <c r="A4" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+    </row>
+    <row r="5" spans="1:6" ht="14.4">
+      <c r="A5" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="28.8">
-      <c r="A2" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="B2" s="15" t="s">
+      <c r="C5" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+    </row>
+    <row r="6" spans="1:6" ht="28.8">
+      <c r="A6" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C6" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+    </row>
+    <row r="7" spans="1:6" ht="86.4">
+      <c r="A7" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D7" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+    </row>
+    <row r="8" spans="1:6" ht="28.8">
+      <c r="A8" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-    </row>
-    <row r="3" spans="1:6" ht="14.4">
-      <c r="A3" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="C3" s="15" t="s">
+      <c r="D8" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+    </row>
+    <row r="9" spans="1:6" ht="28.8">
+      <c r="A9" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+    </row>
+    <row r="10" spans="1:6" ht="144">
+      <c r="A10" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-    </row>
-    <row r="4" spans="1:6" ht="136.80000000000001" customHeight="1">
-      <c r="A4" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-    </row>
-    <row r="5" spans="1:6" ht="14.4">
-      <c r="A5" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-    </row>
-    <row r="6" spans="1:6" ht="28.8">
-      <c r="A6" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-    </row>
-    <row r="7" spans="1:6" ht="86.4">
-      <c r="A7" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-    </row>
-    <row r="8" spans="1:6" ht="28.8">
-      <c r="A8" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-    </row>
-    <row r="9" spans="1:6" ht="28.8">
-      <c r="A9" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-    </row>
-    <row r="10" spans="1:6" ht="144">
-      <c r="A10" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
+      <c r="D10" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2993,15 +4477,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E478D2DA-2B8C-45DE-9406-9F4B224C2A25}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="1">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="1">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="2">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
+    <sheetView workbookViewId="3"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -3010,7 +4495,7 @@
     <col min="3" max="3" width="15.21875" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" customWidth="1"/>
     <col min="5" max="5" width="15.77734375" customWidth="1"/>
-    <col min="6" max="6" width="14" style="27" customWidth="1"/>
+    <col min="6" max="6" width="14" style="22" customWidth="1"/>
     <col min="7" max="7" width="43.77734375" customWidth="1"/>
     <col min="8" max="8" width="14.77734375" customWidth="1"/>
     <col min="9" max="9" width="22.5546875" customWidth="1"/>
@@ -3030,9 +4515,9 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F1" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="22" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
@@ -3046,11 +4531,11 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="32" t="s">
-        <v>143</v>
+      <c r="A2" s="26" t="s">
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C2" t="s">
         <v>47</v>
@@ -3061,19 +4546,19 @@
       <c r="E2">
         <v>3166</v>
       </c>
-      <c r="F2" s="27">
+      <c r="F2" s="22">
         <v>3.4299999999999997E-2</v>
       </c>
       <c r="G2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="32" t="s">
-        <v>143</v>
+      <c r="A3" s="26" t="s">
+        <v>142</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
@@ -3082,15 +4567,15 @@
         <v>47</v>
       </c>
       <c r="G3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="32" t="s">
-        <v>143</v>
+      <c r="A4" s="26" t="s">
+        <v>142</v>
       </c>
       <c r="B4" t="s">
         <v>33</v>
@@ -3099,32 +4584,32 @@
         <v>47</v>
       </c>
       <c r="G4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="28.8">
-      <c r="A5" s="32" t="s">
-        <v>150</v>
+      <c r="A5" s="26" t="s">
+        <v>149</v>
       </c>
       <c r="B5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C5" t="s">
         <v>47</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="32" t="s">
-        <v>150</v>
+      <c r="A6" s="26" t="s">
+        <v>149</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>
@@ -3133,15 +4618,15 @@
         <v>47</v>
       </c>
       <c r="G6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="43.2">
-      <c r="A7" s="32" t="s">
-        <v>150</v>
+      <c r="A7" s="26" t="s">
+        <v>149</v>
       </c>
       <c r="B7" t="s">
         <v>33</v>
@@ -3150,32 +4635,32 @@
         <v>45</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="17" t="s">
-        <v>162</v>
+      <c r="A8" s="16" t="s">
+        <v>161</v>
       </c>
       <c r="B8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C8" t="s">
         <v>45</v>
       </c>
       <c r="G8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="17" t="s">
-        <v>162</v>
+      <c r="A9" s="16" t="s">
+        <v>161</v>
       </c>
       <c r="B9" t="s">
         <v>30</v>
@@ -3184,15 +4669,15 @@
         <v>45</v>
       </c>
       <c r="G9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="17" t="s">
-        <v>162</v>
+      <c r="A10" s="16" t="s">
+        <v>161</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>
@@ -3201,32 +4686,32 @@
         <v>47</v>
       </c>
       <c r="G10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="17" t="s">
-        <v>164</v>
+      <c r="A11" s="16" t="s">
+        <v>163</v>
       </c>
       <c r="B11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C11" t="s">
         <v>31</v>
       </c>
       <c r="G11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="28.8">
-      <c r="A12" s="17" t="s">
-        <v>164</v>
+      <c r="A12" s="16" t="s">
+        <v>163</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
@@ -3235,15 +4720,15 @@
         <v>45</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="17" t="s">
-        <v>164</v>
+      <c r="A13" s="16" t="s">
+        <v>163</v>
       </c>
       <c r="B13" t="s">
         <v>33</v>
@@ -3252,32 +4737,32 @@
         <v>31</v>
       </c>
       <c r="G13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="33" t="s">
-        <v>151</v>
+      <c r="A14" s="27" t="s">
+        <v>150</v>
       </c>
       <c r="B14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C14" t="s">
         <v>47</v>
       </c>
       <c r="G14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="33" t="s">
-        <v>151</v>
+      <c r="A15" s="27" t="s">
+        <v>150</v>
       </c>
       <c r="B15" t="s">
         <v>30</v>
@@ -3286,15 +4771,15 @@
         <v>47</v>
       </c>
       <c r="G15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="33" t="s">
-        <v>151</v>
+      <c r="A16" s="27" t="s">
+        <v>150</v>
       </c>
       <c r="B16" t="s">
         <v>33</v>
@@ -3303,32 +4788,32 @@
         <v>47</v>
       </c>
       <c r="G16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="28.8">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="B17" t="s">
         <v>153</v>
-      </c>
-      <c r="B17" t="s">
-        <v>154</v>
       </c>
       <c r="C17" t="s">
         <v>45</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="33" t="s">
-        <v>153</v>
+      <c r="A18" s="27" t="s">
+        <v>152</v>
       </c>
       <c r="B18" t="s">
         <v>30</v>
@@ -3337,15 +4822,15 @@
         <v>31</v>
       </c>
       <c r="G18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="33" t="s">
-        <v>153</v>
+      <c r="A19" s="27" t="s">
+        <v>152</v>
       </c>
       <c r="B19" t="s">
         <v>33</v>
@@ -3354,26 +4839,11 @@
         <v>45</v>
       </c>
       <c r="G19" t="s">
-        <v>172</v>
-      </c>
-      <c r="I19" s="25" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="I20" s="26"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="I21" s="26"/>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="I22" s="26"/>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="I23" s="26"/>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="I24" s="26"/>
+        <v>171</v>
+      </c>
+      <c r="I19" s="21" t="s">
+        <v>115</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add latex tables from excel using python
</commit_message>
<xml_diff>
--- a/documents/QnA_OSM.xlsx
+++ b/documents/QnA_OSM.xlsx
@@ -5,14 +5,13 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dev\master-thesis\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dev\masters-thesis\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DCB643-2B9D-4D1F-852A-F820E401B3F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227A5DDF-CE80-4D47-8002-033744A772E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="16305" activeTab="1" xr2:uid="{7CE71D1C-BB51-4650-8C03-0809E0E5E000}"/>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{A399FF6A-B9DA-4C49-8017-E0DA3374A652}"/>
+    <workbookView xWindow="31935" yWindow="3135" windowWidth="21600" windowHeight="11775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="16305" activeTab="1" xr2:uid="{A399FF6A-B9DA-4C49-8017-E0DA3374A652}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="268">
   <si>
     <t>Query</t>
   </si>
@@ -64,16 +63,10 @@
     <t>Query ID</t>
   </si>
   <si>
-    <t>nidarosdomen_polygon_retrieval</t>
-  </si>
-  <si>
     <t>Agent Type</t>
   </si>
   <si>
     <t xml:space="preserve">Retrieve a polygon of Nidarosdomen. </t>
-  </si>
-  <si>
-    <t>Correct  Response</t>
   </si>
   <si>
     <t>Adding a polygon of Nidarosdomen to the map.</t>
@@ -98,9 +91,6 @@
   </si>
   <si>
     <t>LangSmith Traces</t>
-  </si>
-  <si>
-    <t>num_trees_along_munkegata</t>
   </si>
   <si>
     <t>- Filter road data to get roads names 'Munkegata' and use a bounding box to only get results for Trondheim
@@ -129,12 +119,6 @@
     <t>vestfold_bbox</t>
   </si>
   <si>
-    <t>Minimum longitude: 9.7553357
-Minimum latitude: 58.720455
-Maximum longitude: 10.6750198
-Maximum latitude: 59.674011</t>
-  </si>
-  <si>
     <t>- Get  the correct county outline from places_polygons
 - Find the min/max lat/lon values (the bounding box)</t>
   </si>
@@ -188,9 +172,6 @@
     <t>Provide an outline of Oslo but exclude residential areas by computing their difference.</t>
   </si>
   <si>
-    <t>oslo_residental_difference</t>
-  </si>
-  <si>
     <t xml:space="preserve">The polygonal outline of Oslo with cutouts where there area areas classified as residental. </t>
   </si>
   <si>
@@ -211,9 +192,6 @@
 Fetched landuse polygons instead of the outline. Limited number of features, plus features from all over Norway. </t>
   </si>
   <si>
-    <t>glomma_counties_intersection</t>
-  </si>
-  <si>
     <t>How many counties does Glomma run through?</t>
   </si>
   <si>
@@ -303,9 +281,6 @@
   </si>
   <si>
     <t>/home/dev/master-thesis/tex/figs/nidarosdomen_retrieval_sql.png</t>
-  </si>
-  <si>
-    <t>nidarosdomen_retrieval</t>
   </si>
   <si>
     <t>3bba3d1f-f395-4ff7-a4b3-2c06c4041b71</t>
@@ -566,9 +541,6 @@
     <t xml:space="preserve">Retrieve roads in Oslo that have speed limit greater than or equal to 70 km/h. </t>
   </si>
   <si>
-    <t>oslo_roads_maxspeed_gte_70_kmh</t>
-  </si>
-  <si>
     <t>oslo_roads_maxspeed_gte_70_kmh_novice</t>
   </si>
   <si>
@@ -918,6 +890,27 @@
   </si>
   <si>
     <t>5d140677-fb58-4889-bbe2-97dec8addf17</t>
+  </si>
+  <si>
+    <t>Correct Response</t>
+  </si>
+  <si>
+    <t>oslo_roads_gte_70_kmh</t>
+  </si>
+  <si>
+    <t>oslo_residental_diff</t>
+  </si>
+  <si>
+    <t>num_trees_munkegata</t>
+  </si>
+  <si>
+    <t>glomma_counties</t>
+  </si>
+  <si>
+    <t>nidarosdomen_polygon</t>
+  </si>
+  <si>
+    <t>(9.7553357, 58.720455, 10.6750198, 59.674011)</t>
   </si>
 </sst>
 </file>
@@ -1435,7 +1428,7 @@
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{DF94BDDE-72C2-4E46-ACD5-0E5A636ABE68}" name="Query ID" dataDxfId="13"/>
     <tableColumn id="3" xr3:uid="{D36448D7-13F4-4A67-88D5-39F0C9732E25}" name="Query" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{88EFB23F-53BA-48C7-8DB1-E4BFB7F240EE}" name="Correct  Response" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{88EFB23F-53BA-48C7-8DB1-E4BFB7F240EE}" name="Correct Response" dataDxfId="11"/>
     <tableColumn id="5" xr3:uid="{568271BE-C334-41D7-BECB-CE936A642BD1}" name="Steps" dataDxfId="10"/>
     <tableColumn id="6" xr3:uid="{13F83F64-A4E0-456B-9916-E486752D5330}" name="Difficulty" dataDxfId="9"/>
   </tableColumns>
@@ -1740,9 +1733,8 @@
   <dimension ref="A1:I109"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="63" workbookViewId="2">
-      <selection activeCell="F89" sqref="F89"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="1">
+      <selection activeCell="A47" sqref="A47:A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1763,7 +1755,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>5</v>
@@ -1772,30 +1764,30 @@
         <v>4</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="57.6">
       <c r="A2" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D2" s="10">
         <v>87.16</v>
@@ -1807,24 +1799,24 @@
         <v>3.465E-2</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="I2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D3" s="10">
         <v>97.85</v>
@@ -1836,22 +1828,22 @@
         <v>3.1019999999999999E-2</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D4" s="10">
         <v>70.36</v>
@@ -1863,22 +1855,22 @@
         <v>5.0950000000000002E-2</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="72">
       <c r="A5" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D5" s="10">
         <v>68.099999999999994</v>
@@ -1890,24 +1882,24 @@
         <v>5.2220000000000003E-2</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="I5" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D6" s="10">
         <v>49.48</v>
@@ -1919,22 +1911,22 @@
         <v>2.2259999999999999E-2</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D7" s="10">
         <v>76.84</v>
@@ -1946,22 +1938,22 @@
         <v>4.6179999999999999E-2</v>
       </c>
       <c r="G7" s="35" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D8" s="10">
         <v>129.03</v>
@@ -1973,24 +1965,24 @@
         <v>4.5600000000000002E-2</v>
       </c>
       <c r="G8" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>118</v>
-      </c>
       <c r="I8" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="57.6">
       <c r="A9" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D9" s="10">
         <v>114.39</v>
@@ -2002,24 +1994,24 @@
         <v>5.6070000000000002E-2</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="I9" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" thickBot="1">
       <c r="A10" s="32" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D10" s="30">
         <v>95.83</v>
@@ -2031,22 +2023,22 @@
         <v>6.164E-2</v>
       </c>
       <c r="G10" s="31" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="H10" s="29"/>
       <c r="I10" s="33" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D11" s="10">
         <v>93.21</v>
@@ -2058,24 +2050,24 @@
         <v>3.2629999999999999E-2</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="I11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="57.6">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="43.2">
       <c r="A12" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D12" s="10">
         <v>134.62</v>
@@ -2087,24 +2079,24 @@
         <v>3.8510000000000003E-2</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="I12" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D13" s="10">
         <v>253.77</v>
@@ -2116,22 +2108,22 @@
         <v>6.9680000000000006E-2</v>
       </c>
       <c r="G13" s="35" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="57.6">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="43.2">
       <c r="A14" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D14" s="10">
         <v>66.42</v>
@@ -2143,24 +2135,24 @@
         <v>5.5550000000000002E-2</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="I14" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="43.2">
       <c r="A15" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D15" s="10">
         <v>125.96</v>
@@ -2172,24 +2164,24 @@
         <v>4.8899999999999999E-2</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="I15" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D16" s="10">
         <v>109.29</v>
@@ -2201,24 +2193,24 @@
         <v>4.87E-2</v>
       </c>
       <c r="G16" s="35" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="I16" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D17" s="10">
         <v>65.47</v>
@@ -2230,24 +2222,24 @@
         <v>2.009E-2</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="I17" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="28.8">
       <c r="A18" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D18" s="10">
         <v>61.22</v>
@@ -2259,24 +2251,24 @@
         <v>3.4770000000000002E-2</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="I18" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15" thickBot="1">
       <c r="A19" s="32" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D19" s="30">
         <v>156</v>
@@ -2288,22 +2280,22 @@
         <v>5.2049999999999999E-2</v>
       </c>
       <c r="G19" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="H19" s="29"/>
       <c r="I19" s="33" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D20" s="10">
         <v>78.08</v>
@@ -2315,24 +2307,24 @@
         <v>2.555E-2</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="I20" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D21" s="10">
         <v>67.45</v>
@@ -2344,22 +2336,22 @@
         <v>2.5850000000000001E-2</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D22" s="10">
         <v>20.23</v>
@@ -2371,24 +2363,24 @@
         <v>1.617E-2</v>
       </c>
       <c r="G22" s="35" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="I22" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D23" s="10">
         <v>44.33</v>
@@ -2400,24 +2392,24 @@
         <v>2.682E-2</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I23" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D24" s="10">
         <v>30.5</v>
@@ -2429,22 +2421,22 @@
         <v>2.5049999999999999E-2</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D25" s="10">
         <v>31.09</v>
@@ -2456,22 +2448,22 @@
         <v>2.5049999999999999E-2</v>
       </c>
       <c r="G25" s="35" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D26" s="10">
         <v>18.89</v>
@@ -2483,24 +2475,24 @@
         <v>1.3350000000000001E-2</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="I26" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D27" s="10">
         <v>19.739999999999998</v>
@@ -2512,22 +2504,22 @@
         <v>1.387E-2</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="58.2" thickBot="1">
       <c r="A28" s="29" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D28" s="30">
         <v>47.36</v>
@@ -2539,24 +2531,24 @@
         <v>2.767E-2</v>
       </c>
       <c r="G28" s="31" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="H28" s="32" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I28" s="33" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="3" t="s">
-        <v>50</v>
+        <v>265</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D29" s="10">
         <v>69.73</v>
@@ -2568,24 +2560,24 @@
         <v>2.2929999999999999E-2</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="I29" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="3" t="s">
-        <v>50</v>
+        <v>265</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D30" s="10">
         <v>65.569999999999993</v>
@@ -2597,22 +2589,22 @@
         <v>1.0619999999999999E-2</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="3" t="s">
-        <v>50</v>
+        <v>265</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D31" s="10">
         <v>67.37</v>
@@ -2624,22 +2616,22 @@
         <v>2.443E-2</v>
       </c>
       <c r="G31" s="35" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="5" t="s">
-        <v>50</v>
+      <c r="A32" s="3" t="s">
+        <v>265</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D32" s="10">
         <v>663.22</v>
@@ -2651,24 +2643,24 @@
         <v>3.9739999999999998E-2</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="I32" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="5" t="s">
-        <v>50</v>
+      <c r="A33" s="3" t="s">
+        <v>265</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D33" s="10">
         <v>295.93</v>
@@ -2680,24 +2672,24 @@
         <v>4.9779999999999998E-2</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="I33" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="5" t="s">
-        <v>50</v>
+      <c r="A34" s="3" t="s">
+        <v>265</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D34" s="10">
         <v>285.23</v>
@@ -2709,22 +2701,22 @@
         <v>2.3009999999999999E-2</v>
       </c>
       <c r="G34" s="35" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="5" t="s">
-        <v>50</v>
+      <c r="A35" s="3" t="s">
+        <v>265</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D35" s="10">
         <v>36.54</v>
@@ -2736,24 +2728,24 @@
         <v>1.2529999999999999E-2</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="I35" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="28.8">
-      <c r="A36" s="5" t="s">
-        <v>50</v>
+      <c r="A36" s="3" t="s">
+        <v>265</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D36" s="10">
         <v>63.65</v>
@@ -2765,24 +2757,24 @@
         <v>1.9140000000000001E-2</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="I36" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1">
-      <c r="A37" s="29" t="s">
-        <v>50</v>
+      <c r="A37" s="3" t="s">
+        <v>265</v>
       </c>
       <c r="B37" s="29" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D37" s="30">
         <v>22.81</v>
@@ -2794,22 +2786,22 @@
         <v>1.125E-2</v>
       </c>
       <c r="G37" s="31" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="H37" s="29"/>
       <c r="I37" s="33" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D38" s="10">
         <v>41.82</v>
@@ -2821,24 +2813,24 @@
         <v>1.7749999999999998E-2</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I38" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D39" s="10">
         <v>71.819999999999993</v>
@@ -2850,22 +2842,22 @@
         <v>2.283E-2</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D40" s="10">
         <v>47</v>
@@ -2877,22 +2869,22 @@
         <v>1.831E-2</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="57.6">
       <c r="A41" s="3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D41" s="10">
         <v>29.37</v>
@@ -2904,24 +2896,24 @@
         <v>2.4570000000000002E-2</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="I41" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D42" s="10">
         <v>41.95</v>
@@ -2933,22 +2925,22 @@
         <v>3.2480000000000002E-2</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="H42" s="5"/>
       <c r="I42" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D43" s="10">
         <v>40.549999999999997</v>
@@ -2960,22 +2952,22 @@
         <v>2.6409999999999999E-2</v>
       </c>
       <c r="G43" s="35" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="H43" s="5"/>
       <c r="I43" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D44" s="10">
         <v>37.520000000000003</v>
@@ -2987,24 +2979,24 @@
         <v>1.7239999999999998E-2</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I44" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D45" s="10">
         <v>27.55</v>
@@ -3016,22 +3008,22 @@
         <v>1.533E-2</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H45" s="5"/>
       <c r="I45" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="15" thickBot="1">
       <c r="A46" s="32" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B46" s="29" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D46" s="30">
         <v>41.22</v>
@@ -3043,22 +3035,22 @@
         <v>1.8610000000000002E-2</v>
       </c>
       <c r="G46" s="31" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="H46" s="29"/>
       <c r="I46" s="33" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="5" t="s">
-        <v>81</v>
+        <v>266</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D47" s="10">
         <v>29.82</v>
@@ -3070,24 +3062,24 @@
         <v>1.9890000000000001E-2</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="I47" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="5" t="s">
-        <v>81</v>
+        <v>266</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D48" s="10">
         <v>31.73</v>
@@ -3099,22 +3091,22 @@
         <v>1.9990000000000001E-2</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="H48" s="5"/>
       <c r="I48" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="5" t="s">
-        <v>81</v>
+        <v>266</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D49" s="10">
         <v>31.61</v>
@@ -3126,22 +3118,22 @@
         <v>2.002E-2</v>
       </c>
       <c r="G49" s="35" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="H49" s="5"/>
       <c r="I49" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="5" t="s">
-        <v>81</v>
+        <v>266</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D50" s="10">
         <v>35.1</v>
@@ -3153,24 +3145,24 @@
         <v>4.5560000000000003E-2</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="I50" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="5" t="s">
-        <v>81</v>
+        <v>266</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D51" s="10">
         <v>25.36</v>
@@ -3182,22 +3174,22 @@
         <v>3.705E-2</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="H51" s="5"/>
       <c r="I51" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="5" t="s">
-        <v>81</v>
+        <v>266</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D52" s="10">
         <v>33.35</v>
@@ -3209,22 +3201,22 @@
         <v>3.739E-2</v>
       </c>
       <c r="G52" s="35" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="H52" s="5"/>
       <c r="I52" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="5" t="s">
-        <v>81</v>
+        <v>266</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D53" s="10">
         <v>34.6</v>
@@ -3236,24 +3228,24 @@
         <v>1.5509999999999999E-2</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="I53" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="5" t="s">
-        <v>81</v>
+        <v>266</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D54" s="10">
         <v>63.43</v>
@@ -3265,22 +3257,22 @@
         <v>1.6029999999999999E-2</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="H54" s="5"/>
       <c r="I54" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="15" thickBot="1">
-      <c r="A55" s="29" t="s">
-        <v>81</v>
+      <c r="A55" s="5" t="s">
+        <v>266</v>
       </c>
       <c r="B55" s="29" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C55" s="29" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D55" s="30">
         <v>34.770000000000003</v>
@@ -3292,22 +3284,22 @@
         <v>1.6E-2</v>
       </c>
       <c r="G55" s="31" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="H55" s="29"/>
       <c r="I55" s="33" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="3" t="s">
-        <v>18</v>
+        <v>264</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D56" s="10">
         <v>75.599999999999994</v>
@@ -3319,24 +3311,24 @@
         <v>3.0589999999999999E-2</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="I56" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="3" t="s">
-        <v>18</v>
+        <v>264</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D57" s="10">
         <v>80.13</v>
@@ -3348,22 +3340,22 @@
         <v>3.0700000000000002E-2</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="H57" s="3"/>
       <c r="I57" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="3" t="s">
-        <v>18</v>
+        <v>264</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D58" s="10">
         <v>57.66</v>
@@ -3375,24 +3367,24 @@
         <v>2.503E-2</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="I58" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="43.2">
       <c r="A59" s="3" t="s">
-        <v>18</v>
+        <v>264</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D59" s="10">
         <v>122.99</v>
@@ -3404,24 +3396,24 @@
         <v>3.9579999999999997E-2</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="I59" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="3" t="s">
-        <v>18</v>
+        <v>264</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D60" s="10">
         <v>916.13</v>
@@ -3433,22 +3425,22 @@
         <v>2.4060000000000002E-2</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="H60" s="3"/>
       <c r="I60" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="3" t="s">
-        <v>18</v>
+        <v>264</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D61" s="10">
         <v>911.18</v>
@@ -3460,22 +3452,22 @@
         <v>9.3390000000000001E-2</v>
       </c>
       <c r="G61" s="35" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="H61" s="5"/>
       <c r="I61" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="43.2">
       <c r="A62" s="3" t="s">
-        <v>18</v>
+        <v>264</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D62" s="10">
         <v>63.93</v>
@@ -3487,24 +3479,24 @@
         <v>1.8970000000000001E-2</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="I62" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="3" t="s">
-        <v>18</v>
+        <v>264</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D63" s="10">
         <v>77.45</v>
@@ -3516,24 +3508,24 @@
         <v>3.4759999999999999E-2</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="I63" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="15" thickBot="1">
-      <c r="A64" s="32" t="s">
-        <v>18</v>
+      <c r="A64" s="3" t="s">
+        <v>264</v>
       </c>
       <c r="B64" s="29" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C64" s="29" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D64" s="30">
         <v>64.47</v>
@@ -3545,24 +3537,24 @@
         <v>1.668E-2</v>
       </c>
       <c r="G64" s="31" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="I64" s="33" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="86.4">
       <c r="A65" s="5" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D65" s="10">
         <v>652.88</v>
@@ -3574,24 +3566,24 @@
         <v>9.425E-2</v>
       </c>
       <c r="G65" s="35" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="I65" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="5" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D66" s="10">
         <v>102.38</v>
@@ -3603,22 +3595,22 @@
         <v>3.7699999999999997E-2</v>
       </c>
       <c r="G66" s="35" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="H66" s="3"/>
       <c r="I66" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="5" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D67" s="10">
         <v>258.52</v>
@@ -3630,22 +3622,22 @@
         <v>6.9589999999999999E-2</v>
       </c>
       <c r="G67" s="35" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="H67" s="5"/>
       <c r="I67" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="5" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D68" s="10">
         <v>118.54</v>
@@ -3657,24 +3649,24 @@
         <v>6.9169999999999995E-2</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="I68" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="28.8">
       <c r="A69" s="5" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D69" s="10">
         <v>129.4</v>
@@ -3686,22 +3678,22 @@
         <v>8.6059999999999998E-2</v>
       </c>
       <c r="G69" s="35" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="H69" s="3"/>
       <c r="I69" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="5" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D70" s="10">
         <v>373.37</v>
@@ -3713,22 +3705,22 @@
         <v>0.11268</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="H70" s="5"/>
       <c r="I70" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="72">
       <c r="A71" s="5" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D71" s="10">
         <v>80.489999999999995</v>
@@ -3740,24 +3732,24 @@
         <v>3.9710000000000002E-2</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="I71" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="5" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D72" s="10">
         <v>83.78</v>
@@ -3769,22 +3761,22 @@
         <v>2.768E-2</v>
       </c>
       <c r="G72" s="35" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="H72" s="3"/>
       <c r="I72" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="15" thickBot="1">
       <c r="A73" s="29" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B73" s="29" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C73" s="29" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D73" s="30">
         <v>88.63</v>
@@ -3796,22 +3788,22 @@
         <v>3.739E-2</v>
       </c>
       <c r="G73" s="31" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="H73" s="29"/>
       <c r="I73" s="33" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="57.6">
       <c r="A74" s="5" t="s">
-        <v>43</v>
+        <v>263</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D74" s="10">
         <v>119.39</v>
@@ -3823,24 +3815,24 @@
         <v>2.4670000000000001E-2</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I74" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" s="5" t="s">
-        <v>43</v>
+        <v>263</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D75" s="10">
         <v>114.92</v>
@@ -3852,24 +3844,24 @@
         <v>3.1530000000000002E-2</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="I75" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="5" t="s">
-        <v>43</v>
+        <v>263</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D76" s="10">
         <v>121.17</v>
@@ -3881,22 +3873,22 @@
         <v>2.7230000000000001E-2</v>
       </c>
       <c r="G76" s="35" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="H76" s="5"/>
       <c r="I76" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" s="5" t="s">
-        <v>43</v>
+        <v>263</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D77" s="10">
         <v>673.96</v>
@@ -3908,24 +3900,24 @@
         <v>4.1889999999999997E-2</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="I77" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" s="5" t="s">
-        <v>43</v>
+        <v>263</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D78" s="10">
         <v>2190.08</v>
@@ -3937,24 +3929,24 @@
         <v>3.9629999999999999E-2</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="I78" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" s="5" t="s">
-        <v>43</v>
+        <v>263</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D79" s="10">
         <v>2290.09</v>
@@ -3966,22 +3958,22 @@
         <v>3.7679999999999998E-2</v>
       </c>
       <c r="G79" s="35" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="H79" s="5"/>
       <c r="I79" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="80" spans="1:9">
       <c r="A80" s="5" t="s">
-        <v>43</v>
+        <v>263</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D80" s="10">
         <v>168.13</v>
@@ -3993,24 +3985,24 @@
         <v>2.01E-2</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I80" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="43.2">
       <c r="A81" s="5" t="s">
-        <v>43</v>
+        <v>263</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D81" s="10">
         <v>94.4</v>
@@ -4022,24 +4014,24 @@
         <v>2.6360000000000001E-2</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I81" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="15" thickBot="1">
-      <c r="A82" s="29" t="s">
-        <v>43</v>
+      <c r="A82" s="5" t="s">
+        <v>263</v>
       </c>
       <c r="B82" s="29" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C82" s="29" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D82" s="30">
         <v>136.12</v>
@@ -4051,22 +4043,22 @@
         <v>2.623E-2</v>
       </c>
       <c r="G82" s="31" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="H82" s="29"/>
       <c r="I82" s="33" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" ht="86.4">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="72">
       <c r="A83" s="3" t="s">
-        <v>159</v>
+        <v>262</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D83" s="10">
         <v>44.44</v>
@@ -4078,24 +4070,24 @@
         <v>2.0389999999999998E-2</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="I83" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="3" t="s">
-        <v>159</v>
+        <v>262</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D84" s="10">
         <v>58.61</v>
@@ -4107,22 +4099,22 @@
         <v>2.1090000000000001E-2</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="H84" s="3"/>
       <c r="I84" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="85" spans="1:9">
       <c r="A85" s="3" t="s">
-        <v>159</v>
+        <v>262</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D85" s="10">
         <v>35.549999999999997</v>
@@ -4134,22 +4126,22 @@
         <v>2.0629999999999999E-2</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="H85" s="5"/>
       <c r="I85" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="43.2">
       <c r="A86" s="3" t="s">
-        <v>159</v>
+        <v>262</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D86" s="10">
         <v>983.76</v>
@@ -4161,24 +4153,24 @@
         <v>4.0579999999999998E-2</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="I86" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" s="3" t="s">
-        <v>159</v>
+        <v>262</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D87" s="10">
         <v>757.7</v>
@@ -4190,22 +4182,22 @@
         <v>3.8929999999999999E-2</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="H87" s="3"/>
       <c r="I87" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" s="3" t="s">
-        <v>159</v>
+        <v>262</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D88" s="10">
         <v>849.06</v>
@@ -4217,22 +4209,22 @@
         <v>3.9170000000000003E-2</v>
       </c>
       <c r="G88" s="35" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="H88" s="5"/>
       <c r="I88" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="43.2">
       <c r="A89" s="3" t="s">
-        <v>159</v>
+        <v>262</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D89" s="10">
         <v>59.47</v>
@@ -4244,24 +4236,24 @@
         <v>1.6449999999999999E-2</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="H89" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I89" t="s">
         <v>95</v>
-      </c>
-      <c r="I89" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="3" t="s">
-        <v>159</v>
+        <v>262</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D90" s="10">
         <v>44.79</v>
@@ -4273,22 +4265,22 @@
         <v>1.6590000000000001E-2</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="H90" s="3"/>
       <c r="I90" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="15" thickBot="1">
-      <c r="A91" s="32" t="s">
-        <v>159</v>
+      <c r="A91" s="3" t="s">
+        <v>262</v>
       </c>
       <c r="B91" s="29" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C91" s="29" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D91" s="30">
         <v>41.67</v>
@@ -4300,22 +4292,22 @@
         <v>1.6119999999999999E-2</v>
       </c>
       <c r="G91" s="31" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="H91" s="29"/>
       <c r="I91" s="33" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="57.6">
       <c r="A92" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D92" s="10">
         <v>56.33</v>
@@ -4327,24 +4319,24 @@
         <v>2.1149999999999999E-2</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="H92" s="3" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="I92" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="28.8">
       <c r="A93" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D93" s="10">
         <v>50.38</v>
@@ -4356,22 +4348,22 @@
         <v>3.4750000000000003E-2</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="H93" s="5"/>
       <c r="I93" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="94" spans="1:9">
       <c r="A94" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D94" s="10">
         <v>55.82</v>
@@ -4383,22 +4375,22 @@
         <v>2.64E-2</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="H94" s="5"/>
       <c r="I94" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="95" spans="1:9">
       <c r="A95" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D95" s="10">
         <v>24.08</v>
@@ -4410,24 +4402,24 @@
         <v>1.772E-2</v>
       </c>
       <c r="G95" s="6" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="H95" s="5" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="I95" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="96" spans="1:9">
       <c r="A96" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D96" s="10">
         <v>33.630000000000003</v>
@@ -4439,22 +4431,22 @@
         <v>2.6040000000000001E-2</v>
       </c>
       <c r="G96" s="6" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="H96" s="5"/>
       <c r="I96" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="97" spans="1:9">
       <c r="A97" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D97" s="10">
         <v>42.36</v>
@@ -4466,22 +4458,22 @@
         <v>3.2559999999999999E-2</v>
       </c>
       <c r="G97" s="35" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="H97" s="5"/>
       <c r="I97" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="98" spans="1:9">
       <c r="A98" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D98" s="10">
         <v>25.81</v>
@@ -4493,24 +4485,24 @@
         <v>1.3259999999999999E-2</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="H98" s="5" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="I98" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="99" spans="1:9">
       <c r="A99" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D99" s="10">
         <v>32.590000000000003</v>
@@ -4522,22 +4514,22 @@
         <v>1.6469999999999999E-2</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H99" s="5"/>
       <c r="I99" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="15" thickBot="1">
       <c r="A100" s="32" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B100" s="29" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C100" s="29" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D100" s="30">
         <v>20</v>
@@ -4549,22 +4541,22 @@
         <v>1.384E-2</v>
       </c>
       <c r="G100" s="31" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="H100" s="29"/>
       <c r="I100" s="33" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="101" spans="1:9">
       <c r="A101" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D101" s="10">
         <v>52.24</v>
@@ -4576,24 +4568,24 @@
         <v>3.3930000000000002E-2</v>
       </c>
       <c r="G101" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H101" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I101" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="102" spans="1:9">
       <c r="A102" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D102" s="10">
         <v>204.07</v>
@@ -4605,22 +4597,22 @@
         <v>5.5259999999999997E-2</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="H102" s="5"/>
       <c r="I102" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="103" spans="1:9">
       <c r="A103" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D103" s="10">
         <v>133.4</v>
@@ -4632,22 +4624,22 @@
         <v>4.283E-2</v>
       </c>
       <c r="G103" s="35" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="H103" s="5"/>
       <c r="I103" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="104" spans="1:9">
       <c r="A104" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B104" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B104" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="C104" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D104" s="10">
         <v>68.23</v>
@@ -4659,24 +4651,24 @@
         <v>6.3450000000000006E-2</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H104" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I104" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="105" spans="1:9">
       <c r="A105" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B105" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B105" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="C105" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D105" s="10">
         <v>86.32</v>
@@ -4688,22 +4680,22 @@
         <v>6.7949999999999997E-2</v>
       </c>
       <c r="G105" s="6" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="H105" s="5"/>
       <c r="I105" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="106" spans="1:9">
       <c r="A106" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B106" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B106" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="C106" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D106" s="10">
         <v>89.98</v>
@@ -4715,22 +4707,22 @@
         <v>7.3849999999999999E-2</v>
       </c>
       <c r="G106" s="35" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H106" s="5"/>
       <c r="I106" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" ht="57.6">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="43.2">
       <c r="A107" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D107" s="10">
         <v>26.49</v>
@@ -4742,24 +4734,24 @@
         <v>1.553E-2</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H107" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I107" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="108" spans="1:9">
       <c r="A108" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D108" s="10">
         <v>47.59</v>
@@ -4771,22 +4763,22 @@
         <v>2.1950000000000001E-2</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="H108" s="5"/>
       <c r="I108" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="15" thickBot="1">
       <c r="A109" s="29" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B109" s="29" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C109" s="29" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D109" s="30">
         <v>36.200000000000003</v>
@@ -4798,11 +4790,11 @@
         <v>1.6729999999999998E-2</v>
       </c>
       <c r="G109" s="31" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="H109" s="29"/>
       <c r="I109" s="33" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -4818,13 +4810,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3BFF00C-9B20-4D57-A0F3-3732FF3EA698}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="57" zoomScaleNormal="57" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="75" workbookViewId="1">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -4844,207 +4833,207 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>10</v>
+        <v>261</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="43.2">
       <c r="A2" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="94.8" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="100.8">
       <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8">
       <c r="A5" s="3" t="s">
-        <v>50</v>
+        <v>265</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="158.4">
       <c r="A6" s="3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="43.2">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>266</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="100.8">
       <c r="A8" s="3" t="s">
-        <v>18</v>
+        <v>264</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="52.2" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="57.6">
       <c r="A10" s="3" t="s">
-        <v>43</v>
+        <v>263</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="57.6">
       <c r="A11" s="3" t="s">
-        <v>159</v>
+        <v>262</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="72">
       <c r="A12" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>25</v>
+        <v>267</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="72">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -5075,7 +5064,6 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
@@ -5093,155 +5081,155 @@
         <v>6</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="28.8">
       <c r="A2" s="24" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6" ht="14.4">
       <c r="A3" s="24" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" ht="136.80000000000001" customHeight="1">
       <c r="A4" s="24" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:6" ht="14.4">
       <c r="A5" s="16" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:6" ht="28.8">
       <c r="A6" s="16" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6" ht="86.4">
       <c r="A7" s="16" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
     </row>
     <row r="8" spans="1:6" ht="28.8">
       <c r="A8" s="25" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
     </row>
     <row r="9" spans="1:6" ht="28.8">
       <c r="A9" s="25" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
     </row>
     <row r="10" spans="1:6" ht="144">
       <c r="A10" s="25" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
@@ -5259,8 +5247,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
-    <sheetView zoomScale="82" workbookViewId="2">
+    <sheetView zoomScale="82" workbookViewId="1">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -5282,7 +5269,7 @@
         <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -5291,30 +5278,30 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="F1" s="22" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="26" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D2">
         <v>105.27</v>
@@ -5326,299 +5313,299 @@
         <v>3.4299999999999997E-2</v>
       </c>
       <c r="G2" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="26" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="26" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G4" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="28.8">
       <c r="A5" s="26" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="26" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G6" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="43.2">
       <c r="A7" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="I7" s="12" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="16" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B8" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="16" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G9" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="16" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G10" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="16" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B11" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G11" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="28.8">
       <c r="A12" s="16" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="16" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G13" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="27" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B14" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G14" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="27" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G15" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="27" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G16" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="28.8">
       <c r="A17" s="27" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B17" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="27" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G18" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="27" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G19" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="I19" s="21" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete tests with updated db query tool
</commit_message>
<xml_diff>
--- a/documents/QnA_OSM.xlsx
+++ b/documents/QnA_OSM.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dev\masters-thesis\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B8DB92-9D3B-4EB4-859E-84F2C18A7573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED81073-48CC-4F12-98F6-B09C27A2383F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31935" yWindow="3135" windowWidth="21600" windowHeight="11775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="16305" activeTab="2" xr2:uid="{A399FF6A-B9DA-4C49-8017-E0DA3374A652}"/>
+    <workbookView xWindow="1512" yWindow="1272" windowWidth="21624" windowHeight="11784" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="16305" activeTab="1" xr2:uid="{A399FF6A-B9DA-4C49-8017-E0DA3374A652}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="16305" activeTab="2" xr2:uid="{6C98443E-C637-4C57-82B4-E28D057BD50C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tests" sheetId="1" r:id="rId1"/>
-    <sheet name="Questions" sheetId="2" r:id="rId2"/>
-    <sheet name="Prompt Levels" sheetId="3" r:id="rId3"/>
-    <sheet name="PL Tests" sheetId="4" r:id="rId4"/>
+    <sheet name="Tests_old" sheetId="5" r:id="rId1"/>
+    <sheet name="Tests" sheetId="1" r:id="rId2"/>
+    <sheet name="Questions" sheetId="2" r:id="rId3"/>
+    <sheet name="Prompt Levels" sheetId="3" r:id="rId4"/>
+    <sheet name="PL Tests" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="304">
   <si>
     <t>Query</t>
   </si>
@@ -896,6 +898,131 @@
   </si>
   <si>
     <t>(9.7553357, 58.720455, 10.6750198, 59.674011)</t>
+  </si>
+  <si>
+    <t>Reason for Failure</t>
+  </si>
+  <si>
+    <t>required_followup</t>
+  </si>
+  <si>
+    <t>inaccurate_parameters</t>
+  </si>
+  <si>
+    <t>wrong_or_inaccurate_data</t>
+  </si>
+  <si>
+    <t>inaccurate_or_erroneous_code</t>
+  </si>
+  <si>
+    <t>d1c40bac-7bff-4c7e-8f8a-8c9f78035325</t>
+  </si>
+  <si>
+    <t>efbfbf44-9d85-4511-a92f-0a8a2423bd60
+a0b559d5-cdc5-427f-a7f8-c1f3275d7c13</t>
+  </si>
+  <si>
+    <t>b46138fd-31f4-443a-b926-2ad509d2f6a1
+4945d55f-1300-4d56-bd8d-4be1d2265bce</t>
+  </si>
+  <si>
+    <t>2209ca54-0dbb-4c48-8b4c-73c1a5f97687</t>
+  </si>
+  <si>
+    <t>e9c9e507-d9d8-487e-8aaa-9512b6530aef</t>
+  </si>
+  <si>
+    <t>51bca182-2139-4501-8fc6-505d0e257658</t>
+  </si>
+  <si>
+    <t>cdc17b6c-37e3-454c-bec2-6cf4263c16e7</t>
+  </si>
+  <si>
+    <t>bcb4f4a3-987e-432c-bcf7-7ec8de53097b</t>
+  </si>
+  <si>
+    <t>3cc24c05-e700-4511-96ff-905747a24055</t>
+  </si>
+  <si>
+    <t>3ff9a1b8-c472-44e1-a9df-0a5119b1faf8</t>
+  </si>
+  <si>
+    <t>c89d9c0e-5f57-487c-87cc-95a282548d0a</t>
+  </si>
+  <si>
+    <t>e52c6e20-7e1b-43b8-9d3d-0d9052825ba5</t>
+  </si>
+  <si>
+    <t>880ad48d-c90c-46b7-8116-5854f77e15cc</t>
+  </si>
+  <si>
+    <t>05955e0e-e410-46d4-83a1-69f067520e24</t>
+  </si>
+  <si>
+    <t>1bdf5a23-c5af-446e-a3db-c59c7f36d517</t>
+  </si>
+  <si>
+    <t>daaa7c7f-4d37-4c83-8ba2-33827fc2da17</t>
+  </si>
+  <si>
+    <t>6eb27608-e1b6-4dc4-af30-52dd00212178</t>
+  </si>
+  <si>
+    <t>a503c127-5aac-4633-8fd8-d642825ed1f4</t>
+  </si>
+  <si>
+    <t>f1ebd745-0a73-4f9c-a832-d19c40c09aa8</t>
+  </si>
+  <si>
+    <t>3068b01f-f583-44b1-9101-f7ae1f6bd412</t>
+  </si>
+  <si>
+    <t>ccdbd6c3-0fbb-4140-a2ea-b3d587559e57</t>
+  </si>
+  <si>
+    <t>b1dc2f9f-271e-4076-8b86-1cc23c957503</t>
+  </si>
+  <si>
+    <t>27706909-d483-4a61-8a38-ada78511c1c9</t>
+  </si>
+  <si>
+    <t>d4d1bd55-155a-4bbf-a227-75213e468973</t>
+  </si>
+  <si>
+    <t>f868bc7f-410f-45a6-9646-80c7905b8cfc</t>
+  </si>
+  <si>
+    <t>0761be32-9cfb-403b-968e-813e2d0b60bb</t>
+  </si>
+  <si>
+    <t>c31066af-fcb1-4668-bbbc-1ffc2c6b4e31</t>
+  </si>
+  <si>
+    <t>f89ce5de-1563-4128-9b48-af2d8d92d752</t>
+  </si>
+  <si>
+    <t>1b1f88f3-d853-4f95-b80c-60bab144970a</t>
+  </si>
+  <si>
+    <t>bbfe0a5a-d63d-4026-835c-182040270dad</t>
+  </si>
+  <si>
+    <t>944d143c-e4cc-4e46-b472-8a3682208bd8</t>
+  </si>
+  <si>
+    <t>78a0f5bd-8c92-40ae-bf18-fa5bc3c34d0b</t>
+  </si>
+  <si>
+    <t>d2c03c03-a0eb-4e7b-a425-9367c9e99151</t>
+  </si>
+  <si>
+    <t>1fbd4d52-fb34-46a0-b6c6-2802e3c6bf20</t>
+  </si>
+  <si>
+    <t>0567d4f4-3e26-4c4e-a573-4f1760fbf98c</t>
+  </si>
+  <si>
+    <t>1042590a-c464-4892-a14f-b6da87c2c3ff</t>
   </si>
 </sst>
 </file>
@@ -1033,7 +1160,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1100,12 +1227,70 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="37">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1383,70 +1568,93 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{83D2B9CE-16C8-4DB7-89A3-592E6CC65025}" name="Table3" displayName="Table3" ref="A1:I109" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3E5ADE26-EEAE-43F3-9F4A-1D074CA261C5}" name="Table36" displayName="Table36" ref="A1:J109" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8">
+  <autoFilter ref="A1:J109" xr:uid="{83D2B9CE-16C8-4DB7-89A3-592E6CC65025}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I109">
+    <sortCondition ref="A2:A109"/>
+    <sortCondition ref="B2:B109"/>
+  </sortState>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{92ED4BCE-FC72-4BFE-B7BF-146AC02E260B}" name="Query ID" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{687659E0-450C-44F9-9EBB-F73732669236}" name="Agent Type" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{1B2851B1-FA93-497C-A3AF-ADF0566FA121}" name="Outcome" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{F3425F5C-8B3A-4FB0-AF42-9FA30792500E}" name="Duration [s]" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{ADAF3E28-BF66-4E9F-A5B0-89C2D442F947}" name="Tokens" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{4150BE77-C1BD-4843-8320-29AF7C00CAFA}" name="Cost [$]" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{29F88C50-3EAB-42D3-8A58-97FFA9D22E1B}" name="LangSmith Traces" dataDxfId="1" dataCellStyle="Hyperlink"/>
+    <tableColumn id="7" xr3:uid="{37F682B6-D553-4DEC-AB91-F0B11BFCD6D1}" name="Comments" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{AB696860-67D7-40BF-BB26-CF7D9306BA69}" name="Model"/>
+    <tableColumn id="9" xr3:uid="{792B33F4-3427-4629-839C-3B17F1DA17CA}" name="Reason for Failure"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{83D2B9CE-16C8-4DB7-89A3-592E6CC65025}" name="Table3" displayName="Table3" ref="A1:I109" totalsRowShown="0" headerRowDxfId="36" headerRowBorderDxfId="35">
   <autoFilter ref="A1:I109" xr:uid="{83D2B9CE-16C8-4DB7-89A3-592E6CC65025}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I109">
     <sortCondition ref="A2:A109"/>
     <sortCondition ref="B2:B109"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5E217325-9314-4066-9478-85ED196C3B0A}" name="Query ID" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{97EF1974-2076-449A-A0D4-15EA85F8280F}" name="Agent Type" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{8D1D516B-C100-437C-94C9-405B27E99C54}" name="Outcome" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{62F2D408-C3F9-4A29-8859-C68FE5808C7B}" name="Duration [s]" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{E204E73A-EDA9-4F27-8D7B-6E638A0FF18B}" name="Tokens" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{D7F4AA3D-7E52-4896-B7EA-B50F31C8EB43}" name="Cost [$]" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{A1053517-318C-4EC5-B223-7161442ACA6F}" name="LangSmith Traces" dataDxfId="18" dataCellStyle="Hyperlink"/>
-    <tableColumn id="7" xr3:uid="{67E2112F-399B-47A4-AB16-E0E342B8B15C}" name="Comments" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{5E217325-9314-4066-9478-85ED196C3B0A}" name="Query ID" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{97EF1974-2076-449A-A0D4-15EA85F8280F}" name="Agent Type" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{8D1D516B-C100-437C-94C9-405B27E99C54}" name="Outcome" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{62F2D408-C3F9-4A29-8859-C68FE5808C7B}" name="Duration [s]" dataDxfId="31"/>
+    <tableColumn id="8" xr3:uid="{E204E73A-EDA9-4F27-8D7B-6E638A0FF18B}" name="Tokens" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{D7F4AA3D-7E52-4896-B7EA-B50F31C8EB43}" name="Cost [$]" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{A1053517-318C-4EC5-B223-7161442ACA6F}" name="LangSmith Traces" dataDxfId="28" dataCellStyle="Hyperlink"/>
+    <tableColumn id="7" xr3:uid="{67E2112F-399B-47A4-AB16-E0E342B8B15C}" name="Comments" dataDxfId="27"/>
     <tableColumn id="10" xr3:uid="{63EE7C62-A488-4C94-A292-957054A783BD}" name="Model"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{78FA15C9-D8E3-4683-98B8-69E5AAB2BDFB}" name="Table2" displayName="Table2" ref="A1:E13" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{78FA15C9-D8E3-4683-98B8-69E5AAB2BDFB}" name="Table2" displayName="Table2" ref="A1:E13" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25">
   <autoFilter ref="A1:E13" xr:uid="{78FA15C9-D8E3-4683-98B8-69E5AAB2BDFB}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E13">
     <sortCondition ref="A2:A13"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{DF94BDDE-72C2-4E46-ACD5-0E5A636ABE68}" name="Query ID" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{D36448D7-13F4-4A67-88D5-39F0C9732E25}" name="Query" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{88EFB23F-53BA-48C7-8DB1-E4BFB7F240EE}" name="Correct Response" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{568271BE-C334-41D7-BECB-CE936A642BD1}" name="Steps" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{13F83F64-A4E0-456B-9916-E486752D5330}" name="Difficulty" dataDxfId="9"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{196D0887-5250-43FF-A287-28CA4A8E592F}" name="Table1" displayName="Table1" ref="A1:D7" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:D7" xr:uid="{196D0887-5250-43FF-A287-28CA4A8E592F}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BB7680CC-D6B4-4A54-8010-3749DEE3CBE6}" name="Query ID" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{D915BF0A-EE69-4AF7-9164-9E88C8FDBE7E}" name="Level" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{5274E49A-ABB1-4FBE-A864-8E07DAA5C8A9}" name="Type" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{80F6FFEF-7E46-4686-BA17-BB3CBD130F08}" name="Formulation" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{DF94BDDE-72C2-4E46-ACD5-0E5A636ABE68}" name="Query ID" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{D36448D7-13F4-4A67-88D5-39F0C9732E25}" name="Query" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{88EFB23F-53BA-48C7-8DB1-E4BFB7F240EE}" name="Correct Response" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{568271BE-C334-41D7-BECB-CE936A642BD1}" name="Steps" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{13F83F64-A4E0-456B-9916-E486752D5330}" name="Difficulty" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{196D0887-5250-43FF-A287-28CA4A8E592F}" name="Table1" displayName="Table1" ref="A1:D7" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A1:D7" xr:uid="{196D0887-5250-43FF-A287-28CA4A8E592F}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{BB7680CC-D6B4-4A54-8010-3749DEE3CBE6}" name="Query ID" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{D915BF0A-EE69-4AF7-9164-9E88C8FDBE7E}" name="Level" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{5274E49A-ABB1-4FBE-A864-8E07DAA5C8A9}" name="Type" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{80F6FFEF-7E46-4686-BA17-BB3CBD130F08}" name="Formulation" dataDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6FDFBCD9-DEE7-43F6-B225-8DEF2DE803FD}" name="Table4" displayName="Table4" ref="A1:I19" totalsRowShown="0">
   <autoFilter ref="A1:I19" xr:uid="{6FDFBCD9-DEE7-43F6-B225-8DEF2DE803FD}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{D03B1644-1C7C-4FCE-9DB9-747262C3C960}" name="Query ID" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{D03B1644-1C7C-4FCE-9DB9-747262C3C960}" name="Query ID" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{D379A25A-D035-498B-B8CF-AD0E2A81496B}" name="Agent Type"/>
     <tableColumn id="3" xr3:uid="{E57A08B9-2E85-4F54-8E95-AB8F5DD74EF8}" name="Outcome"/>
     <tableColumn id="4" xr3:uid="{6E678DF2-F0CD-40A6-AEDB-CC2E158D34C7}" name="Duration [s]"/>
     <tableColumn id="5" xr3:uid="{E7E60375-F0D0-4F78-98DC-842559FEA71B}" name="Tokens"/>
-    <tableColumn id="6" xr3:uid="{6A2B8CFD-216F-42A3-AD46-D5BDE92AE5B4}" name="Cost [$]" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{6A2B8CFD-216F-42A3-AD46-D5BDE92AE5B4}" name="Cost [$]" dataDxfId="11"/>
     <tableColumn id="7" xr3:uid="{E12EEE88-959B-4D71-A927-9789CECC1F97}" name="LangSmith Traces"/>
     <tableColumn id="8" xr3:uid="{42C9F38F-B4D9-45B5-BB31-A67F037C65AA}" name="Comments"/>
-    <tableColumn id="9" xr3:uid="{659C8448-0B70-40B5-AA26-7C10544D76F8}" name="Model" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{659C8448-0B70-40B5-AA26-7C10544D76F8}" name="Model" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1714,25 +1922,3194 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I109"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43005859-3282-4A92-B97F-C0C604696409}">
+  <dimension ref="A1:J109"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0"/>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="1">
-      <selection activeCell="A47" sqref="A47:A55"/>
+    <sheetView topLeftCell="A72" zoomScale="55" workbookViewId="1">
+      <selection activeCell="G91" sqref="G91"/>
     </sheetView>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="38" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="47.21875" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="82.44140625" customWidth="1"/>
-    <col min="9" max="9" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.6640625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="27.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="57.6">
+      <c r="A2" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="10">
+        <v>87.16</v>
+      </c>
+      <c r="E2" s="10">
+        <v>3347</v>
+      </c>
+      <c r="F2" s="9">
+        <v>3.465E-2</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="I2" t="s">
+        <v>107</v>
+      </c>
+      <c r="J2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="10">
+        <v>97.85</v>
+      </c>
+      <c r="E3" s="10">
+        <v>3042</v>
+      </c>
+      <c r="F3" s="9">
+        <v>3.1019999999999999E-2</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="10">
+        <v>70.36</v>
+      </c>
+      <c r="E4" s="10">
+        <v>4563</v>
+      </c>
+      <c r="F4" s="28">
+        <v>5.0950000000000002E-2</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" t="s">
+        <v>107</v>
+      </c>
+      <c r="J4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="72">
+      <c r="A5" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="10">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="E5" s="10">
+        <v>4736</v>
+      </c>
+      <c r="F5" s="9">
+        <v>5.2220000000000003E-2</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="I5" t="s">
+        <v>107</v>
+      </c>
+      <c r="J5" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="10">
+        <v>49.48</v>
+      </c>
+      <c r="E6" s="10">
+        <v>2192</v>
+      </c>
+      <c r="F6" s="9">
+        <v>2.2259999999999999E-2</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" t="s">
+        <v>107</v>
+      </c>
+      <c r="J6" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="10">
+        <v>76.84</v>
+      </c>
+      <c r="E7" s="10">
+        <v>4270</v>
+      </c>
+      <c r="F7" s="28">
+        <v>4.6179999999999999E-2</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="10">
+        <v>129.03</v>
+      </c>
+      <c r="E8" s="10">
+        <v>4498</v>
+      </c>
+      <c r="F8" s="9">
+        <v>4.5600000000000002E-2</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="57.6">
+      <c r="A9" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="10">
+        <v>114.39</v>
+      </c>
+      <c r="E9" s="10">
+        <v>5269</v>
+      </c>
+      <c r="F9" s="9">
+        <v>5.6070000000000002E-2</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="I9" t="s">
+        <v>107</v>
+      </c>
+      <c r="J9" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1">
+      <c r="A10" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="30">
+        <v>95.83</v>
+      </c>
+      <c r="E10" s="30">
+        <v>5584</v>
+      </c>
+      <c r="F10" s="34">
+        <v>6.164E-2</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="H10" s="29"/>
+      <c r="I10" s="33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="10">
+        <v>93.21</v>
+      </c>
+      <c r="E11" s="10">
+        <v>3047</v>
+      </c>
+      <c r="F11" s="9">
+        <v>3.2629999999999999E-2</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="I11" t="s">
+        <v>107</v>
+      </c>
+      <c r="J11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="43.2">
+      <c r="A12" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="10">
+        <v>134.62</v>
+      </c>
+      <c r="E12" s="10">
+        <v>3713</v>
+      </c>
+      <c r="F12" s="9">
+        <v>3.8510000000000003E-2</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="I12" t="s">
+        <v>107</v>
+      </c>
+      <c r="J12" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="10">
+        <v>253.77</v>
+      </c>
+      <c r="E13" s="10">
+        <v>6956</v>
+      </c>
+      <c r="F13" s="28">
+        <v>6.9680000000000006E-2</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" t="s">
+        <v>107</v>
+      </c>
+      <c r="J13" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="78.599999999999994" customHeight="1">
+      <c r="A14" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="10">
+        <v>66.42</v>
+      </c>
+      <c r="E14" s="10">
+        <v>5421</v>
+      </c>
+      <c r="F14" s="9">
+        <v>5.5550000000000002E-2</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="43.2">
+      <c r="A15" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="10">
+        <v>125.96</v>
+      </c>
+      <c r="E15" s="10">
+        <v>4650</v>
+      </c>
+      <c r="F15" s="9">
+        <v>4.8899999999999999E-2</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="I15" t="s">
+        <v>107</v>
+      </c>
+      <c r="J15" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="10">
+        <v>109.29</v>
+      </c>
+      <c r="E16" s="10">
+        <v>4768</v>
+      </c>
+      <c r="F16" s="28">
+        <v>4.87E-2</v>
+      </c>
+      <c r="G16" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="I16" t="s">
+        <v>107</v>
+      </c>
+      <c r="J16" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="10">
+        <v>65.47</v>
+      </c>
+      <c r="E17" s="10">
+        <v>1909</v>
+      </c>
+      <c r="F17" s="9">
+        <v>2.009E-2</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="I17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="28.8">
+      <c r="A18" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="10">
+        <v>61.22</v>
+      </c>
+      <c r="E18" s="10">
+        <v>2837</v>
+      </c>
+      <c r="F18" s="9">
+        <v>3.4770000000000002E-2</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="I18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickBot="1">
+      <c r="A19" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="30">
+        <v>156</v>
+      </c>
+      <c r="E19" s="30">
+        <v>4485</v>
+      </c>
+      <c r="F19" s="34">
+        <v>5.2049999999999999E-2</v>
+      </c>
+      <c r="G19" s="31" t="s">
+        <v>195</v>
+      </c>
+      <c r="H19" s="29"/>
+      <c r="I19" s="33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="10">
+        <v>78.08</v>
+      </c>
+      <c r="E20" s="10">
+        <v>2389</v>
+      </c>
+      <c r="F20" s="9">
+        <v>2.555E-2</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="10">
+        <v>67.45</v>
+      </c>
+      <c r="E21" s="10">
+        <v>2399</v>
+      </c>
+      <c r="F21" s="9">
+        <v>2.5850000000000001E-2</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="10">
+        <v>20.23</v>
+      </c>
+      <c r="E22" s="10">
+        <v>1471</v>
+      </c>
+      <c r="F22" s="28">
+        <v>1.617E-2</v>
+      </c>
+      <c r="G22" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="I22" t="s">
+        <v>107</v>
+      </c>
+      <c r="J22" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="10">
+        <v>44.33</v>
+      </c>
+      <c r="E23" s="10">
+        <v>2532</v>
+      </c>
+      <c r="F23" s="9">
+        <v>2.682E-2</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="10">
+        <v>30.5</v>
+      </c>
+      <c r="E24" s="10">
+        <v>2355</v>
+      </c>
+      <c r="F24" s="9">
+        <v>2.5049999999999999E-2</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="H24" s="5"/>
+      <c r="I24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="10">
+        <v>31.09</v>
+      </c>
+      <c r="E25" s="10">
+        <v>2355</v>
+      </c>
+      <c r="F25" s="28">
+        <v>2.5049999999999999E-2</v>
+      </c>
+      <c r="G25" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="H25" s="5"/>
+      <c r="I25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="10">
+        <v>18.89</v>
+      </c>
+      <c r="E26" s="10">
+        <v>1149</v>
+      </c>
+      <c r="F26" s="9">
+        <v>1.3350000000000001E-2</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="10">
+        <v>19.739999999999998</v>
+      </c>
+      <c r="E27" s="10">
+        <v>1169</v>
+      </c>
+      <c r="F27" s="9">
+        <v>1.387E-2</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="H27" s="5"/>
+      <c r="I27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="58.2" thickBot="1">
+      <c r="A28" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="30">
+        <v>47.36</v>
+      </c>
+      <c r="E28" s="30">
+        <v>2489</v>
+      </c>
+      <c r="F28" s="34">
+        <v>2.767E-2</v>
+      </c>
+      <c r="G28" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="H28" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="I28" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="J28" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="10">
+        <v>69.73</v>
+      </c>
+      <c r="E29" s="10">
+        <v>2253</v>
+      </c>
+      <c r="F29" s="9">
+        <v>2.2929999999999999E-2</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="10">
+        <v>65.569999999999993</v>
+      </c>
+      <c r="E30" s="10">
+        <v>1945</v>
+      </c>
+      <c r="F30" s="9">
+        <v>1.0619999999999999E-2</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="H30" s="5"/>
+      <c r="I30" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="10">
+        <v>67.37</v>
+      </c>
+      <c r="E31" s="10">
+        <v>2397</v>
+      </c>
+      <c r="F31" s="28">
+        <v>2.443E-2</v>
+      </c>
+      <c r="G31" s="35" t="s">
+        <v>201</v>
+      </c>
+      <c r="H31" s="5"/>
+      <c r="I31" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="10">
+        <v>663.22</v>
+      </c>
+      <c r="E32" s="10">
+        <v>3658</v>
+      </c>
+      <c r="F32" s="9">
+        <v>3.9739999999999998E-2</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="10">
+        <v>295.93</v>
+      </c>
+      <c r="E33" s="10">
+        <v>4388</v>
+      </c>
+      <c r="F33" s="9">
+        <v>4.9779999999999998E-2</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="I33" t="s">
+        <v>107</v>
+      </c>
+      <c r="J33" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="10">
+        <v>285.23</v>
+      </c>
+      <c r="E34" s="10">
+        <v>2281</v>
+      </c>
+      <c r="F34" s="28">
+        <v>2.3009999999999999E-2</v>
+      </c>
+      <c r="G34" s="35" t="s">
+        <v>200</v>
+      </c>
+      <c r="H34" s="5"/>
+      <c r="I34" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="10">
+        <v>36.54</v>
+      </c>
+      <c r="E35" s="10">
+        <v>1231</v>
+      </c>
+      <c r="F35" s="9">
+        <v>1.2529999999999999E-2</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="28.8">
+      <c r="A36" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="10">
+        <v>63.65</v>
+      </c>
+      <c r="E36" s="10">
+        <v>1810</v>
+      </c>
+      <c r="F36" s="9">
+        <v>1.9140000000000001E-2</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="I36" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="15" thickBot="1">
+      <c r="A37" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B37" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="30">
+        <v>22.81</v>
+      </c>
+      <c r="E37" s="30">
+        <v>1079</v>
+      </c>
+      <c r="F37" s="34">
+        <v>1.125E-2</v>
+      </c>
+      <c r="G37" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="H37" s="29"/>
+      <c r="I37" s="33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" s="10">
+        <v>41.82</v>
+      </c>
+      <c r="E38" s="10">
+        <v>1713</v>
+      </c>
+      <c r="F38" s="9">
+        <v>1.7749999999999998E-2</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I38" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="10">
+        <v>71.819999999999993</v>
+      </c>
+      <c r="E39" s="10">
+        <v>2223</v>
+      </c>
+      <c r="F39" s="9">
+        <v>2.283E-2</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="H39" s="5"/>
+      <c r="I39" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="10">
+        <v>47</v>
+      </c>
+      <c r="E40" s="10">
+        <v>1797</v>
+      </c>
+      <c r="F40" s="28">
+        <v>1.831E-2</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="H40" s="5"/>
+      <c r="I40" t="s">
+        <v>107</v>
+      </c>
+      <c r="J40" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="57.6">
+      <c r="A41" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="10">
+        <v>29.37</v>
+      </c>
+      <c r="E41" s="10">
+        <v>2415</v>
+      </c>
+      <c r="F41" s="9">
+        <v>2.4570000000000002E-2</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I41" t="s">
+        <v>95</v>
+      </c>
+      <c r="J41" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="10">
+        <v>41.95</v>
+      </c>
+      <c r="E42" s="10">
+        <v>2810</v>
+      </c>
+      <c r="F42" s="9">
+        <v>3.2480000000000002E-2</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="H42" s="5"/>
+      <c r="I42" t="s">
+        <v>107</v>
+      </c>
+      <c r="J42" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" s="10">
+        <v>40.549999999999997</v>
+      </c>
+      <c r="E43" s="10">
+        <v>2407</v>
+      </c>
+      <c r="F43" s="28">
+        <v>2.6409999999999999E-2</v>
+      </c>
+      <c r="G43" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="H43" s="5"/>
+      <c r="I43" t="s">
+        <v>107</v>
+      </c>
+      <c r="J43" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" s="10">
+        <v>37.520000000000003</v>
+      </c>
+      <c r="E44" s="10">
+        <v>1654</v>
+      </c>
+      <c r="F44" s="9">
+        <v>1.7239999999999998E-2</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" s="10">
+        <v>27.55</v>
+      </c>
+      <c r="E45" s="10">
+        <v>1483</v>
+      </c>
+      <c r="F45" s="9">
+        <v>1.533E-2</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="H45" s="5"/>
+      <c r="I45" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="15" thickBot="1">
+      <c r="A46" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C46" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D46" s="30">
+        <v>41.22</v>
+      </c>
+      <c r="E46" s="30">
+        <v>1765</v>
+      </c>
+      <c r="F46" s="34">
+        <v>1.8610000000000002E-2</v>
+      </c>
+      <c r="G46" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="H46" s="29"/>
+      <c r="I46" s="33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D47" s="10">
+        <v>29.82</v>
+      </c>
+      <c r="E47" s="10">
+        <v>1923</v>
+      </c>
+      <c r="F47" s="9">
+        <v>1.9890000000000001E-2</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D48" s="10">
+        <v>31.73</v>
+      </c>
+      <c r="E48" s="10">
+        <v>1909</v>
+      </c>
+      <c r="F48" s="9">
+        <v>1.9990000000000001E-2</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="H48" s="5"/>
+      <c r="I48" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D49" s="10">
+        <v>31.61</v>
+      </c>
+      <c r="E49" s="10">
+        <v>1922</v>
+      </c>
+      <c r="F49" s="28">
+        <v>2.002E-2</v>
+      </c>
+      <c r="G49" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="H49" s="5"/>
+      <c r="I49" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D50" s="10">
+        <v>35.1</v>
+      </c>
+      <c r="E50" s="10">
+        <v>4510</v>
+      </c>
+      <c r="F50" s="9">
+        <v>4.5560000000000003E-2</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="I50" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D51" s="10">
+        <v>25.36</v>
+      </c>
+      <c r="E51" s="10">
+        <v>3649</v>
+      </c>
+      <c r="F51" s="9">
+        <v>3.705E-2</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="H51" s="5"/>
+      <c r="I51" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D52" s="10">
+        <v>33.35</v>
+      </c>
+      <c r="E52" s="10">
+        <v>3663</v>
+      </c>
+      <c r="F52" s="28">
+        <v>3.739E-2</v>
+      </c>
+      <c r="G52" s="35" t="s">
+        <v>214</v>
+      </c>
+      <c r="H52" s="5"/>
+      <c r="I52" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D53" s="10">
+        <v>34.6</v>
+      </c>
+      <c r="E53" s="10">
+        <v>1495</v>
+      </c>
+      <c r="F53" s="9">
+        <v>1.5509999999999999E-2</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I53" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D54" s="10">
+        <v>63.43</v>
+      </c>
+      <c r="E54" s="10">
+        <v>1519</v>
+      </c>
+      <c r="F54" s="9">
+        <v>1.6029999999999999E-2</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="H54" s="5"/>
+      <c r="I54" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="15" thickBot="1">
+      <c r="A55" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B55" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C55" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D55" s="30">
+        <v>34.770000000000003</v>
+      </c>
+      <c r="E55" s="30">
+        <v>1518</v>
+      </c>
+      <c r="F55" s="34">
+        <v>1.6E-2</v>
+      </c>
+      <c r="G55" s="31" t="s">
+        <v>216</v>
+      </c>
+      <c r="H55" s="29"/>
+      <c r="I55" s="33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D56" s="10">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="E56" s="10">
+        <v>2977</v>
+      </c>
+      <c r="F56" s="9">
+        <v>3.0589999999999999E-2</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I56" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D57" s="10">
+        <v>80.13</v>
+      </c>
+      <c r="E57" s="10">
+        <v>2984</v>
+      </c>
+      <c r="F57" s="9">
+        <v>3.0700000000000002E-2</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="H57" s="3"/>
+      <c r="I57" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D58" s="10">
+        <v>57.66</v>
+      </c>
+      <c r="E58" s="10">
+        <v>2407</v>
+      </c>
+      <c r="F58" s="28">
+        <v>2.503E-2</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="I58" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="43.2">
+      <c r="A59" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D59" s="10">
+        <v>122.99</v>
+      </c>
+      <c r="E59" s="10">
+        <v>3930</v>
+      </c>
+      <c r="F59" s="9">
+        <v>3.9579999999999997E-2</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I59" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D60" s="10">
+        <v>916.13</v>
+      </c>
+      <c r="E60" s="10">
+        <v>2362</v>
+      </c>
+      <c r="F60" s="9">
+        <v>2.4060000000000002E-2</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="H60" s="3"/>
+      <c r="I60" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D61" s="10">
+        <v>911.18</v>
+      </c>
+      <c r="E61" s="10">
+        <v>8385</v>
+      </c>
+      <c r="F61" s="28">
+        <v>9.3390000000000001E-2</v>
+      </c>
+      <c r="G61" s="35" t="s">
+        <v>225</v>
+      </c>
+      <c r="H61" s="5"/>
+      <c r="I61" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="43.2">
+      <c r="A62" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D62" s="10">
+        <v>63.93</v>
+      </c>
+      <c r="E62" s="10">
+        <v>1831</v>
+      </c>
+      <c r="F62" s="9">
+        <v>1.8970000000000001E-2</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="I62" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D63" s="10">
+        <v>77.45</v>
+      </c>
+      <c r="E63" s="10">
+        <v>3086</v>
+      </c>
+      <c r="F63" s="9">
+        <v>3.4759999999999999E-2</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="I63" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="15" thickBot="1">
+      <c r="A64" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B64" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C64" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D64" s="30">
+        <v>64.47</v>
+      </c>
+      <c r="E64" s="30">
+        <v>1640</v>
+      </c>
+      <c r="F64" s="34">
+        <v>1.668E-2</v>
+      </c>
+      <c r="G64" s="31" t="s">
+        <v>220</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="I64" s="33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="86.4">
+      <c r="A65" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D65" s="10">
+        <v>652.88</v>
+      </c>
+      <c r="E65" s="10">
+        <v>9253</v>
+      </c>
+      <c r="F65" s="9">
+        <v>9.425E-2</v>
+      </c>
+      <c r="G65" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="I65" t="s">
+        <v>107</v>
+      </c>
+      <c r="J65" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D66" s="10">
+        <v>102.38</v>
+      </c>
+      <c r="E66" s="10">
+        <v>3360</v>
+      </c>
+      <c r="F66" s="9">
+        <v>3.7699999999999997E-2</v>
+      </c>
+      <c r="G66" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="H66" s="3"/>
+      <c r="I66" t="s">
+        <v>107</v>
+      </c>
+      <c r="J66" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D67" s="10">
+        <v>258.52</v>
+      </c>
+      <c r="E67" s="10">
+        <v>6271</v>
+      </c>
+      <c r="F67" s="28">
+        <v>6.9589999999999999E-2</v>
+      </c>
+      <c r="G67" s="35" t="s">
+        <v>227</v>
+      </c>
+      <c r="H67" s="5"/>
+      <c r="I67" t="s">
+        <v>107</v>
+      </c>
+      <c r="J67" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D68" s="10">
+        <v>118.54</v>
+      </c>
+      <c r="E68" s="10">
+        <v>6683</v>
+      </c>
+      <c r="F68" s="9">
+        <v>6.9169999999999995E-2</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="I68" t="s">
+        <v>107</v>
+      </c>
+      <c r="J68" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="28.8">
+      <c r="A69" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D69" s="10">
+        <v>129.4</v>
+      </c>
+      <c r="E69" s="10">
+        <v>7782</v>
+      </c>
+      <c r="F69" s="9">
+        <v>8.6059999999999998E-2</v>
+      </c>
+      <c r="G69" s="35" t="s">
+        <v>228</v>
+      </c>
+      <c r="H69" s="3"/>
+      <c r="I69" t="s">
+        <v>107</v>
+      </c>
+      <c r="J69" s="37" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D70" s="10">
+        <v>373.37</v>
+      </c>
+      <c r="E70" s="10">
+        <v>10412</v>
+      </c>
+      <c r="F70" s="28">
+        <v>0.11268</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="H70" s="5"/>
+      <c r="I70" t="s">
+        <v>107</v>
+      </c>
+      <c r="J70" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="72">
+      <c r="A71" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D71" s="10">
+        <v>80.489999999999995</v>
+      </c>
+      <c r="E71" s="10">
+        <v>3253</v>
+      </c>
+      <c r="F71" s="9">
+        <v>3.9710000000000002E-2</v>
+      </c>
+      <c r="G71" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I71" t="s">
+        <v>107</v>
+      </c>
+      <c r="J71" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D72" s="10">
+        <v>83.78</v>
+      </c>
+      <c r="E72" s="10">
+        <v>2466</v>
+      </c>
+      <c r="F72" s="9">
+        <v>2.768E-2</v>
+      </c>
+      <c r="G72" s="35" t="s">
+        <v>230</v>
+      </c>
+      <c r="H72" s="3"/>
+      <c r="I72" t="s">
+        <v>107</v>
+      </c>
+      <c r="J72" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="15" thickBot="1">
+      <c r="A73" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="B73" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C73" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D73" s="30">
+        <v>88.63</v>
+      </c>
+      <c r="E73" s="30">
+        <v>2825</v>
+      </c>
+      <c r="F73" s="34">
+        <v>3.739E-2</v>
+      </c>
+      <c r="G73" s="31" t="s">
+        <v>231</v>
+      </c>
+      <c r="H73" s="29"/>
+      <c r="I73" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="J73" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="57.6">
+      <c r="A74" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D74" s="10">
+        <v>119.39</v>
+      </c>
+      <c r="E74" s="10">
+        <v>2373</v>
+      </c>
+      <c r="F74" s="9">
+        <v>2.4670000000000001E-2</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I74" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D75" s="10">
+        <v>114.92</v>
+      </c>
+      <c r="E75" s="10">
+        <v>3033</v>
+      </c>
+      <c r="F75" s="9">
+        <v>3.1530000000000002E-2</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="H75" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="I75" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D76" s="10">
+        <v>121.17</v>
+      </c>
+      <c r="E76" s="10">
+        <v>2621</v>
+      </c>
+      <c r="F76" s="28">
+        <v>2.7230000000000001E-2</v>
+      </c>
+      <c r="G76" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="H76" s="5"/>
+      <c r="I76" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D77" s="10">
+        <v>673.96</v>
+      </c>
+      <c r="E77" s="10">
+        <v>4013</v>
+      </c>
+      <c r="F77" s="9">
+        <v>4.1889999999999997E-2</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H77" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I77" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D78" s="10">
+        <v>2190.08</v>
+      </c>
+      <c r="E78" s="10">
+        <v>3867</v>
+      </c>
+      <c r="F78" s="9">
+        <v>3.9629999999999999E-2</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H78" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="I78" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D79" s="10">
+        <v>2290.09</v>
+      </c>
+      <c r="E79" s="10">
+        <v>3650</v>
+      </c>
+      <c r="F79" s="28">
+        <v>3.7679999999999998E-2</v>
+      </c>
+      <c r="G79" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="H79" s="5"/>
+      <c r="I79" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D80" s="10">
+        <v>168.13</v>
+      </c>
+      <c r="E80" s="10">
+        <v>1944</v>
+      </c>
+      <c r="F80" s="9">
+        <v>2.01E-2</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H80" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I80" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="43.2">
+      <c r="A81" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D81" s="10">
+        <v>94.4</v>
+      </c>
+      <c r="E81" s="10">
+        <v>2536</v>
+      </c>
+      <c r="F81" s="9">
+        <v>2.6360000000000001E-2</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="I81" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="15" thickBot="1">
+      <c r="A82" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B82" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C82" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D82" s="30">
+        <v>136.12</v>
+      </c>
+      <c r="E82" s="30">
+        <v>2511</v>
+      </c>
+      <c r="F82" s="34">
+        <v>2.623E-2</v>
+      </c>
+      <c r="G82" s="31" t="s">
+        <v>238</v>
+      </c>
+      <c r="H82" s="29"/>
+      <c r="I82" s="33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="72">
+      <c r="A83" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D83" s="10">
+        <v>44.44</v>
+      </c>
+      <c r="E83" s="10">
+        <v>1959</v>
+      </c>
+      <c r="F83" s="9">
+        <v>2.0389999999999998E-2</v>
+      </c>
+      <c r="G83" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I83" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D84" s="10">
+        <v>58.61</v>
+      </c>
+      <c r="E84" s="10">
+        <v>1989</v>
+      </c>
+      <c r="F84" s="9">
+        <v>2.1090000000000001E-2</v>
+      </c>
+      <c r="G84" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="H84" s="3"/>
+      <c r="I84" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D85" s="10">
+        <v>35.549999999999997</v>
+      </c>
+      <c r="E85" s="10">
+        <v>1961</v>
+      </c>
+      <c r="F85" s="28">
+        <v>2.0629999999999999E-2</v>
+      </c>
+      <c r="G85" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="H85" s="5"/>
+      <c r="I85" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="43.2">
+      <c r="A86" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D86" s="10">
+        <v>983.76</v>
+      </c>
+      <c r="E86" s="10">
+        <v>3912</v>
+      </c>
+      <c r="F86" s="9">
+        <v>4.0579999999999998E-2</v>
+      </c>
+      <c r="G86" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I86" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="A87" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D87" s="10">
+        <v>757.7</v>
+      </c>
+      <c r="E87" s="10">
+        <v>3819</v>
+      </c>
+      <c r="F87" s="9">
+        <v>3.8929999999999999E-2</v>
+      </c>
+      <c r="G87" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="H87" s="3"/>
+      <c r="I87" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
+      <c r="A88" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D88" s="10">
+        <v>849.06</v>
+      </c>
+      <c r="E88" s="10">
+        <v>3827</v>
+      </c>
+      <c r="F88" s="28">
+        <v>3.9170000000000003E-2</v>
+      </c>
+      <c r="G88" s="35" t="s">
+        <v>255</v>
+      </c>
+      <c r="H88" s="5"/>
+      <c r="I88" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="43.2">
+      <c r="A89" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D89" s="10">
+        <v>59.47</v>
+      </c>
+      <c r="E89" s="10">
+        <v>1571</v>
+      </c>
+      <c r="F89" s="9">
+        <v>1.6449999999999999E-2</v>
+      </c>
+      <c r="G89" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I89" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
+      <c r="A90" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D90" s="10">
+        <v>44.79</v>
+      </c>
+      <c r="E90" s="10">
+        <v>1565</v>
+      </c>
+      <c r="F90" s="9">
+        <v>1.6590000000000001E-2</v>
+      </c>
+      <c r="G90" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="H90" s="3"/>
+      <c r="I90" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="15" thickBot="1">
+      <c r="A91" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B91" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C91" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D91" s="30">
+        <v>41.67</v>
+      </c>
+      <c r="E91" s="30">
+        <v>1548</v>
+      </c>
+      <c r="F91" s="34">
+        <v>1.6119999999999999E-2</v>
+      </c>
+      <c r="G91" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="H91" s="29"/>
+      <c r="I91" s="33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="57.6">
+      <c r="A92" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D92" s="10">
+        <v>56.33</v>
+      </c>
+      <c r="E92" s="10">
+        <v>2001</v>
+      </c>
+      <c r="F92" s="9">
+        <v>2.1149999999999999E-2</v>
+      </c>
+      <c r="G92" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I92" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="28.8">
+      <c r="A93" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D93" s="10">
+        <v>50.38</v>
+      </c>
+      <c r="E93" s="10">
+        <v>3177</v>
+      </c>
+      <c r="F93" s="9">
+        <v>3.4750000000000003E-2</v>
+      </c>
+      <c r="G93" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="H93" s="5"/>
+      <c r="I93" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
+      <c r="A94" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D94" s="10">
+        <v>55.82</v>
+      </c>
+      <c r="E94" s="10">
+        <v>2480</v>
+      </c>
+      <c r="F94" s="28">
+        <v>2.64E-2</v>
+      </c>
+      <c r="G94" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="H94" s="5"/>
+      <c r="I94" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
+      <c r="A95" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D95" s="10">
+        <v>24.08</v>
+      </c>
+      <c r="E95" s="10">
+        <v>1612</v>
+      </c>
+      <c r="F95" s="9">
+        <v>1.772E-2</v>
+      </c>
+      <c r="G95" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H95" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="I95" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
+      <c r="A96" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D96" s="10">
+        <v>33.630000000000003</v>
+      </c>
+      <c r="E96" s="10">
+        <v>2366</v>
+      </c>
+      <c r="F96" s="9">
+        <v>2.6040000000000001E-2</v>
+      </c>
+      <c r="G96" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="H96" s="5"/>
+      <c r="I96" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="A97" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D97" s="10">
+        <v>42.36</v>
+      </c>
+      <c r="E97" s="10">
+        <v>2808</v>
+      </c>
+      <c r="F97" s="28">
+        <v>3.2559999999999999E-2</v>
+      </c>
+      <c r="G97" s="35" t="s">
+        <v>171</v>
+      </c>
+      <c r="H97" s="5"/>
+      <c r="I97" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="A98" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D98" s="10">
+        <v>25.81</v>
+      </c>
+      <c r="E98" s="10">
+        <v>1170</v>
+      </c>
+      <c r="F98" s="9">
+        <v>1.3259999999999999E-2</v>
+      </c>
+      <c r="G98" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H98" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="I98" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D99" s="10">
+        <v>32.590000000000003</v>
+      </c>
+      <c r="E99" s="10">
+        <v>1561</v>
+      </c>
+      <c r="F99" s="9">
+        <v>1.6469999999999999E-2</v>
+      </c>
+      <c r="G99" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="H99" s="5"/>
+      <c r="I99" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" ht="15" thickBot="1">
+      <c r="A100" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B100" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C100" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D100" s="30">
+        <v>20</v>
+      </c>
+      <c r="E100" s="30">
+        <v>1192</v>
+      </c>
+      <c r="F100" s="34">
+        <v>1.384E-2</v>
+      </c>
+      <c r="G100" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="H100" s="29"/>
+      <c r="I100" s="33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D101" s="10">
+        <v>52.24</v>
+      </c>
+      <c r="E101" s="10">
+        <v>2336</v>
+      </c>
+      <c r="F101" s="9">
+        <v>3.3930000000000002E-2</v>
+      </c>
+      <c r="G101" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H101" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I101" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="A102" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D102" s="10">
+        <v>204.07</v>
+      </c>
+      <c r="E102" s="10">
+        <v>5078</v>
+      </c>
+      <c r="F102" s="9">
+        <v>5.5259999999999997E-2</v>
+      </c>
+      <c r="G102" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="H102" s="5"/>
+      <c r="I102" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="A103" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D103" s="10">
+        <v>133.4</v>
+      </c>
+      <c r="E103" s="10">
+        <v>3985</v>
+      </c>
+      <c r="F103" s="28">
+        <v>4.283E-2</v>
+      </c>
+      <c r="G103" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="H103" s="5"/>
+      <c r="I103" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10">
+      <c r="A104" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D104" s="10">
+        <v>68.23</v>
+      </c>
+      <c r="E104" s="10">
+        <v>6099</v>
+      </c>
+      <c r="F104" s="9">
+        <v>6.3450000000000006E-2</v>
+      </c>
+      <c r="G104" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H104" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I104" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10">
+      <c r="A105" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D105" s="10">
+        <v>86.32</v>
+      </c>
+      <c r="E105" s="10">
+        <v>6007</v>
+      </c>
+      <c r="F105" s="9">
+        <v>6.7949999999999997E-2</v>
+      </c>
+      <c r="G105" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H105" s="5"/>
+      <c r="I105" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10">
+      <c r="A106" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D106" s="10">
+        <v>89.98</v>
+      </c>
+      <c r="E106" s="10">
+        <v>6461</v>
+      </c>
+      <c r="F106" s="28">
+        <v>7.3849999999999999E-2</v>
+      </c>
+      <c r="G106" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="H106" s="5"/>
+      <c r="I106" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" ht="43.2">
+      <c r="A107" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D107" s="10">
+        <v>26.49</v>
+      </c>
+      <c r="E107" s="10">
+        <v>1447</v>
+      </c>
+      <c r="F107" s="9">
+        <v>1.553E-2</v>
+      </c>
+      <c r="G107" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H107" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I107" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10">
+      <c r="A108" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D108" s="10">
+        <v>47.59</v>
+      </c>
+      <c r="E108" s="10">
+        <v>1963</v>
+      </c>
+      <c r="F108" s="9">
+        <v>2.1950000000000001E-2</v>
+      </c>
+      <c r="G108" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="H108" s="5"/>
+      <c r="I108" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" ht="15" thickBot="1">
+      <c r="A109" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B109" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C109" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D109" s="30">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="E109" s="30">
+        <v>1555</v>
+      </c>
+      <c r="F109" s="34">
+        <v>1.6729999999999998E-2</v>
+      </c>
+      <c r="G109" s="31" t="s">
+        <v>249</v>
+      </c>
+      <c r="H109" s="29"/>
+      <c r="I109" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="J109" s="33"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I109"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="57" zoomScaleNormal="55" workbookViewId="1">
+      <selection activeCell="D110" sqref="D110"/>
+    </sheetView>
+    <sheetView workbookViewId="2"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="38" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="82.44140625" customWidth="1"/>
+    <col min="9" max="9" width="26.6640625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="27.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1941,25 +5318,23 @@
         <v>27</v>
       </c>
       <c r="D8" s="10">
-        <v>129.03</v>
+        <v>63.51</v>
       </c>
       <c r="E8" s="10">
-        <v>4498</v>
+        <v>2569</v>
       </c>
       <c r="F8" s="9">
-        <v>4.5600000000000002E-2</v>
+        <v>1.064E-2</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>111</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="H8" s="3"/>
       <c r="I8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="57.6">
+    <row r="9" spans="1:9" ht="28.8">
       <c r="A9" s="3" t="s">
         <v>103</v>
       </c>
@@ -1967,28 +5342,26 @@
         <v>30</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D9" s="10">
-        <v>114.39</v>
+        <v>151.46</v>
       </c>
       <c r="E9" s="10">
-        <v>5269</v>
+        <v>6273</v>
       </c>
       <c r="F9" s="9">
-        <v>5.6070000000000002E-2</v>
+        <v>6.5030000000000004E-2</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>192</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="H9" s="3"/>
       <c r="I9" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1">
+    <row r="10" spans="1:9" ht="29.4" thickBot="1">
       <c r="A10" s="32" t="s">
         <v>103</v>
       </c>
@@ -1999,16 +5372,16 @@
         <v>27</v>
       </c>
       <c r="D10" s="30">
-        <v>95.83</v>
+        <v>103.98</v>
       </c>
       <c r="E10" s="30">
-        <v>5584</v>
+        <v>5169</v>
       </c>
       <c r="F10" s="34">
-        <v>6.164E-2</v>
+        <v>5.4109999999999998E-2</v>
       </c>
       <c r="G10" s="31" t="s">
-        <v>168</v>
+        <v>270</v>
       </c>
       <c r="H10" s="29"/>
       <c r="I10" s="33" t="s">
@@ -2100,7 +5473,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="43.2">
+    <row r="14" spans="1:9" ht="78.599999999999994" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>92</v>
       </c>
@@ -2195,28 +5568,26 @@
         <v>30</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="D17" s="10">
-        <v>65.47</v>
+        <v>39.36</v>
       </c>
       <c r="E17" s="10">
-        <v>1909</v>
+        <v>1633</v>
       </c>
       <c r="F17" s="9">
-        <v>2.009E-2</v>
+        <v>1.763E-2</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>97</v>
-      </c>
+        <v>271</v>
+      </c>
+      <c r="H17" s="5"/>
       <c r="I17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="28.8">
+    <row r="18" spans="1:9">
       <c r="A18" s="3" t="s">
         <v>92</v>
       </c>
@@ -2224,23 +5595,21 @@
         <v>30</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="D18" s="10">
-        <v>61.22</v>
+        <v>75.27</v>
       </c>
       <c r="E18" s="10">
-        <v>2837</v>
+        <v>3085</v>
       </c>
       <c r="F18" s="9">
-        <v>3.4770000000000002E-2</v>
+        <v>3.2190000000000003E-2</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>176</v>
-      </c>
+        <v>272</v>
+      </c>
+      <c r="H18" s="3"/>
       <c r="I18" t="s">
         <v>107</v>
       </c>
@@ -2256,16 +5625,16 @@
         <v>27</v>
       </c>
       <c r="D19" s="30">
-        <v>156</v>
+        <v>31.64</v>
       </c>
       <c r="E19" s="30">
-        <v>4485</v>
+        <v>1632</v>
       </c>
       <c r="F19" s="34">
-        <v>5.2049999999999999E-2</v>
+        <v>1.7579999999999998E-2</v>
       </c>
       <c r="G19" s="31" t="s">
-        <v>195</v>
+        <v>273</v>
       </c>
       <c r="H19" s="29"/>
       <c r="I19" s="33" t="s">
@@ -2451,20 +5820,18 @@
         <v>27</v>
       </c>
       <c r="D26" s="10">
-        <v>18.89</v>
+        <v>64.209999999999994</v>
       </c>
       <c r="E26" s="10">
-        <v>1149</v>
+        <v>1874</v>
       </c>
       <c r="F26" s="9">
-        <v>1.3350000000000001E-2</v>
+        <v>2.112E-2</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>69</v>
-      </c>
+        <v>274</v>
+      </c>
+      <c r="H26" s="5"/>
       <c r="I26" t="s">
         <v>95</v>
       </c>
@@ -2480,23 +5847,23 @@
         <v>27</v>
       </c>
       <c r="D27" s="10">
-        <v>19.739999999999998</v>
+        <v>52.28</v>
       </c>
       <c r="E27" s="10">
-        <v>1169</v>
+        <v>1880</v>
       </c>
       <c r="F27" s="9">
-        <v>1.387E-2</v>
+        <v>2.1219999999999999E-2</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>183</v>
+        <v>275</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="58.2" thickBot="1">
+    <row r="28" spans="1:9" ht="15" thickBot="1">
       <c r="A28" s="29" t="s">
         <v>10</v>
       </c>
@@ -2504,23 +5871,21 @@
         <v>30</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D28" s="30">
-        <v>47.36</v>
+        <v>47.62</v>
       </c>
       <c r="E28" s="30">
-        <v>2489</v>
+        <v>1886</v>
       </c>
       <c r="F28" s="34">
-        <v>2.767E-2</v>
+        <v>2.112E-2</v>
       </c>
       <c r="G28" s="31" t="s">
-        <v>185</v>
-      </c>
-      <c r="H28" s="32" t="s">
-        <v>187</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="H28" s="32"/>
       <c r="I28" s="33" t="s">
         <v>107</v>
       </c>
@@ -2704,25 +6069,23 @@
         <v>27</v>
       </c>
       <c r="D35" s="10">
-        <v>36.54</v>
+        <v>102.48</v>
       </c>
       <c r="E35" s="10">
-        <v>1231</v>
+        <v>1828</v>
       </c>
       <c r="F35" s="9">
-        <v>1.2529999999999999E-2</v>
+        <v>1.9779999999999999E-2</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>50</v>
-      </c>
+        <v>277</v>
+      </c>
+      <c r="H35" s="5"/>
       <c r="I35" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="28.8">
+    <row r="36" spans="1:9">
       <c r="A36" s="3" t="s">
         <v>260</v>
       </c>
@@ -2733,20 +6096,18 @@
         <v>27</v>
       </c>
       <c r="D36" s="10">
-        <v>63.65</v>
+        <v>25.01</v>
       </c>
       <c r="E36" s="10">
-        <v>1810</v>
+        <v>1266</v>
       </c>
       <c r="F36" s="9">
-        <v>1.9140000000000001E-2</v>
+        <v>1.592E-2</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>204</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="H36" s="3"/>
       <c r="I36" t="s">
         <v>107</v>
       </c>
@@ -2762,16 +6123,16 @@
         <v>27</v>
       </c>
       <c r="D37" s="30">
-        <v>22.81</v>
+        <v>21.36</v>
       </c>
       <c r="E37" s="30">
-        <v>1079</v>
+        <v>1064</v>
       </c>
       <c r="F37" s="34">
-        <v>1.125E-2</v>
+        <v>1.0880000000000001E-2</v>
       </c>
       <c r="G37" s="31" t="s">
-        <v>203</v>
+        <v>279</v>
       </c>
       <c r="H37" s="29"/>
       <c r="I37" s="33" t="s">
@@ -2955,20 +6316,18 @@
         <v>27</v>
       </c>
       <c r="D44" s="10">
-        <v>37.520000000000003</v>
+        <v>40.08</v>
       </c>
       <c r="E44" s="10">
-        <v>1654</v>
+        <v>1771</v>
       </c>
       <c r="F44" s="9">
-        <v>1.7239999999999998E-2</v>
+        <v>1.8589999999999999E-2</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="H44" s="5" t="s">
-        <v>60</v>
-      </c>
+        <v>280</v>
+      </c>
+      <c r="H44" s="5"/>
       <c r="I44" t="s">
         <v>95</v>
       </c>
@@ -2984,16 +6343,16 @@
         <v>27</v>
       </c>
       <c r="D45" s="10">
-        <v>27.55</v>
+        <v>28.51</v>
       </c>
       <c r="E45" s="10">
-        <v>1483</v>
+        <v>1474</v>
       </c>
       <c r="F45" s="9">
-        <v>1.533E-2</v>
+        <v>1.5219999999999999E-2</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>205</v>
+        <v>281</v>
       </c>
       <c r="H45" s="5"/>
       <c r="I45" t="s">
@@ -3011,16 +6370,16 @@
         <v>27</v>
       </c>
       <c r="D46" s="30">
-        <v>41.22</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="E46" s="30">
-        <v>1765</v>
+        <v>1381</v>
       </c>
       <c r="F46" s="34">
-        <v>1.8610000000000002E-2</v>
+        <v>1.4710000000000001E-2</v>
       </c>
       <c r="G46" s="31" t="s">
-        <v>206</v>
+        <v>282</v>
       </c>
       <c r="H46" s="29"/>
       <c r="I46" s="33" t="s">
@@ -3204,20 +6563,18 @@
         <v>27</v>
       </c>
       <c r="D53" s="10">
-        <v>34.6</v>
+        <v>29.64</v>
       </c>
       <c r="E53" s="10">
-        <v>1495</v>
+        <v>1546</v>
       </c>
       <c r="F53" s="9">
-        <v>1.5509999999999999E-2</v>
+        <v>1.6299999999999999E-2</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="H53" s="5" t="s">
-        <v>74</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="H53" s="5"/>
       <c r="I53" t="s">
         <v>95</v>
       </c>
@@ -3233,16 +6590,16 @@
         <v>27</v>
       </c>
       <c r="D54" s="10">
-        <v>63.43</v>
+        <v>90.61</v>
       </c>
       <c r="E54" s="10">
-        <v>1519</v>
+        <v>1529</v>
       </c>
       <c r="F54" s="9">
-        <v>1.6029999999999999E-2</v>
+        <v>1.617E-2</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>215</v>
+        <v>284</v>
       </c>
       <c r="H54" s="5"/>
       <c r="I54" t="s">
@@ -3260,16 +6617,16 @@
         <v>27</v>
       </c>
       <c r="D55" s="30">
-        <v>34.770000000000003</v>
+        <v>39.39</v>
       </c>
       <c r="E55" s="30">
-        <v>1518</v>
+        <v>1513</v>
       </c>
       <c r="F55" s="34">
-        <v>1.6E-2</v>
+        <v>1.567E-2</v>
       </c>
       <c r="G55" s="31" t="s">
-        <v>216</v>
+        <v>285</v>
       </c>
       <c r="H55" s="29"/>
       <c r="I55" s="33" t="s">
@@ -3444,7 +6801,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="43.2">
+    <row r="62" spans="1:9">
       <c r="A62" s="3" t="s">
         <v>259</v>
       </c>
@@ -3455,20 +6812,18 @@
         <v>42</v>
       </c>
       <c r="D62" s="10">
-        <v>63.93</v>
+        <v>80.41</v>
       </c>
       <c r="E62" s="10">
-        <v>1831</v>
+        <v>1359</v>
       </c>
       <c r="F62" s="9">
-        <v>1.8970000000000001E-2</v>
+        <v>1.387E-2</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="H62" s="3" t="s">
-        <v>218</v>
-      </c>
+        <v>286</v>
+      </c>
+      <c r="H62" s="3"/>
       <c r="I62" t="s">
         <v>95</v>
       </c>
@@ -3484,20 +6839,18 @@
         <v>42</v>
       </c>
       <c r="D63" s="10">
-        <v>77.45</v>
+        <v>67.41</v>
       </c>
       <c r="E63" s="10">
-        <v>3086</v>
+        <v>2626</v>
       </c>
       <c r="F63" s="9">
-        <v>3.4759999999999999E-2</v>
+        <v>3.0960000000000001E-2</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="H63" s="3" t="s">
-        <v>219</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="H63" s="3"/>
       <c r="I63" t="s">
         <v>107</v>
       </c>
@@ -3513,20 +6866,18 @@
         <v>42</v>
       </c>
       <c r="D64" s="30">
-        <v>64.47</v>
+        <v>31.86</v>
       </c>
       <c r="E64" s="30">
-        <v>1640</v>
+        <v>1359</v>
       </c>
       <c r="F64" s="34">
-        <v>1.668E-2</v>
+        <v>1.387E-2</v>
       </c>
       <c r="G64" s="31" t="s">
-        <v>220</v>
-      </c>
-      <c r="H64" s="3" t="s">
-        <v>219</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="H64" s="3"/>
       <c r="I64" s="33" t="s">
         <v>107</v>
       </c>
@@ -3697,7 +7048,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="72">
+    <row r="71" spans="1:9">
       <c r="A71" s="5" t="s">
         <v>120</v>
       </c>
@@ -3708,20 +7059,18 @@
         <v>42</v>
       </c>
       <c r="D71" s="10">
-        <v>80.489999999999995</v>
+        <v>97.79</v>
       </c>
       <c r="E71" s="10">
-        <v>3253</v>
+        <v>2710</v>
       </c>
       <c r="F71" s="9">
-        <v>3.9710000000000002E-2</v>
+        <v>2.8740000000000002E-2</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="H71" s="3" t="s">
-        <v>125</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="H71" s="3"/>
       <c r="I71" t="s">
         <v>107</v>
       </c>
@@ -3737,16 +7086,16 @@
         <v>42</v>
       </c>
       <c r="D72" s="10">
-        <v>83.78</v>
+        <v>73.78</v>
       </c>
       <c r="E72" s="10">
-        <v>2466</v>
+        <v>2575</v>
       </c>
       <c r="F72" s="9">
-        <v>2.768E-2</v>
+        <v>3.0169999999999999E-2</v>
       </c>
       <c r="G72" s="35" t="s">
-        <v>230</v>
+        <v>290</v>
       </c>
       <c r="H72" s="3"/>
       <c r="I72" t="s">
@@ -3764,16 +7113,16 @@
         <v>42</v>
       </c>
       <c r="D73" s="30">
-        <v>88.63</v>
+        <v>127.43</v>
       </c>
       <c r="E73" s="30">
-        <v>2825</v>
+        <v>3318</v>
       </c>
       <c r="F73" s="34">
-        <v>3.739E-2</v>
+        <v>4.1799999999999997E-2</v>
       </c>
       <c r="G73" s="31" t="s">
-        <v>231</v>
+        <v>291</v>
       </c>
       <c r="H73" s="29"/>
       <c r="I73" s="33" t="s">
@@ -3961,25 +7310,23 @@
         <v>27</v>
       </c>
       <c r="D80" s="10">
-        <v>168.13</v>
+        <v>42.49</v>
       </c>
       <c r="E80" s="10">
-        <v>1944</v>
+        <v>1537</v>
       </c>
       <c r="F80" s="9">
-        <v>2.01E-2</v>
+        <v>1.6109999999999999E-2</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H80" s="5" t="s">
-        <v>36</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="H80" s="5"/>
       <c r="I80" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="43.2">
+    <row r="81" spans="1:9">
       <c r="A81" s="5" t="s">
         <v>258</v>
       </c>
@@ -3990,20 +7337,18 @@
         <v>42</v>
       </c>
       <c r="D81" s="10">
-        <v>94.4</v>
+        <v>94.35</v>
       </c>
       <c r="E81" s="10">
-        <v>2536</v>
+        <v>2485</v>
       </c>
       <c r="F81" s="9">
-        <v>2.6360000000000001E-2</v>
+        <v>2.5770000000000001E-2</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="H81" s="3" t="s">
-        <v>239</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="H81" s="3"/>
       <c r="I81" t="s">
         <v>107</v>
       </c>
@@ -4016,19 +7361,19 @@
         <v>30</v>
       </c>
       <c r="C82" s="29" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D82" s="30">
-        <v>136.12</v>
+        <v>52.14</v>
       </c>
       <c r="E82" s="30">
-        <v>2511</v>
+        <v>1790</v>
       </c>
       <c r="F82" s="34">
-        <v>2.623E-2</v>
+        <v>1.8620000000000001E-2</v>
       </c>
       <c r="G82" s="31" t="s">
-        <v>238</v>
+        <v>294</v>
       </c>
       <c r="H82" s="29"/>
       <c r="I82" s="33" t="s">
@@ -4201,7 +7546,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="43.2">
+    <row r="89" spans="1:9">
       <c r="A89" s="3" t="s">
         <v>257</v>
       </c>
@@ -4209,23 +7554,21 @@
         <v>30</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D89" s="10">
-        <v>59.47</v>
+        <v>43.88</v>
       </c>
       <c r="E89" s="10">
-        <v>1571</v>
+        <v>1542</v>
       </c>
       <c r="F89" s="9">
-        <v>1.6449999999999999E-2</v>
+        <v>1.6119999999999999E-2</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="H89" s="3" t="s">
-        <v>88</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="H89" s="3"/>
       <c r="I89" t="s">
         <v>95</v>
       </c>
@@ -4238,19 +7581,19 @@
         <v>30</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D90" s="10">
-        <v>44.79</v>
+        <v>37.26</v>
       </c>
       <c r="E90" s="10">
-        <v>1565</v>
+        <v>1577</v>
       </c>
       <c r="F90" s="9">
-        <v>1.6590000000000001E-2</v>
+        <v>1.6629999999999999E-2</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>250</v>
+        <v>296</v>
       </c>
       <c r="H90" s="3"/>
       <c r="I90" t="s">
@@ -4265,19 +7608,19 @@
         <v>30</v>
       </c>
       <c r="C91" s="29" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D91" s="30">
-        <v>41.67</v>
+        <v>38.380000000000003</v>
       </c>
       <c r="E91" s="30">
-        <v>1548</v>
+        <v>1566</v>
       </c>
       <c r="F91" s="34">
-        <v>1.6119999999999999E-2</v>
+        <v>1.6480000000000002E-2</v>
       </c>
       <c r="G91" s="31" t="s">
-        <v>251</v>
+        <v>297</v>
       </c>
       <c r="H91" s="29"/>
       <c r="I91" s="33" t="s">
@@ -4461,20 +7804,18 @@
         <v>27</v>
       </c>
       <c r="D98" s="10">
-        <v>25.81</v>
+        <v>23.76</v>
       </c>
       <c r="E98" s="10">
-        <v>1170</v>
+        <v>1188</v>
       </c>
       <c r="F98" s="9">
-        <v>1.3259999999999999E-2</v>
+        <v>1.3559999999999999E-2</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="H98" s="5" t="s">
-        <v>114</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="H98" s="5"/>
       <c r="I98" t="s">
         <v>107</v>
       </c>
@@ -4487,19 +7828,19 @@
         <v>30</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D99" s="10">
-        <v>32.590000000000003</v>
+        <v>47.35</v>
       </c>
       <c r="E99" s="10">
-        <v>1561</v>
+        <v>1932</v>
       </c>
       <c r="F99" s="9">
-        <v>1.6469999999999999E-2</v>
+        <v>2.138E-2</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>242</v>
+        <v>299</v>
       </c>
       <c r="H99" s="5"/>
       <c r="I99" t="s">
@@ -4517,16 +7858,16 @@
         <v>27</v>
       </c>
       <c r="D100" s="30">
-        <v>20</v>
+        <v>23.3</v>
       </c>
       <c r="E100" s="30">
-        <v>1192</v>
+        <v>1182</v>
       </c>
       <c r="F100" s="34">
-        <v>1.384E-2</v>
+        <v>1.354E-2</v>
       </c>
       <c r="G100" s="31" t="s">
-        <v>173</v>
+        <v>300</v>
       </c>
       <c r="H100" s="29"/>
       <c r="I100" s="33" t="s">
@@ -4699,7 +8040,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="43.2">
+    <row r="107" spans="1:9">
       <c r="A107" s="5" t="s">
         <v>25</v>
       </c>
@@ -4710,20 +8051,18 @@
         <v>40</v>
       </c>
       <c r="D107" s="10">
-        <v>26.49</v>
+        <v>34.58</v>
       </c>
       <c r="E107" s="10">
-        <v>1447</v>
+        <v>1553</v>
       </c>
       <c r="F107" s="9">
-        <v>1.553E-2</v>
+        <v>1.651E-2</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H107" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>301</v>
+      </c>
+      <c r="H107" s="3"/>
       <c r="I107" t="s">
         <v>95</v>
       </c>
@@ -4739,16 +8078,16 @@
         <v>27</v>
       </c>
       <c r="D108" s="10">
-        <v>47.59</v>
+        <v>34.72</v>
       </c>
       <c r="E108" s="10">
-        <v>1963</v>
+        <v>1540</v>
       </c>
       <c r="F108" s="9">
-        <v>2.1950000000000001E-2</v>
+        <v>1.6379999999999999E-2</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>248</v>
+        <v>302</v>
       </c>
       <c r="H108" s="5"/>
       <c r="I108" t="s">
@@ -4766,16 +8105,16 @@
         <v>40</v>
       </c>
       <c r="D109" s="30">
-        <v>36.200000000000003</v>
+        <v>37.36</v>
       </c>
       <c r="E109" s="30">
-        <v>1555</v>
+        <v>1543</v>
       </c>
       <c r="F109" s="34">
-        <v>1.6729999999999998E-2</v>
+        <v>1.6389999999999998E-2</v>
       </c>
       <c r="G109" s="31" t="s">
-        <v>249</v>
+        <v>303</v>
       </c>
       <c r="H109" s="29"/>
       <c r="I109" s="33" t="s">
@@ -4791,13 +8130,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3BFF00C-9B20-4D57-A0F3-3732FF3EA698}">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A54" zoomScale="57" zoomScaleNormal="57" workbookViewId="0"/>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="65" workbookViewId="2">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5043,14 +8385,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CACDBB6-EC7B-48C7-A660-9515B930A1AA}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
@@ -5175,20 +8518,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E478D2DA-2B8C-45DE-9406-9F4B224C2A25}">
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
     <sheetView zoomScale="82" workbookViewId="1">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>

</xml_diff>

<commit_message>
Add datasets and results to appendix
</commit_message>
<xml_diff>
--- a/documents/QnA_OSM.xlsx
+++ b/documents/QnA_OSM.xlsx
@@ -8,11 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dev\masters-thesis\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED81073-48CC-4F12-98F6-B09C27A2383F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9608783E-420E-4E2D-8747-01E392052CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1512" yWindow="1272" windowWidth="21624" windowHeight="11784" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="16305" activeTab="1" xr2:uid="{A399FF6A-B9DA-4C49-8017-E0DA3374A652}"/>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="16305" activeTab="2" xr2:uid="{6C98443E-C637-4C57-82B4-E28D057BD50C}"/>
+    <workbookView xWindow="32805" yWindow="4005" windowWidth="21600" windowHeight="11775" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="16305" firstSheet="1" activeTab="4" xr2:uid="{A399FF6A-B9DA-4C49-8017-E0DA3374A652}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9420" activeTab="2" xr2:uid="{6C98443E-C637-4C57-82B4-E28D057BD50C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="3" xr2:uid="{A1106171-8E2E-4F31-9944-D203DA9C4581}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests_old" sheetId="5" r:id="rId1"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="295">
   <si>
     <t>Query</t>
   </si>
@@ -481,31 +482,10 @@
     <t>expert</t>
   </si>
   <si>
-    <t>oslo_bergen_geodesic_novice</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>Please plot the shortest flight path on a map between Oslo and Bergen's airports.</t>
   </si>
   <si>
-    <t>normal</t>
-  </si>
-  <si>
-    <t>step-by-step</t>
-  </si>
-  <si>
     <t>Could you count how many trees there are on Munkegata street in Trondheim?</t>
-  </si>
-  <si>
-    <t>oslo_bergen_geodesic_expert_sbs</t>
-  </si>
-  <si>
-    <t>munkegata_trees_count_novice</t>
-  </si>
-  <si>
-    <t>munkegata_trees_count_expert_sbs</t>
   </si>
   <si>
     <t xml:space="preserve">sql </t>
@@ -534,12 +514,6 @@
 a8af379b-bb7f-4564-a30b-64f528812c54</t>
   </si>
   <si>
-    <t>oslo_roads_maxspeed_gte_70_kmh_novice</t>
-  </si>
-  <si>
-    <t>oslo_roads_maxspeed_gte_70_kmh_expert_sbs</t>
-  </si>
-  <si>
     <t>1. Retrieve an outline of Oslo. 
 2. Calculate max/min lat/lon values for this bounding box, and use it to retrieve a subset of the road data. 
 3. Select road segments within the outline from step 1 that have a max speed &gt;= 70.  
@@ -1029,9 +1003,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -1160,7 +1133,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1199,12 +1172,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1227,70 +1195,13 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="35">
     <dxf>
       <font>
         <b val="0"/>
@@ -1330,9 +1241,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -1387,20 +1295,6 @@
         <scheme val="major"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1554,6 +1448,62 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1568,21 +1518,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3E5ADE26-EEAE-43F3-9F4A-1D074CA261C5}" name="Table36" displayName="Table36" ref="A1:J109" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3E5ADE26-EEAE-43F3-9F4A-1D074CA261C5}" name="Table36" displayName="Table36" ref="A1:J109" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33">
   <autoFilter ref="A1:J109" xr:uid="{83D2B9CE-16C8-4DB7-89A3-592E6CC65025}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I109">
     <sortCondition ref="A2:A109"/>
     <sortCondition ref="B2:B109"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{92ED4BCE-FC72-4BFE-B7BF-146AC02E260B}" name="Query ID" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{687659E0-450C-44F9-9EBB-F73732669236}" name="Agent Type" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{1B2851B1-FA93-497C-A3AF-ADF0566FA121}" name="Outcome" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{F3425F5C-8B3A-4FB0-AF42-9FA30792500E}" name="Duration [s]" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{ADAF3E28-BF66-4E9F-A5B0-89C2D442F947}" name="Tokens" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{4150BE77-C1BD-4843-8320-29AF7C00CAFA}" name="Cost [$]" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{29F88C50-3EAB-42D3-8A58-97FFA9D22E1B}" name="LangSmith Traces" dataDxfId="1" dataCellStyle="Hyperlink"/>
-    <tableColumn id="7" xr3:uid="{37F682B6-D553-4DEC-AB91-F0B11BFCD6D1}" name="Comments" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{92ED4BCE-FC72-4BFE-B7BF-146AC02E260B}" name="Query ID" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{687659E0-450C-44F9-9EBB-F73732669236}" name="Agent Type" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{1B2851B1-FA93-497C-A3AF-ADF0566FA121}" name="Outcome" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{F3425F5C-8B3A-4FB0-AF42-9FA30792500E}" name="Duration [s]" dataDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{ADAF3E28-BF66-4E9F-A5B0-89C2D442F947}" name="Tokens" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{4150BE77-C1BD-4843-8320-29AF7C00CAFA}" name="Cost [$]" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{29F88C50-3EAB-42D3-8A58-97FFA9D22E1B}" name="LangSmith Traces" dataDxfId="26" dataCellStyle="Hyperlink"/>
+    <tableColumn id="7" xr3:uid="{37F682B6-D553-4DEC-AB91-F0B11BFCD6D1}" name="Comments" dataDxfId="25"/>
     <tableColumn id="10" xr3:uid="{AB696860-67D7-40BF-BB26-CF7D9306BA69}" name="Model"/>
     <tableColumn id="9" xr3:uid="{792B33F4-3427-4629-839C-3B17F1DA17CA}" name="Reason for Failure"/>
   </tableColumns>
@@ -1591,21 +1541,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{83D2B9CE-16C8-4DB7-89A3-592E6CC65025}" name="Table3" displayName="Table3" ref="A1:I109" totalsRowShown="0" headerRowDxfId="36" headerRowBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{83D2B9CE-16C8-4DB7-89A3-592E6CC65025}" name="Table3" displayName="Table3" ref="A1:I109" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23">
   <autoFilter ref="A1:I109" xr:uid="{83D2B9CE-16C8-4DB7-89A3-592E6CC65025}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I109">
     <sortCondition ref="A2:A109"/>
     <sortCondition ref="B2:B109"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5E217325-9314-4066-9478-85ED196C3B0A}" name="Query ID" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{97EF1974-2076-449A-A0D4-15EA85F8280F}" name="Agent Type" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{8D1D516B-C100-437C-94C9-405B27E99C54}" name="Outcome" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{62F2D408-C3F9-4A29-8859-C68FE5808C7B}" name="Duration [s]" dataDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{E204E73A-EDA9-4F27-8D7B-6E638A0FF18B}" name="Tokens" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{D7F4AA3D-7E52-4896-B7EA-B50F31C8EB43}" name="Cost [$]" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{A1053517-318C-4EC5-B223-7161442ACA6F}" name="LangSmith Traces" dataDxfId="28" dataCellStyle="Hyperlink"/>
-    <tableColumn id="7" xr3:uid="{67E2112F-399B-47A4-AB16-E0E342B8B15C}" name="Comments" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{5E217325-9314-4066-9478-85ED196C3B0A}" name="Query ID" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{97EF1974-2076-449A-A0D4-15EA85F8280F}" name="Agent Type" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{8D1D516B-C100-437C-94C9-405B27E99C54}" name="Outcome" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{62F2D408-C3F9-4A29-8859-C68FE5808C7B}" name="Duration [s]" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{E204E73A-EDA9-4F27-8D7B-6E638A0FF18B}" name="Tokens" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{D7F4AA3D-7E52-4896-B7EA-B50F31C8EB43}" name="Cost [$]" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{A1053517-318C-4EC5-B223-7161442ACA6F}" name="LangSmith Traces" dataDxfId="16" dataCellStyle="Hyperlink"/>
+    <tableColumn id="7" xr3:uid="{67E2112F-399B-47A4-AB16-E0E342B8B15C}" name="Comments" dataDxfId="15"/>
     <tableColumn id="10" xr3:uid="{63EE7C62-A488-4C94-A292-957054A783BD}" name="Model"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1613,48 +1563,44 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{78FA15C9-D8E3-4683-98B8-69E5AAB2BDFB}" name="Table2" displayName="Table2" ref="A1:E13" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{78FA15C9-D8E3-4683-98B8-69E5AAB2BDFB}" name="Table2" displayName="Table2" ref="A1:E13" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13">
   <autoFilter ref="A1:E13" xr:uid="{78FA15C9-D8E3-4683-98B8-69E5AAB2BDFB}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E13">
     <sortCondition ref="A2:A13"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{DF94BDDE-72C2-4E46-ACD5-0E5A636ABE68}" name="Query ID" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{D36448D7-13F4-4A67-88D5-39F0C9732E25}" name="Query" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{88EFB23F-53BA-48C7-8DB1-E4BFB7F240EE}" name="Correct Response" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{568271BE-C334-41D7-BECB-CE936A642BD1}" name="Steps" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{13F83F64-A4E0-456B-9916-E486752D5330}" name="Difficulty" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{DF94BDDE-72C2-4E46-ACD5-0E5A636ABE68}" name="Query ID" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{D36448D7-13F4-4A67-88D5-39F0C9732E25}" name="Query" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{88EFB23F-53BA-48C7-8DB1-E4BFB7F240EE}" name="Correct Response" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{568271BE-C334-41D7-BECB-CE936A642BD1}" name="Steps" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{13F83F64-A4E0-456B-9916-E486752D5330}" name="Difficulty" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{196D0887-5250-43FF-A287-28CA4A8E592F}" name="Table1" displayName="Table1" ref="A1:D7" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A1:D7" xr:uid="{196D0887-5250-43FF-A287-28CA4A8E592F}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BB7680CC-D6B4-4A54-8010-3749DEE3CBE6}" name="Query ID" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{D915BF0A-EE69-4AF7-9164-9E88C8FDBE7E}" name="Level" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{5274E49A-ABB1-4FBE-A864-8E07DAA5C8A9}" name="Type" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{80F6FFEF-7E46-4686-BA17-BB3CBD130F08}" name="Formulation" dataDxfId="13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{196D0887-5250-43FF-A287-28CA4A8E592F}" name="Table1" displayName="Table1" ref="A1:C7" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:C7" xr:uid="{196D0887-5250-43FF-A287-28CA4A8E592F}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{BB7680CC-D6B4-4A54-8010-3749DEE3CBE6}" name="Query ID" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{D915BF0A-EE69-4AF7-9164-9E88C8FDBE7E}" name="Level" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{80F6FFEF-7E46-4686-BA17-BB3CBD130F08}" name="Formulation" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6FDFBCD9-DEE7-43F6-B225-8DEF2DE803FD}" name="Table4" displayName="Table4" ref="A1:I19" totalsRowShown="0">
-  <autoFilter ref="A1:I19" xr:uid="{6FDFBCD9-DEE7-43F6-B225-8DEF2DE803FD}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{D03B1644-1C7C-4FCE-9DB9-747262C3C960}" name="Query ID" dataDxfId="12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6FDFBCD9-DEE7-43F6-B225-8DEF2DE803FD}" name="Table4" displayName="Table4" ref="A1:F19" totalsRowShown="0">
+  <autoFilter ref="A1:F19" xr:uid="{6FDFBCD9-DEE7-43F6-B225-8DEF2DE803FD}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{D03B1644-1C7C-4FCE-9DB9-747262C3C960}" name="Query ID" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{D379A25A-D035-498B-B8CF-AD0E2A81496B}" name="Agent Type"/>
+    <tableColumn id="4" xr3:uid="{0B06EB9C-79F7-4FB3-8AFB-77EAA09977B9}" name="Level"/>
     <tableColumn id="3" xr3:uid="{E57A08B9-2E85-4F54-8E95-AB8F5DD74EF8}" name="Outcome"/>
-    <tableColumn id="4" xr3:uid="{6E678DF2-F0CD-40A6-AEDB-CC2E158D34C7}" name="Duration [s]"/>
-    <tableColumn id="5" xr3:uid="{E7E60375-F0D0-4F78-98DC-842559FEA71B}" name="Tokens"/>
-    <tableColumn id="6" xr3:uid="{6A2B8CFD-216F-42A3-AD46-D5BDE92AE5B4}" name="Cost [$]" dataDxfId="11"/>
     <tableColumn id="7" xr3:uid="{E12EEE88-959B-4D71-A927-9789CECC1F97}" name="LangSmith Traces"/>
-    <tableColumn id="8" xr3:uid="{42C9F38F-B4D9-45B5-BB31-A67F037C65AA}" name="Comments"/>
-    <tableColumn id="9" xr3:uid="{659C8448-0B70-40B5-AA26-7C10544D76F8}" name="Model" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{659C8448-0B70-40B5-AA26-7C10544D76F8}" name="Model" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1930,6 +1876,7 @@
       <selection activeCell="G91" sqref="G91"/>
     </sheetView>
     <sheetView workbookViewId="2"/>
+    <sheetView workbookViewId="3"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -1973,8 +1920,8 @@
       <c r="I1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="36" t="s">
-        <v>263</v>
+      <c r="J1" s="11" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="57.6">
@@ -2006,7 +1953,7 @@
         <v>107</v>
       </c>
       <c r="J2" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2029,14 +1976,14 @@
         <v>3.1019999999999999E-2</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" t="s">
         <v>107</v>
       </c>
       <c r="J3" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2055,18 +2002,18 @@
       <c r="E4" s="10">
         <v>4563</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="25">
         <v>5.0950000000000002E-2</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" t="s">
         <v>107</v>
       </c>
       <c r="J4" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="72">
@@ -2098,7 +2045,7 @@
         <v>107</v>
       </c>
       <c r="J5" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -2121,14 +2068,14 @@
         <v>2.2259999999999999E-2</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" t="s">
         <v>107</v>
       </c>
       <c r="J6" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2147,18 +2094,18 @@
       <c r="E7" s="10">
         <v>4270</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="25">
         <v>4.6179999999999999E-2</v>
       </c>
-      <c r="G7" s="35" t="s">
-        <v>169</v>
+      <c r="G7" s="32" t="s">
+        <v>160</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" t="s">
         <v>107</v>
       </c>
       <c r="J7" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2210,42 +2157,42 @@
         <v>5.6070000000000002E-2</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I9" t="s">
         <v>107</v>
       </c>
       <c r="J9" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="30">
+      <c r="C10" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="27">
         <v>95.83</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="27">
         <v>5584</v>
       </c>
-      <c r="F10" s="34">
+      <c r="F10" s="31">
         <v>6.164E-2</v>
       </c>
-      <c r="G10" s="31" t="s">
-        <v>168</v>
-      </c>
-      <c r="H10" s="29"/>
-      <c r="I10" s="33" t="s">
+      <c r="G10" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="H10" s="26"/>
+      <c r="I10" s="30" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2278,7 +2225,7 @@
         <v>107</v>
       </c>
       <c r="J11" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="43.2">
@@ -2301,16 +2248,16 @@
         <v>3.8510000000000003E-2</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="I12" t="s">
         <v>107</v>
       </c>
       <c r="J12" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -2329,18 +2276,18 @@
       <c r="E13" s="10">
         <v>6956</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="25">
         <v>6.9680000000000006E-2</v>
       </c>
-      <c r="G13" s="35" t="s">
-        <v>194</v>
+      <c r="G13" s="32" t="s">
+        <v>185</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" t="s">
         <v>107</v>
       </c>
       <c r="J13" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="78.599999999999994" customHeight="1">
@@ -2392,16 +2339,16 @@
         <v>4.8899999999999999E-2</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="I15" t="s">
         <v>107</v>
       </c>
       <c r="J15" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -2420,20 +2367,20 @@
       <c r="E16" s="10">
         <v>4768</v>
       </c>
-      <c r="F16" s="28">
+      <c r="F16" s="25">
         <v>4.87E-2</v>
       </c>
-      <c r="G16" s="35" t="s">
-        <v>193</v>
+      <c r="G16" s="32" t="s">
+        <v>184</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="I16" t="s">
         <v>107</v>
       </c>
       <c r="J16" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -2485,39 +2432,39 @@
         <v>3.4770000000000002E-2</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="I18" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="30">
+      <c r="C19" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="27">
         <v>156</v>
       </c>
-      <c r="E19" s="30">
+      <c r="E19" s="27">
         <v>4485</v>
       </c>
-      <c r="F19" s="34">
+      <c r="F19" s="31">
         <v>5.2049999999999999E-2</v>
       </c>
-      <c r="G19" s="31" t="s">
-        <v>195</v>
-      </c>
-      <c r="H19" s="29"/>
-      <c r="I19" s="33" t="s">
+      <c r="G19" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="H19" s="26"/>
+      <c r="I19" s="30" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2570,7 +2517,7 @@
         <v>2.5850000000000001E-2</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" t="s">
@@ -2593,20 +2540,20 @@
       <c r="E22" s="10">
         <v>1471</v>
       </c>
-      <c r="F22" s="28">
+      <c r="F22" s="25">
         <v>1.617E-2</v>
       </c>
-      <c r="G22" s="35" t="s">
-        <v>182</v>
+      <c r="G22" s="32" t="s">
+        <v>173</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="I22" t="s">
         <v>107</v>
       </c>
       <c r="J22" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -2658,7 +2605,7 @@
         <v>2.5049999999999999E-2</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" t="s">
@@ -2681,11 +2628,11 @@
       <c r="E25" s="10">
         <v>2355</v>
       </c>
-      <c r="F25" s="28">
+      <c r="F25" s="25">
         <v>2.5049999999999999E-2</v>
       </c>
-      <c r="G25" s="35" t="s">
-        <v>180</v>
+      <c r="G25" s="32" t="s">
+        <v>171</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" t="s">
@@ -2741,7 +2688,7 @@
         <v>1.387E-2</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" t="s">
@@ -2749,40 +2696,40 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="58.2" thickBot="1">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="30">
+      <c r="D28" s="27">
         <v>47.36</v>
       </c>
-      <c r="E28" s="30">
+      <c r="E28" s="27">
         <v>2489</v>
       </c>
-      <c r="F28" s="34">
+      <c r="F28" s="31">
         <v>2.767E-2</v>
       </c>
-      <c r="G28" s="31" t="s">
-        <v>185</v>
-      </c>
-      <c r="H28" s="32" t="s">
-        <v>187</v>
-      </c>
-      <c r="I28" s="33" t="s">
+      <c r="G28" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="H28" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="I28" s="30" t="s">
         <v>107</v>
       </c>
       <c r="J28" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="3" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>26</v>
@@ -2811,7 +2758,7 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="3" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>26</v>
@@ -2829,7 +2776,7 @@
         <v>1.0619999999999999E-2</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" t="s">
@@ -2838,7 +2785,7 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="3" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>26</v>
@@ -2852,11 +2799,11 @@
       <c r="E31" s="10">
         <v>2397</v>
       </c>
-      <c r="F31" s="28">
+      <c r="F31" s="25">
         <v>2.443E-2</v>
       </c>
-      <c r="G31" s="35" t="s">
-        <v>201</v>
+      <c r="G31" s="32" t="s">
+        <v>192</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" t="s">
@@ -2865,7 +2812,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="3" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>29</v>
@@ -2894,7 +2841,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="3" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>29</v>
@@ -2912,21 +2859,21 @@
         <v>4.9779999999999998E-2</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="I33" t="s">
         <v>107</v>
       </c>
       <c r="J33" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="3" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>29</v>
@@ -2940,11 +2887,11 @@
       <c r="E34" s="10">
         <v>2281</v>
       </c>
-      <c r="F34" s="28">
+      <c r="F34" s="25">
         <v>2.3009999999999999E-2</v>
       </c>
-      <c r="G34" s="35" t="s">
-        <v>200</v>
+      <c r="G34" s="32" t="s">
+        <v>191</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" t="s">
@@ -2953,7 +2900,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="3" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>30</v>
@@ -2982,7 +2929,7 @@
     </row>
     <row r="36" spans="1:10" ht="28.8">
       <c r="A36" s="3" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>30</v>
@@ -3000,10 +2947,10 @@
         <v>1.9140000000000001E-2</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="I36" t="s">
         <v>107</v>
@@ -3011,28 +2958,28 @@
     </row>
     <row r="37" spans="1:10" ht="15" thickBot="1">
       <c r="A37" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="B37" s="29" t="s">
+        <v>251</v>
+      </c>
+      <c r="B37" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C37" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D37" s="30">
+      <c r="C37" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="27">
         <v>22.81</v>
       </c>
-      <c r="E37" s="30">
+      <c r="E37" s="27">
         <v>1079</v>
       </c>
-      <c r="F37" s="34">
+      <c r="F37" s="31">
         <v>1.125E-2</v>
       </c>
-      <c r="G37" s="31" t="s">
-        <v>203</v>
-      </c>
-      <c r="H37" s="29"/>
-      <c r="I37" s="33" t="s">
+      <c r="G37" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="H37" s="26"/>
+      <c r="I37" s="30" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3085,7 +3032,7 @@
         <v>2.283E-2</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" t="s">
@@ -3108,18 +3055,18 @@
       <c r="E40" s="10">
         <v>1797</v>
       </c>
-      <c r="F40" s="28">
+      <c r="F40" s="25">
         <v>1.831E-2</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" t="s">
         <v>107</v>
       </c>
       <c r="J40" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="57.6">
@@ -3151,7 +3098,7 @@
         <v>95</v>
       </c>
       <c r="J41" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -3174,14 +3121,14 @@
         <v>3.2480000000000002E-2</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="H42" s="5"/>
       <c r="I42" t="s">
         <v>107</v>
       </c>
       <c r="J42" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -3200,18 +3147,18 @@
       <c r="E43" s="10">
         <v>2407</v>
       </c>
-      <c r="F43" s="28">
+      <c r="F43" s="25">
         <v>2.6409999999999999E-2</v>
       </c>
-      <c r="G43" s="35" t="s">
-        <v>208</v>
+      <c r="G43" s="32" t="s">
+        <v>199</v>
       </c>
       <c r="H43" s="5"/>
       <c r="I43" t="s">
         <v>107</v>
       </c>
       <c r="J43" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -3263,7 +3210,7 @@
         <v>1.533E-2</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="H45" s="5"/>
       <c r="I45" t="s">
@@ -3271,35 +3218,35 @@
       </c>
     </row>
     <row r="46" spans="1:10" ht="15" thickBot="1">
-      <c r="A46" s="32" t="s">
+      <c r="A46" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="29" t="s">
+      <c r="B46" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C46" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D46" s="30">
+      <c r="C46" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D46" s="27">
         <v>41.22</v>
       </c>
-      <c r="E46" s="30">
+      <c r="E46" s="27">
         <v>1765</v>
       </c>
-      <c r="F46" s="34">
+      <c r="F46" s="31">
         <v>1.8610000000000002E-2</v>
       </c>
-      <c r="G46" s="31" t="s">
-        <v>206</v>
-      </c>
-      <c r="H46" s="29"/>
-      <c r="I46" s="33" t="s">
+      <c r="G46" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="H46" s="26"/>
+      <c r="I46" s="30" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="5" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>26</v>
@@ -3328,7 +3275,7 @@
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="5" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>26</v>
@@ -3346,7 +3293,7 @@
         <v>1.9990000000000001E-2</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="H48" s="5"/>
       <c r="I48" t="s">
@@ -3355,7 +3302,7 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="5" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>26</v>
@@ -3369,11 +3316,11 @@
       <c r="E49" s="10">
         <v>1922</v>
       </c>
-      <c r="F49" s="28">
+      <c r="F49" s="25">
         <v>2.002E-2</v>
       </c>
-      <c r="G49" s="35" t="s">
-        <v>212</v>
+      <c r="G49" s="32" t="s">
+        <v>203</v>
       </c>
       <c r="H49" s="5"/>
       <c r="I49" t="s">
@@ -3382,7 +3329,7 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="5" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>29</v>
@@ -3411,7 +3358,7 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="5" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>29</v>
@@ -3429,7 +3376,7 @@
         <v>3.705E-2</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="H51" s="5"/>
       <c r="I51" t="s">
@@ -3438,7 +3385,7 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="5" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>29</v>
@@ -3452,11 +3399,11 @@
       <c r="E52" s="10">
         <v>3663</v>
       </c>
-      <c r="F52" s="28">
+      <c r="F52" s="25">
         <v>3.739E-2</v>
       </c>
-      <c r="G52" s="35" t="s">
-        <v>214</v>
+      <c r="G52" s="32" t="s">
+        <v>205</v>
       </c>
       <c r="H52" s="5"/>
       <c r="I52" t="s">
@@ -3465,7 +3412,7 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="5" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>30</v>
@@ -3494,7 +3441,7 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="5" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>30</v>
@@ -3512,7 +3459,7 @@
         <v>1.6029999999999999E-2</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="H54" s="5"/>
       <c r="I54" t="s">
@@ -3521,34 +3468,34 @@
     </row>
     <row r="55" spans="1:9" ht="15" thickBot="1">
       <c r="A55" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="B55" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="B55" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C55" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D55" s="30">
+      <c r="C55" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D55" s="27">
         <v>34.770000000000003</v>
       </c>
-      <c r="E55" s="30">
+      <c r="E55" s="27">
         <v>1518</v>
       </c>
-      <c r="F55" s="34">
+      <c r="F55" s="31">
         <v>1.6E-2</v>
       </c>
-      <c r="G55" s="31" t="s">
-        <v>216</v>
-      </c>
-      <c r="H55" s="29"/>
-      <c r="I55" s="33" t="s">
+      <c r="G55" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="H55" s="26"/>
+      <c r="I55" s="30" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="3" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>26</v>
@@ -3577,7 +3524,7 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="3" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>26</v>
@@ -3595,7 +3542,7 @@
         <v>3.0700000000000002E-2</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="H57" s="3"/>
       <c r="I57" t="s">
@@ -3604,7 +3551,7 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="3" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>26</v>
@@ -3618,14 +3565,14 @@
       <c r="E58" s="10">
         <v>2407</v>
       </c>
-      <c r="F58" s="28">
+      <c r="F58" s="25">
         <v>2.503E-2</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="I58" t="s">
         <v>107</v>
@@ -3633,7 +3580,7 @@
     </row>
     <row r="59" spans="1:9" ht="43.2">
       <c r="A59" s="3" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>29</v>
@@ -3662,7 +3609,7 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="3" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>29</v>
@@ -3680,7 +3627,7 @@
         <v>2.4060000000000002E-2</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="H60" s="3"/>
       <c r="I60" t="s">
@@ -3689,7 +3636,7 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="3" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>29</v>
@@ -3703,11 +3650,11 @@
       <c r="E61" s="10">
         <v>8385</v>
       </c>
-      <c r="F61" s="28">
+      <c r="F61" s="25">
         <v>9.3390000000000001E-2</v>
       </c>
-      <c r="G61" s="35" t="s">
-        <v>225</v>
+      <c r="G61" s="32" t="s">
+        <v>216</v>
       </c>
       <c r="H61" s="5"/>
       <c r="I61" t="s">
@@ -3716,7 +3663,7 @@
     </row>
     <row r="62" spans="1:9" ht="43.2">
       <c r="A62" s="3" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>30</v>
@@ -3737,7 +3684,7 @@
         <v>82</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="I62" t="s">
         <v>95</v>
@@ -3745,7 +3692,7 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="3" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>30</v>
@@ -3763,10 +3710,10 @@
         <v>3.4759999999999999E-2</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="I63" t="s">
         <v>107</v>
@@ -3774,30 +3721,30 @@
     </row>
     <row r="64" spans="1:9" ht="15" thickBot="1">
       <c r="A64" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="B64" s="29" t="s">
+        <v>250</v>
+      </c>
+      <c r="B64" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C64" s="29" t="s">
+      <c r="C64" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="D64" s="30">
+      <c r="D64" s="27">
         <v>64.47</v>
       </c>
-      <c r="E64" s="30">
+      <c r="E64" s="27">
         <v>1640</v>
       </c>
-      <c r="F64" s="34">
+      <c r="F64" s="31">
         <v>1.668E-2</v>
       </c>
-      <c r="G64" s="31" t="s">
-        <v>220</v>
+      <c r="G64" s="28" t="s">
+        <v>211</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="I64" s="33" t="s">
+        <v>210</v>
+      </c>
+      <c r="I64" s="30" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3820,7 +3767,7 @@
       <c r="F65" s="9">
         <v>9.425E-2</v>
       </c>
-      <c r="G65" s="35" t="s">
+      <c r="G65" s="32" t="s">
         <v>124</v>
       </c>
       <c r="H65" s="3" t="s">
@@ -3830,7 +3777,7 @@
         <v>107</v>
       </c>
       <c r="J65" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -3852,15 +3799,15 @@
       <c r="F66" s="9">
         <v>3.7699999999999997E-2</v>
       </c>
-      <c r="G66" s="35" t="s">
-        <v>226</v>
+      <c r="G66" s="32" t="s">
+        <v>217</v>
       </c>
       <c r="H66" s="3"/>
       <c r="I66" t="s">
         <v>107</v>
       </c>
       <c r="J66" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -3879,18 +3826,18 @@
       <c r="E67" s="10">
         <v>6271</v>
       </c>
-      <c r="F67" s="28">
+      <c r="F67" s="25">
         <v>6.9589999999999999E-2</v>
       </c>
-      <c r="G67" s="35" t="s">
-        <v>227</v>
+      <c r="G67" s="32" t="s">
+        <v>218</v>
       </c>
       <c r="H67" s="5"/>
       <c r="I67" t="s">
         <v>107</v>
       </c>
       <c r="J67" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -3922,7 +3869,7 @@
         <v>107</v>
       </c>
       <c r="J68" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="28.8">
@@ -3944,15 +3891,15 @@
       <c r="F69" s="9">
         <v>8.6059999999999998E-2</v>
       </c>
-      <c r="G69" s="35" t="s">
-        <v>228</v>
+      <c r="G69" s="32" t="s">
+        <v>219</v>
       </c>
       <c r="H69" s="3"/>
       <c r="I69" t="s">
         <v>107</v>
       </c>
-      <c r="J69" s="37" t="s">
-        <v>266</v>
+      <c r="J69" s="33" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -3971,18 +3918,18 @@
       <c r="E70" s="10">
         <v>10412</v>
       </c>
-      <c r="F70" s="28">
+      <c r="F70" s="25">
         <v>0.11268</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="H70" s="5"/>
       <c r="I70" t="s">
         <v>107</v>
       </c>
       <c r="J70" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="72">
@@ -4014,7 +3961,7 @@
         <v>107</v>
       </c>
       <c r="J71" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -4036,50 +3983,50 @@
       <c r="F72" s="9">
         <v>2.768E-2</v>
       </c>
-      <c r="G72" s="35" t="s">
-        <v>230</v>
+      <c r="G72" s="32" t="s">
+        <v>221</v>
       </c>
       <c r="H72" s="3"/>
       <c r="I72" t="s">
         <v>107</v>
       </c>
       <c r="J72" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="15" thickBot="1">
-      <c r="A73" s="29" t="s">
+      <c r="A73" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="B73" s="29" t="s">
+      <c r="B73" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C73" s="29" t="s">
+      <c r="C73" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="D73" s="30">
+      <c r="D73" s="27">
         <v>88.63</v>
       </c>
-      <c r="E73" s="30">
+      <c r="E73" s="27">
         <v>2825</v>
       </c>
-      <c r="F73" s="34">
+      <c r="F73" s="31">
         <v>3.739E-2</v>
       </c>
-      <c r="G73" s="31" t="s">
-        <v>231</v>
-      </c>
-      <c r="H73" s="29"/>
-      <c r="I73" s="33" t="s">
+      <c r="G73" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="H73" s="26"/>
+      <c r="I73" s="30" t="s">
         <v>107</v>
       </c>
       <c r="J73" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="57.6">
       <c r="A74" s="5" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>26</v>
@@ -4108,7 +4055,7 @@
     </row>
     <row r="75" spans="1:10">
       <c r="A75" s="5" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>26</v>
@@ -4126,10 +4073,10 @@
         <v>3.1530000000000002E-2</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="I75" t="s">
         <v>107</v>
@@ -4137,7 +4084,7 @@
     </row>
     <row r="76" spans="1:10">
       <c r="A76" s="5" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>26</v>
@@ -4151,11 +4098,11 @@
       <c r="E76" s="10">
         <v>2621</v>
       </c>
-      <c r="F76" s="28">
+      <c r="F76" s="25">
         <v>2.7230000000000001E-2</v>
       </c>
-      <c r="G76" s="35" t="s">
-        <v>234</v>
+      <c r="G76" s="32" t="s">
+        <v>225</v>
       </c>
       <c r="H76" s="5"/>
       <c r="I76" t="s">
@@ -4164,7 +4111,7 @@
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="5" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>29</v>
@@ -4193,7 +4140,7 @@
     </row>
     <row r="78" spans="1:10">
       <c r="A78" s="5" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>29</v>
@@ -4211,10 +4158,10 @@
         <v>3.9629999999999999E-2</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="I78" t="s">
         <v>107</v>
@@ -4222,7 +4169,7 @@
     </row>
     <row r="79" spans="1:10">
       <c r="A79" s="5" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>29</v>
@@ -4236,11 +4183,11 @@
       <c r="E79" s="10">
         <v>3650</v>
       </c>
-      <c r="F79" s="28">
+      <c r="F79" s="25">
         <v>3.7679999999999998E-2</v>
       </c>
-      <c r="G79" s="35" t="s">
-        <v>243</v>
+      <c r="G79" s="32" t="s">
+        <v>234</v>
       </c>
       <c r="H79" s="5"/>
       <c r="I79" t="s">
@@ -4249,7 +4196,7 @@
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="5" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>30</v>
@@ -4278,7 +4225,7 @@
     </row>
     <row r="81" spans="1:9" ht="43.2">
       <c r="A81" s="5" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>30</v>
@@ -4296,10 +4243,10 @@
         <v>2.6360000000000001E-2</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="I81" t="s">
         <v>107</v>
@@ -4307,34 +4254,34 @@
     </row>
     <row r="82" spans="1:9" ht="15" thickBot="1">
       <c r="A82" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="B82" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="B82" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C82" s="29" t="s">
+      <c r="C82" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="D82" s="30">
+      <c r="D82" s="27">
         <v>136.12</v>
       </c>
-      <c r="E82" s="30">
+      <c r="E82" s="27">
         <v>2511</v>
       </c>
-      <c r="F82" s="34">
+      <c r="F82" s="31">
         <v>2.623E-2</v>
       </c>
-      <c r="G82" s="31" t="s">
-        <v>238</v>
-      </c>
-      <c r="H82" s="29"/>
-      <c r="I82" s="33" t="s">
+      <c r="G82" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="H82" s="26"/>
+      <c r="I82" s="30" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="72">
       <c r="A83" s="3" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>26</v>
@@ -4363,7 +4310,7 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="3" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B84" s="5" t="s">
         <v>26</v>
@@ -4381,7 +4328,7 @@
         <v>2.1090000000000001E-2</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="H84" s="3"/>
       <c r="I84" t="s">
@@ -4390,7 +4337,7 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" s="3" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>26</v>
@@ -4404,11 +4351,11 @@
       <c r="E85" s="10">
         <v>1961</v>
       </c>
-      <c r="F85" s="28">
+      <c r="F85" s="25">
         <v>2.0629999999999999E-2</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="H85" s="5"/>
       <c r="I85" t="s">
@@ -4417,7 +4364,7 @@
     </row>
     <row r="86" spans="1:9" ht="43.2">
       <c r="A86" s="3" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>29</v>
@@ -4446,7 +4393,7 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" s="3" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>29</v>
@@ -4464,7 +4411,7 @@
         <v>3.8929999999999999E-2</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="H87" s="3"/>
       <c r="I87" t="s">
@@ -4473,7 +4420,7 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" s="3" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B88" s="5" t="s">
         <v>29</v>
@@ -4487,11 +4434,11 @@
       <c r="E88" s="10">
         <v>3827</v>
       </c>
-      <c r="F88" s="28">
+      <c r="F88" s="25">
         <v>3.9170000000000003E-2</v>
       </c>
-      <c r="G88" s="35" t="s">
-        <v>255</v>
+      <c r="G88" s="32" t="s">
+        <v>246</v>
       </c>
       <c r="H88" s="5"/>
       <c r="I88" t="s">
@@ -4500,7 +4447,7 @@
     </row>
     <row r="89" spans="1:9" ht="43.2">
       <c r="A89" s="3" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B89" s="5" t="s">
         <v>30</v>
@@ -4529,7 +4476,7 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="3" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>30</v>
@@ -4547,7 +4494,7 @@
         <v>1.6590000000000001E-2</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="H90" s="3"/>
       <c r="I90" t="s">
@@ -4556,28 +4503,28 @@
     </row>
     <row r="91" spans="1:9" ht="15" thickBot="1">
       <c r="A91" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="B91" s="29" t="s">
+        <v>248</v>
+      </c>
+      <c r="B91" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C91" s="29" t="s">
+      <c r="C91" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="D91" s="30">
+      <c r="D91" s="27">
         <v>41.67</v>
       </c>
-      <c r="E91" s="30">
+      <c r="E91" s="27">
         <v>1548</v>
       </c>
-      <c r="F91" s="34">
+      <c r="F91" s="31">
         <v>1.6119999999999999E-2</v>
       </c>
-      <c r="G91" s="31" t="s">
-        <v>251</v>
-      </c>
-      <c r="H91" s="29"/>
-      <c r="I91" s="33" t="s">
+      <c r="G91" s="28" t="s">
+        <v>242</v>
+      </c>
+      <c r="H91" s="26"/>
+      <c r="I91" s="30" t="s">
         <v>107</v>
       </c>
     </row>
@@ -4630,7 +4577,7 @@
         <v>3.4750000000000003E-2</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="H93" s="5"/>
       <c r="I93" t="s">
@@ -4653,11 +4600,11 @@
       <c r="E94" s="10">
         <v>2480</v>
       </c>
-      <c r="F94" s="28">
+      <c r="F94" s="25">
         <v>2.64E-2</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="H94" s="5"/>
       <c r="I94" t="s">
@@ -4713,7 +4660,7 @@
         <v>2.6040000000000001E-2</v>
       </c>
       <c r="G96" s="6" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="H96" s="5"/>
       <c r="I96" t="s">
@@ -4736,11 +4683,11 @@
       <c r="E97" s="10">
         <v>2808</v>
       </c>
-      <c r="F97" s="28">
+      <c r="F97" s="25">
         <v>3.2559999999999999E-2</v>
       </c>
-      <c r="G97" s="35" t="s">
-        <v>171</v>
+      <c r="G97" s="32" t="s">
+        <v>162</v>
       </c>
       <c r="H97" s="5"/>
       <c r="I97" t="s">
@@ -4796,7 +4743,7 @@
         <v>1.6469999999999999E-2</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="H99" s="5"/>
       <c r="I99" t="s">
@@ -4804,29 +4751,29 @@
       </c>
     </row>
     <row r="100" spans="1:10" ht="15" thickBot="1">
-      <c r="A100" s="32" t="s">
+      <c r="A100" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B100" s="29" t="s">
+      <c r="B100" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C100" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D100" s="30">
+      <c r="C100" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D100" s="27">
         <v>20</v>
       </c>
-      <c r="E100" s="30">
+      <c r="E100" s="27">
         <v>1192</v>
       </c>
-      <c r="F100" s="34">
+      <c r="F100" s="31">
         <v>1.384E-2</v>
       </c>
-      <c r="G100" s="31" t="s">
-        <v>173</v>
-      </c>
-      <c r="H100" s="29"/>
-      <c r="I100" s="33" t="s">
+      <c r="G100" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="H100" s="26"/>
+      <c r="I100" s="30" t="s">
         <v>107</v>
       </c>
     </row>
@@ -4879,7 +4826,7 @@
         <v>5.5259999999999997E-2</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="H102" s="5"/>
       <c r="I102" t="s">
@@ -4902,11 +4849,11 @@
       <c r="E103" s="10">
         <v>3985</v>
       </c>
-      <c r="F103" s="28">
+      <c r="F103" s="25">
         <v>4.283E-2</v>
       </c>
-      <c r="G103" s="35" t="s">
-        <v>247</v>
+      <c r="G103" s="32" t="s">
+        <v>238</v>
       </c>
       <c r="H103" s="5"/>
       <c r="I103" t="s">
@@ -4962,7 +4909,7 @@
         <v>6.7949999999999997E-2</v>
       </c>
       <c r="G105" s="6" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="H105" s="5"/>
       <c r="I105" t="s">
@@ -4985,11 +4932,11 @@
       <c r="E106" s="10">
         <v>6461</v>
       </c>
-      <c r="F106" s="28">
+      <c r="F106" s="25">
         <v>7.3849999999999999E-2</v>
       </c>
-      <c r="G106" s="35" t="s">
-        <v>245</v>
+      <c r="G106" s="32" t="s">
+        <v>236</v>
       </c>
       <c r="H106" s="5"/>
       <c r="I106" t="s">
@@ -5045,7 +4992,7 @@
         <v>2.1950000000000001E-2</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="H108" s="5"/>
       <c r="I108" t="s">
@@ -5053,32 +5000,32 @@
       </c>
     </row>
     <row r="109" spans="1:10" ht="15" thickBot="1">
-      <c r="A109" s="29" t="s">
+      <c r="A109" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B109" s="29" t="s">
+      <c r="B109" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C109" s="29" t="s">
+      <c r="C109" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="D109" s="30">
+      <c r="D109" s="27">
         <v>36.200000000000003</v>
       </c>
-      <c r="E109" s="30">
+      <c r="E109" s="27">
         <v>1555</v>
       </c>
-      <c r="F109" s="34">
+      <c r="F109" s="31">
         <v>1.6729999999999998E-2</v>
       </c>
-      <c r="G109" s="31" t="s">
-        <v>249</v>
-      </c>
-      <c r="H109" s="29"/>
-      <c r="I109" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="J109" s="33"/>
+      <c r="G109" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="H109" s="26"/>
+      <c r="I109" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="J109" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5093,10 +5040,11 @@
   <dimension ref="A1:I109"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0"/>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="57" zoomScaleNormal="55" workbookViewId="1">
+    <sheetView topLeftCell="A65" zoomScale="57" zoomScaleNormal="55" workbookViewId="1">
       <selection activeCell="D110" sqref="D110"/>
     </sheetView>
     <sheetView workbookViewId="2"/>
+    <sheetView workbookViewId="3"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -5190,7 +5138,7 @@
         <v>3.1019999999999999E-2</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" t="s">
@@ -5213,11 +5161,11 @@
       <c r="E4" s="10">
         <v>4563</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="25">
         <v>5.0950000000000002E-2</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" t="s">
@@ -5273,7 +5221,7 @@
         <v>2.2259999999999999E-2</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" t="s">
@@ -5296,11 +5244,11 @@
       <c r="E7" s="10">
         <v>4270</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="25">
         <v>4.6179999999999999E-2</v>
       </c>
-      <c r="G7" s="35" t="s">
-        <v>169</v>
+      <c r="G7" s="32" t="s">
+        <v>160</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" t="s">
@@ -5327,7 +5275,7 @@
         <v>1.064E-2</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" t="s">
@@ -5354,7 +5302,7 @@
         <v>6.5030000000000004E-2</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" t="s">
@@ -5362,29 +5310,29 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="29.4" thickBot="1">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="30">
+      <c r="C10" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="27">
         <v>103.98</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="27">
         <v>5169</v>
       </c>
-      <c r="F10" s="34">
+      <c r="F10" s="31">
         <v>5.4109999999999998E-2</v>
       </c>
-      <c r="G10" s="31" t="s">
-        <v>270</v>
-      </c>
-      <c r="H10" s="29"/>
-      <c r="I10" s="33" t="s">
+      <c r="G10" s="28" t="s">
+        <v>261</v>
+      </c>
+      <c r="H10" s="26"/>
+      <c r="I10" s="30" t="s">
         <v>107</v>
       </c>
     </row>
@@ -5437,10 +5385,10 @@
         <v>3.8510000000000003E-2</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="I12" t="s">
         <v>107</v>
@@ -5462,11 +5410,11 @@
       <c r="E13" s="10">
         <v>6956</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="25">
         <v>6.9680000000000006E-2</v>
       </c>
-      <c r="G13" s="35" t="s">
-        <v>194</v>
+      <c r="G13" s="32" t="s">
+        <v>185</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" t="s">
@@ -5522,10 +5470,10 @@
         <v>4.8899999999999999E-2</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="I15" t="s">
         <v>107</v>
@@ -5547,14 +5495,14 @@
       <c r="E16" s="10">
         <v>4768</v>
       </c>
-      <c r="F16" s="28">
+      <c r="F16" s="25">
         <v>4.87E-2</v>
       </c>
-      <c r="G16" s="35" t="s">
-        <v>193</v>
+      <c r="G16" s="32" t="s">
+        <v>184</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="I16" t="s">
         <v>107</v>
@@ -5580,7 +5528,7 @@
         <v>1.763E-2</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" t="s">
@@ -5607,7 +5555,7 @@
         <v>3.2190000000000003E-2</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" t="s">
@@ -5615,29 +5563,29 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="15" thickBot="1">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="30">
+      <c r="C19" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="27">
         <v>31.64</v>
       </c>
-      <c r="E19" s="30">
+      <c r="E19" s="27">
         <v>1632</v>
       </c>
-      <c r="F19" s="34">
+      <c r="F19" s="31">
         <v>1.7579999999999998E-2</v>
       </c>
-      <c r="G19" s="31" t="s">
-        <v>273</v>
-      </c>
-      <c r="H19" s="29"/>
-      <c r="I19" s="33" t="s">
+      <c r="G19" s="28" t="s">
+        <v>264</v>
+      </c>
+      <c r="H19" s="26"/>
+      <c r="I19" s="30" t="s">
         <v>107</v>
       </c>
     </row>
@@ -5690,7 +5638,7 @@
         <v>2.5850000000000001E-2</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" t="s">
@@ -5713,14 +5661,14 @@
       <c r="E22" s="10">
         <v>1471</v>
       </c>
-      <c r="F22" s="28">
+      <c r="F22" s="25">
         <v>1.617E-2</v>
       </c>
-      <c r="G22" s="35" t="s">
-        <v>182</v>
+      <c r="G22" s="32" t="s">
+        <v>173</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="I22" t="s">
         <v>107</v>
@@ -5775,7 +5723,7 @@
         <v>2.5049999999999999E-2</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" t="s">
@@ -5798,11 +5746,11 @@
       <c r="E25" s="10">
         <v>2355</v>
       </c>
-      <c r="F25" s="28">
+      <c r="F25" s="25">
         <v>2.5049999999999999E-2</v>
       </c>
-      <c r="G25" s="35" t="s">
-        <v>180</v>
+      <c r="G25" s="32" t="s">
+        <v>171</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" t="s">
@@ -5829,7 +5777,7 @@
         <v>2.112E-2</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" t="s">
@@ -5856,7 +5804,7 @@
         <v>2.1219999999999999E-2</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" t="s">
@@ -5864,35 +5812,35 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="15" thickBot="1">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="30">
+      <c r="C28" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="27">
         <v>47.62</v>
       </c>
-      <c r="E28" s="30">
+      <c r="E28" s="27">
         <v>1886</v>
       </c>
-      <c r="F28" s="34">
+      <c r="F28" s="31">
         <v>2.112E-2</v>
       </c>
-      <c r="G28" s="31" t="s">
-        <v>276</v>
-      </c>
-      <c r="H28" s="32"/>
-      <c r="I28" s="33" t="s">
+      <c r="G28" s="28" t="s">
+        <v>267</v>
+      </c>
+      <c r="H28" s="29"/>
+      <c r="I28" s="30" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="3" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>26</v>
@@ -5921,7 +5869,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="3" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>26</v>
@@ -5939,7 +5887,7 @@
         <v>1.0619999999999999E-2</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" t="s">
@@ -5948,7 +5896,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="3" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>26</v>
@@ -5962,11 +5910,11 @@
       <c r="E31" s="10">
         <v>2397</v>
       </c>
-      <c r="F31" s="28">
+      <c r="F31" s="25">
         <v>2.443E-2</v>
       </c>
-      <c r="G31" s="35" t="s">
-        <v>201</v>
+      <c r="G31" s="32" t="s">
+        <v>192</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" t="s">
@@ -5975,7 +5923,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="3" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>29</v>
@@ -6004,7 +5952,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="3" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>29</v>
@@ -6022,10 +5970,10 @@
         <v>4.9779999999999998E-2</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="I33" t="s">
         <v>107</v>
@@ -6033,7 +5981,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="3" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>29</v>
@@ -6047,11 +5995,11 @@
       <c r="E34" s="10">
         <v>2281</v>
       </c>
-      <c r="F34" s="28">
+      <c r="F34" s="25">
         <v>2.3009999999999999E-2</v>
       </c>
-      <c r="G34" s="35" t="s">
-        <v>200</v>
+      <c r="G34" s="32" t="s">
+        <v>191</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" t="s">
@@ -6060,7 +6008,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="3" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>30</v>
@@ -6078,7 +6026,7 @@
         <v>1.9779999999999999E-2</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" t="s">
@@ -6087,7 +6035,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="3" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>30</v>
@@ -6105,7 +6053,7 @@
         <v>1.592E-2</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" t="s">
@@ -6114,28 +6062,28 @@
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1">
       <c r="A37" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="B37" s="29" t="s">
+        <v>251</v>
+      </c>
+      <c r="B37" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C37" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D37" s="30">
+      <c r="C37" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="27">
         <v>21.36</v>
       </c>
-      <c r="E37" s="30">
+      <c r="E37" s="27">
         <v>1064</v>
       </c>
-      <c r="F37" s="34">
+      <c r="F37" s="31">
         <v>1.0880000000000001E-2</v>
       </c>
-      <c r="G37" s="31" t="s">
-        <v>279</v>
-      </c>
-      <c r="H37" s="29"/>
-      <c r="I37" s="33" t="s">
+      <c r="G37" s="28" t="s">
+        <v>270</v>
+      </c>
+      <c r="H37" s="26"/>
+      <c r="I37" s="30" t="s">
         <v>107</v>
       </c>
     </row>
@@ -6188,7 +6136,7 @@
         <v>2.283E-2</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" t="s">
@@ -6211,11 +6159,11 @@
       <c r="E40" s="10">
         <v>1797</v>
       </c>
-      <c r="F40" s="28">
+      <c r="F40" s="25">
         <v>1.831E-2</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" t="s">
@@ -6271,7 +6219,7 @@
         <v>3.2480000000000002E-2</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="H42" s="5"/>
       <c r="I42" t="s">
@@ -6294,11 +6242,11 @@
       <c r="E43" s="10">
         <v>2407</v>
       </c>
-      <c r="F43" s="28">
+      <c r="F43" s="25">
         <v>2.6409999999999999E-2</v>
       </c>
-      <c r="G43" s="35" t="s">
-        <v>208</v>
+      <c r="G43" s="32" t="s">
+        <v>199</v>
       </c>
       <c r="H43" s="5"/>
       <c r="I43" t="s">
@@ -6325,7 +6273,7 @@
         <v>1.8589999999999999E-2</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="H44" s="5"/>
       <c r="I44" t="s">
@@ -6352,7 +6300,7 @@
         <v>1.5219999999999999E-2</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="H45" s="5"/>
       <c r="I45" t="s">
@@ -6360,35 +6308,35 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="15" thickBot="1">
-      <c r="A46" s="32" t="s">
+      <c r="A46" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="29" t="s">
+      <c r="B46" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C46" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D46" s="30">
+      <c r="C46" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D46" s="27">
         <v>38.299999999999997</v>
       </c>
-      <c r="E46" s="30">
+      <c r="E46" s="27">
         <v>1381</v>
       </c>
-      <c r="F46" s="34">
+      <c r="F46" s="31">
         <v>1.4710000000000001E-2</v>
       </c>
-      <c r="G46" s="31" t="s">
-        <v>282</v>
-      </c>
-      <c r="H46" s="29"/>
-      <c r="I46" s="33" t="s">
+      <c r="G46" s="28" t="s">
+        <v>273</v>
+      </c>
+      <c r="H46" s="26"/>
+      <c r="I46" s="30" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="5" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>26</v>
@@ -6417,7 +6365,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="5" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>26</v>
@@ -6435,7 +6383,7 @@
         <v>1.9990000000000001E-2</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="H48" s="5"/>
       <c r="I48" t="s">
@@ -6444,7 +6392,7 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="5" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>26</v>
@@ -6458,11 +6406,11 @@
       <c r="E49" s="10">
         <v>1922</v>
       </c>
-      <c r="F49" s="28">
+      <c r="F49" s="25">
         <v>2.002E-2</v>
       </c>
-      <c r="G49" s="35" t="s">
-        <v>212</v>
+      <c r="G49" s="32" t="s">
+        <v>203</v>
       </c>
       <c r="H49" s="5"/>
       <c r="I49" t="s">
@@ -6471,7 +6419,7 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="5" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>29</v>
@@ -6500,7 +6448,7 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="5" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>29</v>
@@ -6518,7 +6466,7 @@
         <v>3.705E-2</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="H51" s="5"/>
       <c r="I51" t="s">
@@ -6527,7 +6475,7 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="5" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>29</v>
@@ -6541,11 +6489,11 @@
       <c r="E52" s="10">
         <v>3663</v>
       </c>
-      <c r="F52" s="28">
+      <c r="F52" s="25">
         <v>3.739E-2</v>
       </c>
-      <c r="G52" s="35" t="s">
-        <v>214</v>
+      <c r="G52" s="32" t="s">
+        <v>205</v>
       </c>
       <c r="H52" s="5"/>
       <c r="I52" t="s">
@@ -6554,7 +6502,7 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="5" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>30</v>
@@ -6572,7 +6520,7 @@
         <v>1.6299999999999999E-2</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="H53" s="5"/>
       <c r="I53" t="s">
@@ -6581,7 +6529,7 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="5" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>30</v>
@@ -6599,7 +6547,7 @@
         <v>1.617E-2</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="H54" s="5"/>
       <c r="I54" t="s">
@@ -6608,34 +6556,34 @@
     </row>
     <row r="55" spans="1:9" ht="15" thickBot="1">
       <c r="A55" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="B55" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="B55" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C55" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D55" s="30">
+      <c r="C55" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D55" s="27">
         <v>39.39</v>
       </c>
-      <c r="E55" s="30">
+      <c r="E55" s="27">
         <v>1513</v>
       </c>
-      <c r="F55" s="34">
+      <c r="F55" s="31">
         <v>1.567E-2</v>
       </c>
-      <c r="G55" s="31" t="s">
-        <v>285</v>
-      </c>
-      <c r="H55" s="29"/>
-      <c r="I55" s="33" t="s">
+      <c r="G55" s="28" t="s">
+        <v>276</v>
+      </c>
+      <c r="H55" s="26"/>
+      <c r="I55" s="30" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="3" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>26</v>
@@ -6664,7 +6612,7 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="3" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>26</v>
@@ -6682,7 +6630,7 @@
         <v>3.0700000000000002E-2</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="H57" s="3"/>
       <c r="I57" t="s">
@@ -6691,7 +6639,7 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="3" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>26</v>
@@ -6705,14 +6653,14 @@
       <c r="E58" s="10">
         <v>2407</v>
       </c>
-      <c r="F58" s="28">
+      <c r="F58" s="25">
         <v>2.503E-2</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="I58" t="s">
         <v>107</v>
@@ -6720,7 +6668,7 @@
     </row>
     <row r="59" spans="1:9" ht="43.2">
       <c r="A59" s="3" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>29</v>
@@ -6749,7 +6697,7 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="3" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>29</v>
@@ -6767,7 +6715,7 @@
         <v>2.4060000000000002E-2</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="H60" s="3"/>
       <c r="I60" t="s">
@@ -6776,7 +6724,7 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="3" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>29</v>
@@ -6790,11 +6738,11 @@
       <c r="E61" s="10">
         <v>8385</v>
       </c>
-      <c r="F61" s="28">
+      <c r="F61" s="25">
         <v>9.3390000000000001E-2</v>
       </c>
-      <c r="G61" s="35" t="s">
-        <v>225</v>
+      <c r="G61" s="32" t="s">
+        <v>216</v>
       </c>
       <c r="H61" s="5"/>
       <c r="I61" t="s">
@@ -6803,7 +6751,7 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="3" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>30</v>
@@ -6821,7 +6769,7 @@
         <v>1.387E-2</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="H62" s="3"/>
       <c r="I62" t="s">
@@ -6830,7 +6778,7 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="3" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>30</v>
@@ -6848,7 +6796,7 @@
         <v>3.0960000000000001E-2</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="H63" s="3"/>
       <c r="I63" t="s">
@@ -6857,28 +6805,28 @@
     </row>
     <row r="64" spans="1:9" ht="15" thickBot="1">
       <c r="A64" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="B64" s="29" t="s">
+        <v>250</v>
+      </c>
+      <c r="B64" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C64" s="29" t="s">
+      <c r="C64" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="D64" s="30">
+      <c r="D64" s="27">
         <v>31.86</v>
       </c>
-      <c r="E64" s="30">
+      <c r="E64" s="27">
         <v>1359</v>
       </c>
-      <c r="F64" s="34">
+      <c r="F64" s="31">
         <v>1.387E-2</v>
       </c>
-      <c r="G64" s="31" t="s">
-        <v>288</v>
+      <c r="G64" s="28" t="s">
+        <v>279</v>
       </c>
       <c r="H64" s="3"/>
-      <c r="I64" s="33" t="s">
+      <c r="I64" s="30" t="s">
         <v>107</v>
       </c>
     </row>
@@ -6901,7 +6849,7 @@
       <c r="F65" s="9">
         <v>9.425E-2</v>
       </c>
-      <c r="G65" s="35" t="s">
+      <c r="G65" s="32" t="s">
         <v>124</v>
       </c>
       <c r="H65" s="3" t="s">
@@ -6930,8 +6878,8 @@
       <c r="F66" s="9">
         <v>3.7699999999999997E-2</v>
       </c>
-      <c r="G66" s="35" t="s">
-        <v>226</v>
+      <c r="G66" s="32" t="s">
+        <v>217</v>
       </c>
       <c r="H66" s="3"/>
       <c r="I66" t="s">
@@ -6954,11 +6902,11 @@
       <c r="E67" s="10">
         <v>6271</v>
       </c>
-      <c r="F67" s="28">
+      <c r="F67" s="25">
         <v>6.9589999999999999E-2</v>
       </c>
-      <c r="G67" s="35" t="s">
-        <v>227</v>
+      <c r="G67" s="32" t="s">
+        <v>218</v>
       </c>
       <c r="H67" s="5"/>
       <c r="I67" t="s">
@@ -7013,8 +6961,8 @@
       <c r="F69" s="9">
         <v>8.6059999999999998E-2</v>
       </c>
-      <c r="G69" s="35" t="s">
-        <v>228</v>
+      <c r="G69" s="32" t="s">
+        <v>219</v>
       </c>
       <c r="H69" s="3"/>
       <c r="I69" t="s">
@@ -7037,11 +6985,11 @@
       <c r="E70" s="10">
         <v>10412</v>
       </c>
-      <c r="F70" s="28">
+      <c r="F70" s="25">
         <v>0.11268</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="H70" s="5"/>
       <c r="I70" t="s">
@@ -7068,7 +7016,7 @@
         <v>2.8740000000000002E-2</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="H71" s="3"/>
       <c r="I71" t="s">
@@ -7094,8 +7042,8 @@
       <c r="F72" s="9">
         <v>3.0169999999999999E-2</v>
       </c>
-      <c r="G72" s="35" t="s">
-        <v>290</v>
+      <c r="G72" s="32" t="s">
+        <v>281</v>
       </c>
       <c r="H72" s="3"/>
       <c r="I72" t="s">
@@ -7103,35 +7051,35 @@
       </c>
     </row>
     <row r="73" spans="1:9" ht="15" thickBot="1">
-      <c r="A73" s="29" t="s">
+      <c r="A73" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="B73" s="29" t="s">
+      <c r="B73" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C73" s="29" t="s">
+      <c r="C73" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="D73" s="30">
+      <c r="D73" s="27">
         <v>127.43</v>
       </c>
-      <c r="E73" s="30">
+      <c r="E73" s="27">
         <v>3318</v>
       </c>
-      <c r="F73" s="34">
+      <c r="F73" s="31">
         <v>4.1799999999999997E-2</v>
       </c>
-      <c r="G73" s="31" t="s">
-        <v>291</v>
-      </c>
-      <c r="H73" s="29"/>
-      <c r="I73" s="33" t="s">
+      <c r="G73" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="H73" s="26"/>
+      <c r="I73" s="30" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="57.6">
       <c r="A74" s="5" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>26</v>
@@ -7160,7 +7108,7 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" s="5" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>26</v>
@@ -7178,10 +7126,10 @@
         <v>3.1530000000000002E-2</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="I75" t="s">
         <v>107</v>
@@ -7189,7 +7137,7 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="5" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>26</v>
@@ -7203,11 +7151,11 @@
       <c r="E76" s="10">
         <v>2621</v>
       </c>
-      <c r="F76" s="28">
+      <c r="F76" s="25">
         <v>2.7230000000000001E-2</v>
       </c>
-      <c r="G76" s="35" t="s">
-        <v>234</v>
+      <c r="G76" s="32" t="s">
+        <v>225</v>
       </c>
       <c r="H76" s="5"/>
       <c r="I76" t="s">
@@ -7216,7 +7164,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" s="5" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>29</v>
@@ -7245,7 +7193,7 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" s="5" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>29</v>
@@ -7263,10 +7211,10 @@
         <v>3.9629999999999999E-2</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="I78" t="s">
         <v>107</v>
@@ -7274,7 +7222,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" s="5" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>29</v>
@@ -7288,11 +7236,11 @@
       <c r="E79" s="10">
         <v>3650</v>
       </c>
-      <c r="F79" s="28">
+      <c r="F79" s="25">
         <v>3.7679999999999998E-2</v>
       </c>
-      <c r="G79" s="35" t="s">
-        <v>243</v>
+      <c r="G79" s="32" t="s">
+        <v>234</v>
       </c>
       <c r="H79" s="5"/>
       <c r="I79" t="s">
@@ -7301,7 +7249,7 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" s="5" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>30</v>
@@ -7319,7 +7267,7 @@
         <v>1.6109999999999999E-2</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="H80" s="5"/>
       <c r="I80" t="s">
@@ -7328,7 +7276,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" s="5" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>30</v>
@@ -7346,7 +7294,7 @@
         <v>2.5770000000000001E-2</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="H81" s="3"/>
       <c r="I81" t="s">
@@ -7355,34 +7303,34 @@
     </row>
     <row r="82" spans="1:9" ht="15" thickBot="1">
       <c r="A82" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="B82" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="B82" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C82" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D82" s="30">
+      <c r="C82" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D82" s="27">
         <v>52.14</v>
       </c>
-      <c r="E82" s="30">
+      <c r="E82" s="27">
         <v>1790</v>
       </c>
-      <c r="F82" s="34">
+      <c r="F82" s="31">
         <v>1.8620000000000001E-2</v>
       </c>
-      <c r="G82" s="31" t="s">
-        <v>294</v>
-      </c>
-      <c r="H82" s="29"/>
-      <c r="I82" s="33" t="s">
+      <c r="G82" s="28" t="s">
+        <v>285</v>
+      </c>
+      <c r="H82" s="26"/>
+      <c r="I82" s="30" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="72">
       <c r="A83" s="3" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>26</v>
@@ -7411,7 +7359,7 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="3" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B84" s="5" t="s">
         <v>26</v>
@@ -7429,7 +7377,7 @@
         <v>2.1090000000000001E-2</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="H84" s="3"/>
       <c r="I84" t="s">
@@ -7438,7 +7386,7 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" s="3" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>26</v>
@@ -7452,11 +7400,11 @@
       <c r="E85" s="10">
         <v>1961</v>
       </c>
-      <c r="F85" s="28">
+      <c r="F85" s="25">
         <v>2.0629999999999999E-2</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="H85" s="5"/>
       <c r="I85" t="s">
@@ -7465,7 +7413,7 @@
     </row>
     <row r="86" spans="1:9" ht="43.2">
       <c r="A86" s="3" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>29</v>
@@ -7494,7 +7442,7 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" s="3" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>29</v>
@@ -7512,7 +7460,7 @@
         <v>3.8929999999999999E-2</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="H87" s="3"/>
       <c r="I87" t="s">
@@ -7521,7 +7469,7 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" s="3" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B88" s="5" t="s">
         <v>29</v>
@@ -7535,11 +7483,11 @@
       <c r="E88" s="10">
         <v>3827</v>
       </c>
-      <c r="F88" s="28">
+      <c r="F88" s="25">
         <v>3.9170000000000003E-2</v>
       </c>
-      <c r="G88" s="35" t="s">
-        <v>255</v>
+      <c r="G88" s="32" t="s">
+        <v>246</v>
       </c>
       <c r="H88" s="5"/>
       <c r="I88" t="s">
@@ -7548,7 +7496,7 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" s="3" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B89" s="5" t="s">
         <v>30</v>
@@ -7566,7 +7514,7 @@
         <v>1.6119999999999999E-2</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="H89" s="3"/>
       <c r="I89" t="s">
@@ -7575,7 +7523,7 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="3" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>30</v>
@@ -7593,7 +7541,7 @@
         <v>1.6629999999999999E-2</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="H90" s="3"/>
       <c r="I90" t="s">
@@ -7602,28 +7550,28 @@
     </row>
     <row r="91" spans="1:9" ht="15" thickBot="1">
       <c r="A91" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="B91" s="29" t="s">
+        <v>248</v>
+      </c>
+      <c r="B91" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C91" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D91" s="30">
+      <c r="C91" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D91" s="27">
         <v>38.380000000000003</v>
       </c>
-      <c r="E91" s="30">
+      <c r="E91" s="27">
         <v>1566</v>
       </c>
-      <c r="F91" s="34">
+      <c r="F91" s="31">
         <v>1.6480000000000002E-2</v>
       </c>
-      <c r="G91" s="31" t="s">
-        <v>297</v>
-      </c>
-      <c r="H91" s="29"/>
-      <c r="I91" s="33" t="s">
+      <c r="G91" s="28" t="s">
+        <v>288</v>
+      </c>
+      <c r="H91" s="26"/>
+      <c r="I91" s="30" t="s">
         <v>107</v>
       </c>
     </row>
@@ -7676,7 +7624,7 @@
         <v>3.4750000000000003E-2</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="H93" s="5"/>
       <c r="I93" t="s">
@@ -7699,11 +7647,11 @@
       <c r="E94" s="10">
         <v>2480</v>
       </c>
-      <c r="F94" s="28">
+      <c r="F94" s="25">
         <v>2.64E-2</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="H94" s="5"/>
       <c r="I94" t="s">
@@ -7759,7 +7707,7 @@
         <v>2.6040000000000001E-2</v>
       </c>
       <c r="G96" s="6" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="H96" s="5"/>
       <c r="I96" t="s">
@@ -7782,11 +7730,11 @@
       <c r="E97" s="10">
         <v>2808</v>
       </c>
-      <c r="F97" s="28">
+      <c r="F97" s="25">
         <v>3.2559999999999999E-2</v>
       </c>
-      <c r="G97" s="35" t="s">
-        <v>171</v>
+      <c r="G97" s="32" t="s">
+        <v>162</v>
       </c>
       <c r="H97" s="5"/>
       <c r="I97" t="s">
@@ -7813,7 +7761,7 @@
         <v>1.3559999999999999E-2</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="H98" s="5"/>
       <c r="I98" t="s">
@@ -7840,7 +7788,7 @@
         <v>2.138E-2</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="H99" s="5"/>
       <c r="I99" t="s">
@@ -7848,29 +7796,29 @@
       </c>
     </row>
     <row r="100" spans="1:9" ht="15" thickBot="1">
-      <c r="A100" s="32" t="s">
+      <c r="A100" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B100" s="29" t="s">
+      <c r="B100" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C100" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D100" s="30">
+      <c r="C100" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D100" s="27">
         <v>23.3</v>
       </c>
-      <c r="E100" s="30">
+      <c r="E100" s="27">
         <v>1182</v>
       </c>
-      <c r="F100" s="34">
+      <c r="F100" s="31">
         <v>1.354E-2</v>
       </c>
-      <c r="G100" s="31" t="s">
-        <v>300</v>
-      </c>
-      <c r="H100" s="29"/>
-      <c r="I100" s="33" t="s">
+      <c r="G100" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="H100" s="26"/>
+      <c r="I100" s="30" t="s">
         <v>107</v>
       </c>
     </row>
@@ -7923,7 +7871,7 @@
         <v>5.5259999999999997E-2</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="H102" s="5"/>
       <c r="I102" t="s">
@@ -7946,11 +7894,11 @@
       <c r="E103" s="10">
         <v>3985</v>
       </c>
-      <c r="F103" s="28">
+      <c r="F103" s="25">
         <v>4.283E-2</v>
       </c>
-      <c r="G103" s="35" t="s">
-        <v>247</v>
+      <c r="G103" s="32" t="s">
+        <v>238</v>
       </c>
       <c r="H103" s="5"/>
       <c r="I103" t="s">
@@ -8006,7 +7954,7 @@
         <v>6.7949999999999997E-2</v>
       </c>
       <c r="G105" s="6" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="H105" s="5"/>
       <c r="I105" t="s">
@@ -8029,11 +7977,11 @@
       <c r="E106" s="10">
         <v>6461</v>
       </c>
-      <c r="F106" s="28">
+      <c r="F106" s="25">
         <v>7.3849999999999999E-2</v>
       </c>
-      <c r="G106" s="35" t="s">
-        <v>245</v>
+      <c r="G106" s="32" t="s">
+        <v>236</v>
       </c>
       <c r="H106" s="5"/>
       <c r="I106" t="s">
@@ -8060,7 +8008,7 @@
         <v>1.651E-2</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="H107" s="3"/>
       <c r="I107" t="s">
@@ -8087,7 +8035,7 @@
         <v>1.6379999999999999E-2</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="H108" s="5"/>
       <c r="I108" t="s">
@@ -8095,29 +8043,29 @@
       </c>
     </row>
     <row r="109" spans="1:9" ht="15" thickBot="1">
-      <c r="A109" s="29" t="s">
+      <c r="A109" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B109" s="29" t="s">
+      <c r="B109" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C109" s="29" t="s">
+      <c r="C109" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="D109" s="30">
+      <c r="D109" s="27">
         <v>37.36</v>
       </c>
-      <c r="E109" s="30">
+      <c r="E109" s="27">
         <v>1543</v>
       </c>
-      <c r="F109" s="34">
+      <c r="F109" s="31">
         <v>1.6389999999999998E-2</v>
       </c>
-      <c r="G109" s="31" t="s">
-        <v>303</v>
-      </c>
-      <c r="H109" s="29"/>
-      <c r="I109" s="33" t="s">
+      <c r="G109" s="28" t="s">
+        <v>294</v>
+      </c>
+      <c r="H109" s="26"/>
+      <c r="I109" s="30" t="s">
         <v>107</v>
       </c>
     </row>
@@ -8134,13 +8082,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3BFF00C-9B20-4D57-A0F3-3732FF3EA698}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="57" zoomScaleNormal="57" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="65" workbookViewId="2">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
+    <sheetView workbookViewId="3"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -8160,7 +8111,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -8174,7 +8125,7 @@
         <v>103</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>108</v>
@@ -8220,7 +8171,7 @@
     </row>
     <row r="5" spans="1:5" ht="28.8">
       <c r="A5" s="3" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>45</v>
@@ -8252,7 +8203,7 @@
     </row>
     <row r="7" spans="1:5" ht="43.2">
       <c r="A7" s="3" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>8</v>
@@ -8269,7 +8220,7 @@
     </row>
     <row r="8" spans="1:5" ht="100.8">
       <c r="A8" s="3" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>19</v>
@@ -8301,7 +8252,7 @@
     </row>
     <row r="10" spans="1:5" ht="57.6">
       <c r="A10" s="3" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>38</v>
@@ -8316,7 +8267,7 @@
     </row>
     <row r="11" spans="1:5" ht="57.6">
       <c r="A11" s="3" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>13</v>
@@ -8339,7 +8290,7 @@
         <v>113</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>22</v>
@@ -8387,134 +8338,115 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CACDBB6-EC7B-48C7-A660-9515B930A1AA}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
     <sheetView workbookViewId="2"/>
+    <sheetView tabSelected="1" zoomScale="84" workbookViewId="3">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="42.88671875" style="23" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" style="19" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" style="19" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" style="19" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="19"/>
+    <col min="1" max="1" width="21" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.21875" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="19" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="22" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="20" t="s">
+      <c r="C1" s="20" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.8">
-      <c r="A2" s="24" t="s">
-        <v>134</v>
+    <row r="2" spans="1:5" ht="28.8">
+      <c r="A2" s="23" t="s">
+        <v>120</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>136</v>
-      </c>
+      <c r="C2" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="15"/>
       <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-    </row>
-    <row r="3" spans="1:6" ht="136.80000000000001" customHeight="1">
-      <c r="A3" s="24" t="s">
-        <v>140</v>
+    </row>
+    <row r="3" spans="1:5" ht="129.6">
+      <c r="A3" s="23" t="s">
+        <v>120</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="D3" s="17" t="s">
-        <v>145</v>
-      </c>
+      <c r="D3" s="15"/>
       <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-    </row>
-    <row r="4" spans="1:6" ht="14.4">
+    </row>
+    <row r="4" spans="1:5" ht="14.4">
       <c r="A4" s="16" t="s">
-        <v>149</v>
+        <v>248</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>161</v>
-      </c>
+      <c r="C4" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="D4" s="15"/>
       <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-    </row>
-    <row r="5" spans="1:6" ht="86.4">
+    </row>
+    <row r="5" spans="1:5" ht="86.4">
       <c r="A5" s="16" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>151</v>
-      </c>
+      <c r="C5" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="15"/>
       <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-    </row>
-    <row r="6" spans="1:6" ht="28.8">
-      <c r="A6" s="25" t="s">
-        <v>141</v>
+    </row>
+    <row r="6" spans="1:5" ht="28.8">
+      <c r="A6" s="24" t="s">
+        <v>250</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>132</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>139</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="D6" s="15"/>
       <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-    </row>
-    <row r="7" spans="1:6" ht="144">
-      <c r="A7" s="25" t="s">
-        <v>142</v>
+    </row>
+    <row r="7" spans="1:5" ht="144">
+      <c r="A7" s="24" t="s">
+        <v>250</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>133</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>153</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="D7" s="15"/>
       <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8527,28 +8459,26 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E478D2DA-2B8C-45DE-9406-9F4B224C2A25}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView zoomScale="82" workbookViewId="1">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScale="82" workbookViewId="1">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
     <sheetView workbookViewId="2"/>
+    <sheetView workbookViewId="3"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="48.5546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" customWidth="1"/>
-    <col min="6" max="6" width="14" style="22" customWidth="1"/>
-    <col min="7" max="7" width="43.77734375" customWidth="1"/>
-    <col min="8" max="8" width="14.77734375" customWidth="1"/>
-    <col min="9" max="9" width="22.5546875" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" customWidth="1"/>
+    <col min="5" max="5" width="39" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:6">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -8556,339 +8486,375 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="F1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="26" t="s">
-        <v>134</v>
+    <row r="2" spans="1:6">
+      <c r="A2" s="23" t="s">
+        <v>120</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" t="s">
         <v>42</v>
       </c>
-      <c r="D2">
-        <v>105.27</v>
-      </c>
-      <c r="E2">
-        <v>3166</v>
-      </c>
-      <c r="F2" s="22">
-        <v>3.4299999999999997E-2</v>
-      </c>
-      <c r="G2" t="s">
-        <v>144</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="26" t="s">
-        <v>134</v>
+      <c r="E2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="23" t="s">
+        <v>120</v>
       </c>
       <c r="B3" t="s">
         <v>26</v>
       </c>
       <c r="C3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" t="s">
         <v>42</v>
       </c>
-      <c r="G3" t="s">
-        <v>159</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="26" t="s">
-        <v>134</v>
+      <c r="E3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="23" t="s">
+        <v>120</v>
       </c>
       <c r="B4" t="s">
         <v>29</v>
       </c>
       <c r="C4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" t="s">
         <v>42</v>
       </c>
-      <c r="G4" t="s">
-        <v>160</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="28.8">
-      <c r="A5" s="26" t="s">
-        <v>140</v>
+      <c r="E4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.8">
+      <c r="A5" s="23" t="s">
+        <v>120</v>
       </c>
       <c r="B5" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="26" t="s">
-        <v>140</v>
+      <c r="E5" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="23" t="s">
+        <v>120</v>
       </c>
       <c r="B6" t="s">
         <v>26</v>
       </c>
       <c r="C6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" t="s">
         <v>42</v>
       </c>
-      <c r="G6" t="s">
-        <v>147</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="43.2">
-      <c r="A7" s="26" t="s">
+      <c r="E6" t="s">
         <v>140</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="43.2">
+      <c r="A7" s="23" t="s">
+        <v>120</v>
       </c>
       <c r="B7" t="s">
         <v>29</v>
       </c>
       <c r="C7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="E7" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="16" t="s">
-        <v>149</v>
+        <v>248</v>
       </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D8" t="s">
         <v>40</v>
       </c>
-      <c r="G8" t="s">
-        <v>162</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="E8" t="s">
+        <v>153</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="16" t="s">
-        <v>149</v>
+        <v>248</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
       </c>
       <c r="C9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" t="s">
         <v>40</v>
       </c>
-      <c r="G9" t="s">
-        <v>164</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="E9" t="s">
+        <v>155</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="16" t="s">
-        <v>149</v>
+        <v>248</v>
       </c>
       <c r="B10" t="s">
         <v>29</v>
       </c>
       <c r="C10" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" t="s">
         <v>42</v>
       </c>
-      <c r="G10" t="s">
-        <v>163</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="E10" t="s">
+        <v>154</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="16" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="B11" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" t="s">
-        <v>165</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="28.8">
+        <v>133</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28.8">
       <c r="A12" s="16" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
       </c>
       <c r="C12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D12" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="E12" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="16" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="B13" t="s">
         <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" t="s">
-        <v>166</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="27" t="s">
-        <v>141</v>
+        <v>133</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" t="s">
+        <v>157</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="24" t="s">
+        <v>250</v>
       </c>
       <c r="B14" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D14" t="s">
         <v>42</v>
       </c>
-      <c r="G14" t="s">
-        <v>167</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="27" t="s">
-        <v>141</v>
+      <c r="E14" t="s">
+        <v>158</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="24" t="s">
+        <v>250</v>
       </c>
       <c r="B15" t="s">
         <v>26</v>
       </c>
       <c r="C15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D15" t="s">
         <v>42</v>
       </c>
-      <c r="G15" t="s">
-        <v>154</v>
-      </c>
-      <c r="I15" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="27" t="s">
-        <v>141</v>
+      <c r="E15" t="s">
+        <v>145</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="24" t="s">
+        <v>250</v>
       </c>
       <c r="B16" t="s">
         <v>29</v>
       </c>
       <c r="C16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" t="s">
         <v>42</v>
       </c>
-      <c r="G16" t="s">
-        <v>158</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="28.8">
-      <c r="A17" s="27" t="s">
-        <v>142</v>
+      <c r="E16" t="s">
+        <v>149</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="28.8">
+      <c r="A17" s="24" t="s">
+        <v>250</v>
       </c>
       <c r="B17" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D17" t="s">
         <v>40</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="I17" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="27" t="s">
-        <v>142</v>
+      <c r="E17" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="24" t="s">
+        <v>250</v>
       </c>
       <c r="B18" t="s">
         <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" t="s">
-        <v>155</v>
-      </c>
-      <c r="I18" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="27" t="s">
-        <v>142</v>
+        <v>133</v>
+      </c>
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="24" t="s">
+        <v>250</v>
       </c>
       <c r="B19" t="s">
         <v>29</v>
       </c>
       <c r="C19" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" t="s">
         <v>40</v>
       </c>
-      <c r="G19" t="s">
-        <v>157</v>
-      </c>
-      <c r="I19" s="21" t="s">
+      <c r="E19" t="s">
+        <v>148</v>
+      </c>
+      <c r="F19" s="21" t="s">
         <v>107</v>
       </c>
     </row>

</xml_diff>